<commit_message>
Added residence permit mapping
</commit_message>
<xml_diff>
--- a/input/mapping_tabeller.xlsx
+++ b/input/mapping_tabeller.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://maerskbroker-my.sharepoint.com/personal/kbo_maerskbroker_com/Documents/FTIND/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="80" documentId="8_{6B022C61-D3E3-4D46-8183-99CFA6E77F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{733A7E0C-83B5-4400-A57E-88AFD7860DCA}"/>
+  <xr:revisionPtr revIDLastSave="120" documentId="8_{6B022C61-D3E3-4D46-8183-99CFA6E77F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E61C07C-6768-4364-8DD2-E374A07BF220}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6B009A8E-40F0-41F8-8A22-826EDE827CF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Lande" sheetId="1" r:id="rId1"/>
+    <sheet name="Ophold" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="279">
   <si>
     <t>Albanien</t>
   </si>
@@ -770,9 +771,6 @@
     <t>MENAPT-lande</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Andre vestlige lande</t>
   </si>
   <si>
@@ -780,6 +778,102 @@
   </si>
   <si>
     <t>Andre ikke-vestlige lande</t>
+  </si>
+  <si>
+    <t>Opholdsgrundlag</t>
+  </si>
+  <si>
+    <t>Familiesammenføring, Andre familiemedlemmer, Refererer til flygtning</t>
+  </si>
+  <si>
+    <t>Ukraine (særlov)</t>
+  </si>
+  <si>
+    <t>Familiesammenføring, Andre familiemedlemmer, Refererer til dansk/nordisk person</t>
+  </si>
+  <si>
+    <t>Familiesammenføring, Mindreårige børn, Refererer til flygtning</t>
+  </si>
+  <si>
+    <t>Familiesammenføring, Andre familiemedlemmer, Uoplyst referenceperson</t>
+  </si>
+  <si>
+    <t>Det øvrige opholdsområde, Adoption</t>
+  </si>
+  <si>
+    <t>Asyl, Andet grundlag</t>
+  </si>
+  <si>
+    <t>Familiesammenføring, Ægteskab eller fast samlivsforhold, Refererer til udlænding, men ikke flygtning</t>
+  </si>
+  <si>
+    <t>Familiesammenføring, Ægteskab eller fast samlivsforhold, Refererer til flygtning</t>
+  </si>
+  <si>
+    <t>EU/EØS, Øvrige grunde</t>
+  </si>
+  <si>
+    <t>EU/EØS, Uddannelse</t>
+  </si>
+  <si>
+    <t>EU/EØS, Lønarbejde</t>
+  </si>
+  <si>
+    <t>Familiesammenføring, Mindreårige børn, Refererer til andre end flygtning</t>
+  </si>
+  <si>
+    <t>Asyl, Flygtningestatus</t>
+  </si>
+  <si>
+    <t>Familiesammenføring, Mindreårige børn, Uoplyst referenceperson</t>
+  </si>
+  <si>
+    <t>Studie mv., Praktikanter</t>
+  </si>
+  <si>
+    <t>Studie mv., Au pair</t>
+  </si>
+  <si>
+    <t>Familiesammenføring, Ægteskab eller fast samlivsforhold, Refererer til dansk/nordisk person</t>
+  </si>
+  <si>
+    <t>Det øvrige opholdsområde, Øvrige grunde</t>
+  </si>
+  <si>
+    <t>Familiesammenføring, Ægteskab eller fast samlivsforhold, Uoplyst referenceperson</t>
+  </si>
+  <si>
+    <t>Studie mv., Øvrige grunde</t>
+  </si>
+  <si>
+    <t>EU/EØS, Familiemedlemmer</t>
+  </si>
+  <si>
+    <t>Studie mv., Uddannelse</t>
+  </si>
+  <si>
+    <t>Erhverv</t>
+  </si>
+  <si>
+    <t>Opholdstype</t>
+  </si>
+  <si>
+    <t>Familiesammenføring</t>
+  </si>
+  <si>
+    <t>Adoption</t>
+  </si>
+  <si>
+    <t>Øvrige grunde</t>
+  </si>
+  <si>
+    <t>Uddannelse/praktik</t>
+  </si>
+  <si>
+    <t>Lønarbejde/erhverv</t>
+  </si>
+  <si>
+    <t>Flygtningestatus/asyl</t>
   </si>
 </sst>
 </file>
@@ -842,6 +936,17 @@
     <tableColumn id="2" xr3:uid="{CCD7F3D7-4C40-4F4A-AC2A-5F386D923C4E}" name="Region"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{50B7EBB8-A417-41D7-8729-B3BADE4E1F68}" name="Ophold" displayName="Ophold" ref="A1:B25" totalsRowShown="0">
+  <autoFilter ref="A1:B25" xr:uid="{50B7EBB8-A417-41D7-8729-B3BADE4E1F68}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{8CD7B636-0360-4CA7-B474-14423B8D214F}" name="Opholdsgrundlag"/>
+    <tableColumn id="2" xr3:uid="{6D73680C-8124-4DC3-BF29-C4F20331F105}" name="Opholdstype"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1187,7 +1292,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1195,7 +1300,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1203,7 +1308,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1211,7 +1316,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1219,7 +1324,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -1227,7 +1332,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -1235,7 +1340,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -1243,7 +1348,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -1251,7 +1356,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -1259,7 +1364,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -1267,7 +1372,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -1275,7 +1380,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -1283,7 +1388,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -1291,7 +1396,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -1299,7 +1404,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -1307,7 +1412,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -1315,7 +1420,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -1323,7 +1428,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -1331,7 +1436,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -1339,7 +1444,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -1347,7 +1452,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -1355,7 +1460,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -1363,7 +1468,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -1371,7 +1476,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -1379,7 +1484,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -1387,7 +1492,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -1395,7 +1500,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -1403,7 +1508,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -1411,7 +1516,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -1419,7 +1524,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -1427,7 +1532,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -1435,7 +1540,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -1443,7 +1548,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -1451,7 +1556,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -1459,7 +1564,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -1467,7 +1572,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -1475,7 +1580,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -1483,7 +1588,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -1491,7 +1596,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -1499,7 +1604,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -1507,7 +1612,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -1515,7 +1620,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -1523,7 +1628,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -1531,7 +1636,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
@@ -1539,7 +1644,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -1547,7 +1652,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
@@ -1555,7 +1660,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -1571,7 +1676,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -1579,7 +1684,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
@@ -1587,7 +1692,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
@@ -1595,7 +1700,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
@@ -1603,7 +1708,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
@@ -1611,7 +1716,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
@@ -1627,7 +1732,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
@@ -1635,7 +1740,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
@@ -1643,7 +1748,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
@@ -1651,7 +1756,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
@@ -1659,7 +1764,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
@@ -1667,7 +1772,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
@@ -1675,7 +1780,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
@@ -1683,7 +1788,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
@@ -1691,7 +1796,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
@@ -1699,7 +1804,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
@@ -1723,7 +1828,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
@@ -1731,7 +1836,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
@@ -1739,7 +1844,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
@@ -1747,7 +1852,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
@@ -1755,7 +1860,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
@@ -1763,7 +1868,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
@@ -1771,7 +1876,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
@@ -1779,7 +1884,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
@@ -1787,7 +1892,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
@@ -1795,7 +1900,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
@@ -1803,7 +1908,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
@@ -1811,7 +1916,7 @@
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
@@ -1819,7 +1924,7 @@
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
@@ -1835,7 +1940,7 @@
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
@@ -1843,7 +1948,7 @@
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
@@ -1851,7 +1956,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
@@ -1875,7 +1980,7 @@
         <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
@@ -1883,7 +1988,7 @@
         <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
@@ -1891,7 +1996,7 @@
         <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
@@ -1899,7 +2004,7 @@
         <v>89</v>
       </c>
       <c r="B91" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
@@ -1907,7 +2012,7 @@
         <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
@@ -1915,7 +2020,7 @@
         <v>91</v>
       </c>
       <c r="B93" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
@@ -1923,7 +2028,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
@@ -1931,7 +2036,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
@@ -1939,7 +2044,7 @@
         <v>94</v>
       </c>
       <c r="B96" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
@@ -1947,7 +2052,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
@@ -1955,7 +2060,7 @@
         <v>96</v>
       </c>
       <c r="B98" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
@@ -1963,7 +2068,7 @@
         <v>97</v>
       </c>
       <c r="B99" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
@@ -1979,7 +2084,7 @@
         <v>99</v>
       </c>
       <c r="B101" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
@@ -1995,7 +2100,7 @@
         <v>101</v>
       </c>
       <c r="B103" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
@@ -2003,7 +2108,7 @@
         <v>102</v>
       </c>
       <c r="B104" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
@@ -2011,7 +2116,7 @@
         <v>103</v>
       </c>
       <c r="B105" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
@@ -2019,7 +2124,7 @@
         <v>104</v>
       </c>
       <c r="B106" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
@@ -2027,7 +2132,7 @@
         <v>105</v>
       </c>
       <c r="B107" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
@@ -2035,7 +2140,7 @@
         <v>106</v>
       </c>
       <c r="B108" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
@@ -2051,7 +2156,7 @@
         <v>108</v>
       </c>
       <c r="B110" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
@@ -2059,7 +2164,7 @@
         <v>109</v>
       </c>
       <c r="B111" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
@@ -2067,7 +2172,7 @@
         <v>110</v>
       </c>
       <c r="B112" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
@@ -2075,7 +2180,7 @@
         <v>111</v>
       </c>
       <c r="B113" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
@@ -2083,7 +2188,7 @@
         <v>112</v>
       </c>
       <c r="B114" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
@@ -2091,7 +2196,7 @@
         <v>113</v>
       </c>
       <c r="B115" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
@@ -2099,7 +2204,7 @@
         <v>114</v>
       </c>
       <c r="B116" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
@@ -2115,7 +2220,7 @@
         <v>116</v>
       </c>
       <c r="B118" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
@@ -2123,7 +2228,7 @@
         <v>117</v>
       </c>
       <c r="B119" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
@@ -2131,7 +2236,7 @@
         <v>118</v>
       </c>
       <c r="B120" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
@@ -2139,7 +2244,7 @@
         <v>119</v>
       </c>
       <c r="B121" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
@@ -2147,7 +2252,7 @@
         <v>120</v>
       </c>
       <c r="B122" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
@@ -2155,7 +2260,7 @@
         <v>121</v>
       </c>
       <c r="B123" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
@@ -2163,7 +2268,7 @@
         <v>122</v>
       </c>
       <c r="B124" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
@@ -2171,7 +2276,7 @@
         <v>123</v>
       </c>
       <c r="B125" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
@@ -2179,7 +2284,7 @@
         <v>124</v>
       </c>
       <c r="B126" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
@@ -2187,7 +2292,7 @@
         <v>125</v>
       </c>
       <c r="B127" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
@@ -2195,7 +2300,7 @@
         <v>126</v>
       </c>
       <c r="B128" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
@@ -2203,7 +2308,7 @@
         <v>127</v>
       </c>
       <c r="B129" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
@@ -2211,7 +2316,7 @@
         <v>128</v>
       </c>
       <c r="B130" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
@@ -2219,7 +2324,7 @@
         <v>129</v>
       </c>
       <c r="B131" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
@@ -2227,7 +2332,7 @@
         <v>130</v>
       </c>
       <c r="B132" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
@@ -2235,7 +2340,7 @@
         <v>131</v>
       </c>
       <c r="B133" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
@@ -2243,7 +2348,7 @@
         <v>132</v>
       </c>
       <c r="B134" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
@@ -2251,7 +2356,7 @@
         <v>133</v>
       </c>
       <c r="B135" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
@@ -2259,7 +2364,7 @@
         <v>134</v>
       </c>
       <c r="B136" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
@@ -2267,7 +2372,7 @@
         <v>135</v>
       </c>
       <c r="B137" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
@@ -2275,7 +2380,7 @@
         <v>136</v>
       </c>
       <c r="B138" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
@@ -2283,7 +2388,7 @@
         <v>137</v>
       </c>
       <c r="B139" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
@@ -2291,7 +2396,7 @@
         <v>138</v>
       </c>
       <c r="B140" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
@@ -2299,7 +2404,7 @@
         <v>139</v>
       </c>
       <c r="B141" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
@@ -2307,7 +2412,7 @@
         <v>140</v>
       </c>
       <c r="B142" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
@@ -2315,7 +2420,7 @@
         <v>141</v>
       </c>
       <c r="B143" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
@@ -2323,7 +2428,7 @@
         <v>142</v>
       </c>
       <c r="B144" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
@@ -2331,7 +2436,7 @@
         <v>143</v>
       </c>
       <c r="B145" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
@@ -2339,7 +2444,7 @@
         <v>144</v>
       </c>
       <c r="B146" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.3">
@@ -2347,7 +2452,7 @@
         <v>145</v>
       </c>
       <c r="B147" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.3">
@@ -2355,7 +2460,7 @@
         <v>146</v>
       </c>
       <c r="B148" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.3">
@@ -2363,7 +2468,7 @@
         <v>147</v>
       </c>
       <c r="B149" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
@@ -2371,7 +2476,7 @@
         <v>148</v>
       </c>
       <c r="B150" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.3">
@@ -2379,7 +2484,7 @@
         <v>149</v>
       </c>
       <c r="B151" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.3">
@@ -2387,7 +2492,7 @@
         <v>150</v>
       </c>
       <c r="B152" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.3">
@@ -2395,7 +2500,7 @@
         <v>151</v>
       </c>
       <c r="B153" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.3">
@@ -2403,7 +2508,7 @@
         <v>152</v>
       </c>
       <c r="B154" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.3">
@@ -2411,7 +2516,7 @@
         <v>153</v>
       </c>
       <c r="B155" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.3">
@@ -2419,7 +2524,7 @@
         <v>154</v>
       </c>
       <c r="B156" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.3">
@@ -2427,7 +2532,7 @@
         <v>155</v>
       </c>
       <c r="B157" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.3">
@@ -2435,7 +2540,7 @@
         <v>156</v>
       </c>
       <c r="B158" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.3">
@@ -2443,7 +2548,7 @@
         <v>157</v>
       </c>
       <c r="B159" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.3">
@@ -2451,7 +2556,7 @@
         <v>158</v>
       </c>
       <c r="B160" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.3">
@@ -2459,7 +2564,7 @@
         <v>159</v>
       </c>
       <c r="B161" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.3">
@@ -2467,7 +2572,7 @@
         <v>160</v>
       </c>
       <c r="B162" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.3">
@@ -2475,7 +2580,7 @@
         <v>161</v>
       </c>
       <c r="B163" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.3">
@@ -2483,7 +2588,7 @@
         <v>162</v>
       </c>
       <c r="B164" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.3">
@@ -2491,7 +2596,7 @@
         <v>163</v>
       </c>
       <c r="B165" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.3">
@@ -2507,7 +2612,7 @@
         <v>165</v>
       </c>
       <c r="B167" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.3">
@@ -2515,7 +2620,7 @@
         <v>166</v>
       </c>
       <c r="B168" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.3">
@@ -2531,7 +2636,7 @@
         <v>168</v>
       </c>
       <c r="B170" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.3">
@@ -2539,7 +2644,7 @@
         <v>169</v>
       </c>
       <c r="B171" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.3">
@@ -2547,7 +2652,7 @@
         <v>170</v>
       </c>
       <c r="B172" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.3">
@@ -2555,7 +2660,7 @@
         <v>171</v>
       </c>
       <c r="B173" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.3">
@@ -2563,7 +2668,7 @@
         <v>172</v>
       </c>
       <c r="B174" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.3">
@@ -2571,7 +2676,7 @@
         <v>173</v>
       </c>
       <c r="B175" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.3">
@@ -2595,7 +2700,7 @@
         <v>176</v>
       </c>
       <c r="B178" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.3">
@@ -2603,7 +2708,7 @@
         <v>177</v>
       </c>
       <c r="B179" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.3">
@@ -2611,7 +2716,7 @@
         <v>178</v>
       </c>
       <c r="B180" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.3">
@@ -2619,7 +2724,7 @@
         <v>179</v>
       </c>
       <c r="B181" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.3">
@@ -2627,7 +2732,7 @@
         <v>180</v>
       </c>
       <c r="B182" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.3">
@@ -2651,7 +2756,7 @@
         <v>183</v>
       </c>
       <c r="B185" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.3">
@@ -2659,7 +2764,7 @@
         <v>184</v>
       </c>
       <c r="B186" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.3">
@@ -2675,7 +2780,7 @@
         <v>186</v>
       </c>
       <c r="B188" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.3">
@@ -2683,7 +2788,7 @@
         <v>187</v>
       </c>
       <c r="B189" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.3">
@@ -2691,7 +2796,7 @@
         <v>188</v>
       </c>
       <c r="B190" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.3">
@@ -2707,7 +2812,7 @@
         <v>190</v>
       </c>
       <c r="B192" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.3">
@@ -2723,7 +2828,7 @@
         <v>192</v>
       </c>
       <c r="B194" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.3">
@@ -2731,7 +2836,7 @@
         <v>193</v>
       </c>
       <c r="B195" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.3">
@@ -2739,7 +2844,7 @@
         <v>194</v>
       </c>
       <c r="B196" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.3">
@@ -2747,7 +2852,7 @@
         <v>195</v>
       </c>
       <c r="B197" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.3">
@@ -2755,7 +2860,7 @@
         <v>196</v>
       </c>
       <c r="B198" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.3">
@@ -2763,7 +2868,7 @@
         <v>197</v>
       </c>
       <c r="B199" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.3">
@@ -2771,7 +2876,7 @@
         <v>198</v>
       </c>
       <c r="B200" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.3">
@@ -2779,7 +2884,7 @@
         <v>199</v>
       </c>
       <c r="B201" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.3">
@@ -2787,7 +2892,7 @@
         <v>200</v>
       </c>
       <c r="B202" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.3">
@@ -2835,7 +2940,7 @@
         <v>206</v>
       </c>
       <c r="B208" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.3">
@@ -2843,7 +2948,7 @@
         <v>207</v>
       </c>
       <c r="B209" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.3">
@@ -2851,7 +2956,7 @@
         <v>208</v>
       </c>
       <c r="B210" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.3">
@@ -2859,7 +2964,7 @@
         <v>209</v>
       </c>
       <c r="B211" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.3">
@@ -2875,7 +2980,7 @@
         <v>211</v>
       </c>
       <c r="B213" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.3">
@@ -2883,7 +2988,7 @@
         <v>212</v>
       </c>
       <c r="B214" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.3">
@@ -2891,7 +2996,7 @@
         <v>213</v>
       </c>
       <c r="B215" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.3">
@@ -2899,7 +3004,7 @@
         <v>214</v>
       </c>
       <c r="B216" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.3">
@@ -2907,7 +3012,7 @@
         <v>215</v>
       </c>
       <c r="B217" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.3">
@@ -2915,7 +3020,7 @@
         <v>216</v>
       </c>
       <c r="B218" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.3">
@@ -2939,7 +3044,7 @@
         <v>219</v>
       </c>
       <c r="B221" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.3">
@@ -2963,7 +3068,7 @@
         <v>222</v>
       </c>
       <c r="B224" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.3">
@@ -2971,7 +3076,7 @@
         <v>223</v>
       </c>
       <c r="B225" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.3">
@@ -2979,7 +3084,7 @@
         <v>224</v>
       </c>
       <c r="B226" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.3">
@@ -2987,7 +3092,7 @@
         <v>225</v>
       </c>
       <c r="B227" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.3">
@@ -2995,7 +3100,7 @@
         <v>226</v>
       </c>
       <c r="B228" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.3">
@@ -3003,7 +3108,7 @@
         <v>227</v>
       </c>
       <c r="B229" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.3">
@@ -3011,7 +3116,7 @@
         <v>228</v>
       </c>
       <c r="B230" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.3">
@@ -3019,7 +3124,7 @@
         <v>229</v>
       </c>
       <c r="B231" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.3">
@@ -3027,7 +3132,7 @@
         <v>230</v>
       </c>
       <c r="B232" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.3">
@@ -3035,7 +3140,7 @@
         <v>231</v>
       </c>
       <c r="B233" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.3">
@@ -3043,7 +3148,7 @@
         <v>232</v>
       </c>
       <c r="B234" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.3">
@@ -3051,7 +3156,7 @@
         <v>233</v>
       </c>
       <c r="B235" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.3">
@@ -3059,7 +3164,7 @@
         <v>234</v>
       </c>
       <c r="B236" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.3">
@@ -3067,7 +3172,7 @@
         <v>235</v>
       </c>
       <c r="B237" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.3">
@@ -3075,7 +3180,7 @@
         <v>236</v>
       </c>
       <c r="B238" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.3">
@@ -3083,7 +3188,7 @@
         <v>237</v>
       </c>
       <c r="B239" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.3">
@@ -3107,7 +3212,230 @@
         <v>240</v>
       </c>
       <c r="B242" t="s">
-        <v>246</v>
+        <v>245</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4698355F-9B01-452E-A3FA-B59AFCC52C49}">
+  <dimension ref="A1:B25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="82.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>249</v>
+      </c>
+      <c r="B3" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>250</v>
+      </c>
+      <c r="B4" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>251</v>
+      </c>
+      <c r="B5" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>252</v>
+      </c>
+      <c r="B6" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B7" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>254</v>
+      </c>
+      <c r="B8" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>255</v>
+      </c>
+      <c r="B9" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>256</v>
+      </c>
+      <c r="B10" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>257</v>
+      </c>
+      <c r="B11" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>258</v>
+      </c>
+      <c r="B12" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>259</v>
+      </c>
+      <c r="B13" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>260</v>
+      </c>
+      <c r="B14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B15" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>262</v>
+      </c>
+      <c r="B16" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>263</v>
+      </c>
+      <c r="B17" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>264</v>
+      </c>
+      <c r="B18" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>265</v>
+      </c>
+      <c r="B19" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>266</v>
+      </c>
+      <c r="B20" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>267</v>
+      </c>
+      <c r="B21" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>268</v>
+      </c>
+      <c r="B22" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>269</v>
+      </c>
+      <c r="B23" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>270</v>
+      </c>
+      <c r="B24" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>271</v>
+      </c>
+      <c r="B25" t="s">
+        <v>277</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added residence permit mapping for EU/not EU
</commit_message>
<xml_diff>
--- a/input/mapping_tabeller.xlsx
+++ b/input/mapping_tabeller.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://maerskbroker-my.sharepoint.com/personal/kbo_maerskbroker_com/Documents/FTIND/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="120" documentId="8_{6B022C61-D3E3-4D46-8183-99CFA6E77F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E61C07C-6768-4364-8DD2-E374A07BF220}"/>
+  <xr:revisionPtr revIDLastSave="132" documentId="8_{6B022C61-D3E3-4D46-8183-99CFA6E77F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB26FACD-B53D-4B88-B80F-599E65A4A4C3}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6B009A8E-40F0-41F8-8A22-826EDE827CF8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{6B009A8E-40F0-41F8-8A22-826EDE827CF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Lande" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="282">
   <si>
     <t>Albanien</t>
   </si>
@@ -874,6 +874,15 @@
   </si>
   <si>
     <t>Flygtningestatus/asyl</t>
+  </si>
+  <si>
+    <t>Opholdsregler</t>
+  </si>
+  <si>
+    <t>Ikke-EU/EØS</t>
+  </si>
+  <si>
+    <t>EU/EØS</t>
   </si>
 </sst>
 </file>
@@ -940,11 +949,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{50B7EBB8-A417-41D7-8729-B3BADE4E1F68}" name="Ophold" displayName="Ophold" ref="A1:B25" totalsRowShown="0">
-  <autoFilter ref="A1:B25" xr:uid="{50B7EBB8-A417-41D7-8729-B3BADE4E1F68}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{50B7EBB8-A417-41D7-8729-B3BADE4E1F68}" name="Ophold" displayName="Ophold" ref="A1:C25" totalsRowShown="0">
+  <autoFilter ref="A1:C25" xr:uid="{50B7EBB8-A417-41D7-8729-B3BADE4E1F68}"/>
+  <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8CD7B636-0360-4CA7-B474-14423B8D214F}" name="Opholdsgrundlag"/>
     <tableColumn id="2" xr3:uid="{6D73680C-8124-4DC3-BF29-C4F20331F105}" name="Opholdstype"/>
+    <tableColumn id="3" xr3:uid="{19B7548E-6F56-489F-9D4F-133C125CEA28}" name="Opholdsregler"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1269,7 +1279,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49A602A4-6912-42DD-80A5-C52D0F353E0C}">
   <dimension ref="A1:B242"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -3226,216 +3236,292 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4698355F-9B01-452E-A3FA-B59AFCC52C49}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="82.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.5546875" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>247</v>
       </c>
       <c r="B1" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>248</v>
       </c>
       <c r="B2" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>249</v>
       </c>
       <c r="B3" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>250</v>
       </c>
       <c r="B4" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>251</v>
       </c>
       <c r="B5" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>252</v>
       </c>
       <c r="B6" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>253</v>
       </c>
       <c r="B7" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>254</v>
       </c>
       <c r="B8" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>255</v>
       </c>
       <c r="B9" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>256</v>
       </c>
       <c r="B10" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>257</v>
       </c>
       <c r="B11" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>258</v>
       </c>
       <c r="B12" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>259</v>
       </c>
       <c r="B13" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>260</v>
       </c>
       <c r="B14" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>261</v>
       </c>
       <c r="B15" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>262</v>
       </c>
       <c r="B16" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>263</v>
       </c>
       <c r="B17" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>264</v>
       </c>
       <c r="B18" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>265</v>
       </c>
       <c r="B19" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>266</v>
       </c>
       <c r="B20" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>267</v>
       </c>
       <c r="B21" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>268</v>
       </c>
       <c r="B22" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>269</v>
       </c>
       <c r="B23" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>270</v>
       </c>
       <c r="B24" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>271</v>
       </c>
       <c r="B25" t="s">
         <v>277</v>
+      </c>
+      <c r="C25" t="s">
+        <v>280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added mapping of political parties based on abbreviations
</commit_message>
<xml_diff>
--- a/input/mapping_tabeller.xlsx
+++ b/input/mapping_tabeller.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://maerskbroker-my.sharepoint.com/personal/kbo_maerskbroker_com/Documents/FTIND/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="132" documentId="8_{6B022C61-D3E3-4D46-8183-99CFA6E77F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB26FACD-B53D-4B88-B80F-599E65A4A4C3}"/>
+  <xr:revisionPtr revIDLastSave="191" documentId="8_{6B022C61-D3E3-4D46-8183-99CFA6E77F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5665293A-C7A8-4A22-BE6A-311074884096}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{6B009A8E-40F0-41F8-8A22-826EDE827CF8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{6B009A8E-40F0-41F8-8A22-826EDE827CF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Lande" sheetId="1" r:id="rId1"/>
     <sheet name="Ophold" sheetId="2" r:id="rId2"/>
+    <sheet name="Partigrupper" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="326">
   <si>
     <t>Albanien</t>
   </si>
@@ -883,19 +884,157 @@
   </si>
   <si>
     <t>EU/EØS</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>DF</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>RV</t>
+  </si>
+  <si>
+    <t>SF</t>
+  </si>
+  <si>
+    <t>KF</t>
+  </si>
+  <si>
+    <t>EL</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>DD</t>
+  </si>
+  <si>
+    <t>LA</t>
+  </si>
+  <si>
+    <t>Udlændinge- Og Integrationsministeren</t>
+  </si>
+  <si>
+    <t>ALT</t>
+  </si>
+  <si>
+    <t>NB</t>
+  </si>
+  <si>
+    <t>Integrationsministeren</t>
+  </si>
+  <si>
+    <t>Justitsministeren</t>
+  </si>
+  <si>
+    <t>Den Fg. Formand</t>
+  </si>
+  <si>
+    <t>UFG</t>
+  </si>
+  <si>
+    <t>Udlændinge-, Integrations- Og Boligministeren</t>
+  </si>
+  <si>
+    <t>Fg. Formand</t>
+  </si>
+  <si>
+    <t>KD</t>
+  </si>
+  <si>
+    <t>FG</t>
+  </si>
+  <si>
+    <t>Fjerde Næstformand</t>
+  </si>
+  <si>
+    <t>Første Næstformand</t>
+  </si>
+  <si>
+    <t>Tredje Næstformand</t>
+  </si>
+  <si>
+    <t>Anden Næstformand</t>
+  </si>
+  <si>
+    <t>PartiGruppeKort</t>
+  </si>
+  <si>
+    <t>PartiGruppe</t>
+  </si>
+  <si>
+    <t>Udlændingeministeren</t>
+  </si>
+  <si>
+    <t>Folketingets formand</t>
+  </si>
+  <si>
+    <t>Socialdemokratiet (S)</t>
+  </si>
+  <si>
+    <t>Venstre (V)</t>
+  </si>
+  <si>
+    <t>Dansk Folkeparti (DF)</t>
+  </si>
+  <si>
+    <t>Socialistisk Folkeparti (SF)</t>
+  </si>
+  <si>
+    <t>Det Radikale Venstre (RV)</t>
+  </si>
+  <si>
+    <t>Det Konservative Folkeparti (KF)</t>
+  </si>
+  <si>
+    <t>Enhedslisten (EL)</t>
+  </si>
+  <si>
+    <t>Liberal Alliance (LA)</t>
+  </si>
+  <si>
+    <t>Kristendemokraterne (KD)</t>
+  </si>
+  <si>
+    <t>Uden for folketingsgrupperne (UFG)</t>
+  </si>
+  <si>
+    <t>Alternativet (ALT)</t>
+  </si>
+  <si>
+    <t>Nye Borgerlige (NB)</t>
+  </si>
+  <si>
+    <t>Frie Grønne, Danmarks Nye Venstrefløjsparti (FG)</t>
+  </si>
+  <si>
+    <t>Moderaterne (M)</t>
+  </si>
+  <si>
+    <t>Danmarksdemokraterne - Inger Støjberg (DD)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -918,8 +1057,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -957,6 +1097,17 @@
     <tableColumn id="3" xr3:uid="{19B7548E-6F56-489F-9D4F-133C125CEA28}" name="Opholdsregler"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D55ED5DE-F9F7-4D09-9799-968B23FB7A7F}" name="Partigrupper" displayName="Partigrupper" ref="A1:B26" totalsRowShown="0">
+  <autoFilter ref="A1:B26" xr:uid="{D55ED5DE-F9F7-4D09-9799-968B23FB7A7F}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{94861714-530E-4945-A68F-797D6EF0AA5E}" name="PartiGruppeKort"/>
+    <tableColumn id="2" xr3:uid="{82F208BF-F2E6-46F4-A1C1-9F9D4267E30C}" name="PartiGruppe"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -3238,7 +3389,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4698355F-9B01-452E-A3FA-B59AFCC52C49}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -3531,4 +3682,235 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A493712-F027-4507-94A0-9698A823257D}">
+  <dimension ref="A1:B26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="38.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>283</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>284</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>286</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>287</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>288</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>289</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>290</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>291</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>292</v>
+      </c>
+      <c r="B12" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>293</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>294</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>295</v>
+      </c>
+      <c r="B15" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>296</v>
+      </c>
+      <c r="B16" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>297</v>
+      </c>
+      <c r="B17" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>298</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>299</v>
+      </c>
+      <c r="B19" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>300</v>
+      </c>
+      <c r="B20" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>301</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>302</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>303</v>
+      </c>
+      <c r="B23" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>304</v>
+      </c>
+      <c r="B24" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>305</v>
+      </c>
+      <c r="B25" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>306</v>
+      </c>
+      <c r="B26" t="s">
+        <v>310</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated mapping of political parties
</commit_message>
<xml_diff>
--- a/input/mapping_tabeller.xlsx
+++ b/input/mapping_tabeller.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://maerskbroker-my.sharepoint.com/personal/kbo_maerskbroker_com/Documents/FTIND/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="191" documentId="8_{6B022C61-D3E3-4D46-8183-99CFA6E77F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5665293A-C7A8-4A22-BE6A-311074884096}"/>
+  <xr:revisionPtr revIDLastSave="215" documentId="8_{6B022C61-D3E3-4D46-8183-99CFA6E77F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4656A3FF-AAA0-40DF-9CAE-B84C41489C7A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{6B009A8E-40F0-41F8-8A22-826EDE827CF8}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="344">
   <si>
     <t>Albanien</t>
   </si>
@@ -1016,6 +1016,60 @@
   </si>
   <si>
     <t>Danmarksdemokraterne - Inger Støjberg (DD)</t>
+  </si>
+  <si>
+    <t>Inuit Ataqatigiit (IA)</t>
+  </si>
+  <si>
+    <t>Siumut (SIU)</t>
+  </si>
+  <si>
+    <t>Tjóðveldisflokkurin (TF)</t>
+  </si>
+  <si>
+    <t>Fólkaflokkurin (FF)</t>
+  </si>
+  <si>
+    <t>Sambandsflokkurin (SP)</t>
+  </si>
+  <si>
+    <t>Ny Alliance (NY)</t>
+  </si>
+  <si>
+    <t>Javnaðarflokkurin (JF)</t>
+  </si>
+  <si>
+    <t>Tjóðveldi (T)</t>
+  </si>
+  <si>
+    <t>Nunatta Qitornai (NQ)</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>NQ</t>
+  </si>
+  <si>
+    <t>SIU</t>
+  </si>
+  <si>
+    <t>TF</t>
+  </si>
+  <si>
+    <t>FF</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>JF</t>
   </si>
 </sst>
 </file>
@@ -1057,8 +1111,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1101,8 +1156,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D55ED5DE-F9F7-4D09-9799-968B23FB7A7F}" name="Partigrupper" displayName="Partigrupper" ref="A1:B26" totalsRowShown="0">
-  <autoFilter ref="A1:B26" xr:uid="{D55ED5DE-F9F7-4D09-9799-968B23FB7A7F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D55ED5DE-F9F7-4D09-9799-968B23FB7A7F}" name="Partigrupper" displayName="Partigrupper" ref="A1:B35" totalsRowShown="0">
+  <autoFilter ref="A1:B35" xr:uid="{D55ED5DE-F9F7-4D09-9799-968B23FB7A7F}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{94861714-530E-4945-A68F-797D6EF0AA5E}" name="PartiGruppeKort"/>
     <tableColumn id="2" xr3:uid="{82F208BF-F2E6-46F4-A1C1-9F9D4267E30C}" name="PartiGruppe"/>
@@ -3686,10 +3741,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A493712-F027-4507-94A0-9698A823257D}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3906,6 +3961,78 @@
         <v>310</v>
       </c>
     </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>335</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>338</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>339</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>340</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>341</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>342</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>343</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>336</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>337</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>334</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added list of custom stopwords
</commit_message>
<xml_diff>
--- a/input/mapping_tabeller.xlsx
+++ b/input/mapping_tabeller.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://maerskbroker-my.sharepoint.com/personal/kbo_maerskbroker_com/Documents/FTIND/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="215" documentId="8_{6B022C61-D3E3-4D46-8183-99CFA6E77F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4656A3FF-AAA0-40DF-9CAE-B84C41489C7A}"/>
+  <xr:revisionPtr revIDLastSave="235" documentId="8_{6B022C61-D3E3-4D46-8183-99CFA6E77F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DBD887C-F43B-4C91-A262-A4111E44DC5D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{6B009A8E-40F0-41F8-8A22-826EDE827CF8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{6B009A8E-40F0-41F8-8A22-826EDE827CF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Lande" sheetId="1" r:id="rId1"/>
     <sheet name="Ophold" sheetId="2" r:id="rId2"/>
     <sheet name="Partigrupper" sheetId="3" r:id="rId3"/>
+    <sheet name="Stopwords" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="372">
   <si>
     <t>Albanien</t>
   </si>
@@ -1070,6 +1071,90 @@
   </si>
   <si>
     <t>JF</t>
+  </si>
+  <si>
+    <t>Ord</t>
+  </si>
+  <si>
+    <t>dansk</t>
+  </si>
+  <si>
+    <t>statsborgerskab</t>
+  </si>
+  <si>
+    <t>hr.</t>
+  </si>
+  <si>
+    <t>ordfører</t>
+  </si>
+  <si>
+    <t>stemme</t>
+  </si>
+  <si>
+    <t>danmark</t>
+  </si>
+  <si>
+    <t>folketing</t>
+  </si>
+  <si>
+    <t>lovforslag</t>
+  </si>
+  <si>
+    <t>venstre</t>
+  </si>
+  <si>
+    <t>lovforslage</t>
+  </si>
+  <si>
+    <t>aftale</t>
+  </si>
+  <si>
+    <t>ordføreren</t>
+  </si>
+  <si>
+    <t>bemærkning</t>
+  </si>
+  <si>
+    <t>ændringsforslag</t>
+  </si>
+  <si>
+    <t>indfødsre</t>
+  </si>
+  <si>
+    <t>parti</t>
+  </si>
+  <si>
+    <t>indfødsretsudvalget</t>
+  </si>
+  <si>
+    <t>afstemning</t>
+  </si>
+  <si>
+    <t>statsborgere</t>
+  </si>
+  <si>
+    <t>statsborger</t>
+  </si>
+  <si>
+    <t>fru</t>
+  </si>
+  <si>
+    <t>justitsminister</t>
+  </si>
+  <si>
+    <t>folketingssal</t>
+  </si>
+  <si>
+    <t>indfødsret</t>
+  </si>
+  <si>
+    <t>integrationsminister</t>
+  </si>
+  <si>
+    <t>DatoTilføjet</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -1114,12 +1199,16 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1163,6 +1252,17 @@
     <tableColumn id="2" xr3:uid="{82F208BF-F2E6-46F4-A1C1-9F9D4267E30C}" name="PartiGruppe"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D929CE4D-DE0E-4371-9D74-DAF23F806F68}" name="Stopwords" displayName="Stopwords" ref="A1:B27" totalsRowShown="0">
+  <autoFilter ref="A1:B27" xr:uid="{D929CE4D-DE0E-4371-9D74-DAF23F806F68}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{703DE216-50CE-4E57-B997-17634E591F71}" name="Ord"/>
+    <tableColumn id="2" xr3:uid="{A35AE28A-3BB9-4161-A171-35C527B7C143}" name="DatoTilføjet" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -3743,7 +3843,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A493712-F027-4507-94A0-9698A823257D}">
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
@@ -3965,7 +4065,7 @@
       <c r="A27" t="s">
         <v>335</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="1" t="s">
         <v>326</v>
       </c>
     </row>
@@ -3973,7 +4073,7 @@
       <c r="A28" t="s">
         <v>338</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="1" t="s">
         <v>327</v>
       </c>
     </row>
@@ -3981,7 +4081,7 @@
       <c r="A29" t="s">
         <v>339</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="1" t="s">
         <v>328</v>
       </c>
     </row>
@@ -3989,7 +4089,7 @@
       <c r="A30" t="s">
         <v>340</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="1" t="s">
         <v>329</v>
       </c>
     </row>
@@ -3997,7 +4097,7 @@
       <c r="A31" t="s">
         <v>341</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="1" t="s">
         <v>330</v>
       </c>
     </row>
@@ -4005,7 +4105,7 @@
       <c r="A32" t="s">
         <v>342</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="1" t="s">
         <v>331</v>
       </c>
     </row>
@@ -4013,7 +4113,7 @@
       <c r="A33" t="s">
         <v>343</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="1" t="s">
         <v>332</v>
       </c>
     </row>
@@ -4021,7 +4121,7 @@
       <c r="A34" t="s">
         <v>336</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="1" t="s">
         <v>333</v>
       </c>
     </row>
@@ -4029,8 +4129,247 @@
       <c r="A35" t="s">
         <v>337</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="1" t="s">
         <v>334</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF47BBDC-009D-4BC6-8244-D6C5D45FAAE9}">
+  <dimension ref="A1:B27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>371</v>
+      </c>
+      <c r="B2" s="2">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>345</v>
+      </c>
+      <c r="B3" s="2">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>346</v>
+      </c>
+      <c r="B4" s="2">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>347</v>
+      </c>
+      <c r="B5" s="2">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>348</v>
+      </c>
+      <c r="B6" s="2">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>349</v>
+      </c>
+      <c r="B7" s="2">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>350</v>
+      </c>
+      <c r="B8" s="2">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>351</v>
+      </c>
+      <c r="B9" s="2">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>352</v>
+      </c>
+      <c r="B10" s="2">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>353</v>
+      </c>
+      <c r="B11" s="2">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>354</v>
+      </c>
+      <c r="B12" s="2">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>355</v>
+      </c>
+      <c r="B13" s="2">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>356</v>
+      </c>
+      <c r="B14" s="2">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>357</v>
+      </c>
+      <c r="B15" s="2">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>358</v>
+      </c>
+      <c r="B16" s="2">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>359</v>
+      </c>
+      <c r="B17" s="2">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>360</v>
+      </c>
+      <c r="B18" s="2">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>361</v>
+      </c>
+      <c r="B19" s="2">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>362</v>
+      </c>
+      <c r="B20" s="2">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>363</v>
+      </c>
+      <c r="B21" s="2">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>364</v>
+      </c>
+      <c r="B22" s="2">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>365</v>
+      </c>
+      <c r="B23" s="2">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>366</v>
+      </c>
+      <c r="B24" s="2">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>367</v>
+      </c>
+      <c r="B25" s="2">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>368</v>
+      </c>
+      <c r="B26" s="2">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>369</v>
+      </c>
+      <c r="B27" s="2">
+        <v>45566</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added manual mapping of LDA topics
</commit_message>
<xml_diff>
--- a/input/mapping_tabeller.xlsx
+++ b/input/mapping_tabeller.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://maerskbroker-my.sharepoint.com/personal/kbo_maerskbroker_com/Documents/FTIND/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="235" documentId="8_{6B022C61-D3E3-4D46-8183-99CFA6E77F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DBD887C-F43B-4C91-A262-A4111E44DC5D}"/>
+  <xr:revisionPtr revIDLastSave="258" documentId="8_{6B022C61-D3E3-4D46-8183-99CFA6E77F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A241D5D-46B4-4312-8C5D-6A73B88158AD}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{6B009A8E-40F0-41F8-8A22-826EDE827CF8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{6B009A8E-40F0-41F8-8A22-826EDE827CF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Lande" sheetId="1" r:id="rId1"/>
     <sheet name="Ophold" sheetId="2" r:id="rId2"/>
     <sheet name="Partigrupper" sheetId="3" r:id="rId3"/>
     <sheet name="Stopwords" sheetId="4" r:id="rId4"/>
+    <sheet name="Emner" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="386">
   <si>
     <t>Albanien</t>
   </si>
@@ -1155,13 +1156,55 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>Emne</t>
+  </si>
+  <si>
+    <t>EmneNr</t>
+  </si>
+  <si>
+    <t>Noter</t>
+  </si>
+  <si>
+    <t>SidstOpdatret</t>
+  </si>
+  <si>
+    <t>Topic 0</t>
+  </si>
+  <si>
+    <t>Topic 1</t>
+  </si>
+  <si>
+    <t>Topic 2</t>
+  </si>
+  <si>
+    <t>Topic 3</t>
+  </si>
+  <si>
+    <t>Topic 4</t>
+  </si>
+  <si>
+    <t>Regeringen overholder ikke de eksisterende indfødsretsaftaler</t>
+  </si>
+  <si>
+    <t>Ansøgerne har arbejdet hårdt for at opfylde de strenge krav og fortjener en "tillykke"</t>
+  </si>
+  <si>
+    <t>Der er forskellige tilføjelser/ændringsforslag under debatten</t>
+  </si>
+  <si>
+    <t>Nogle mener, at Danmark burde bryde med den internationale konvention om statsløse</t>
+  </si>
+  <si>
+    <t>Ingen flere korte bemærkninger inden afstemning</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1174,6 +1217,12 @@
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1196,15 +1245,39 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="6">
+    <dxf>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
@@ -1260,9 +1333,22 @@
   <autoFilter ref="A1:B27" xr:uid="{D929CE4D-DE0E-4371-9D74-DAF23F806F68}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{703DE216-50CE-4E57-B997-17634E591F71}" name="Ord"/>
-    <tableColumn id="2" xr3:uid="{A35AE28A-3BB9-4161-A171-35C527B7C143}" name="DatoTilføjet" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{A35AE28A-3BB9-4161-A171-35C527B7C143}" name="DatoTilføjet" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{2C1F5FC9-D397-455C-AEAF-D1763528A602}" name="Emner" displayName="Emner" ref="A1:D6" totalsRowShown="0" dataDxfId="0">
+  <autoFilter ref="A1:D6" xr:uid="{2C1F5FC9-D397-455C-AEAF-D1763528A602}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{6F47ADCF-7B5E-431B-8209-B52E2671F6C3}" name="EmneNr" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{625A89F7-2E0B-4AE9-8481-CBE8317B581F}" name="Emne" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{64403E5D-601B-4B88-B55D-4ECF3EA9DC38}" name="Noter" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{CF0732A2-488A-4A32-B356-40B8CE60F4B8}" name="SidstOpdatret" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -4146,7 +4232,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF47BBDC-009D-4BC6-8244-D6C5D45FAAE9}">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -4379,4 +4465,104 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F1D6B43-84E6-4039-8D1A-0E6D941491BF}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="50.21875" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>373</v>
+      </c>
+      <c r="B1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C1" t="s">
+        <v>374</v>
+      </c>
+      <c r="D1" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="5">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="5">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="5">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5">
+        <v>45566</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added mapping for LLM interpretations of LDA topics
</commit_message>
<xml_diff>
--- a/input/mapping_tabeller.xlsx
+++ b/input/mapping_tabeller.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://maerskbroker-my.sharepoint.com/personal/kbo_maerskbroker_com/Documents/FTIND/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://maerskbroker-my.sharepoint.com/personal/kbo_mbshipbrokers_com/Documents/FTIND/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="258" documentId="8_{6B022C61-D3E3-4D46-8183-99CFA6E77F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A241D5D-46B4-4312-8C5D-6A73B88158AD}"/>
+  <xr:revisionPtr revIDLastSave="447" documentId="8_{6B022C61-D3E3-4D46-8183-99CFA6E77F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6AF65B6F-17D8-468D-A206-CE391679819A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{6B009A8E-40F0-41F8-8A22-826EDE827CF8}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="631">
   <si>
     <t>Albanien</t>
   </si>
@@ -1158,53 +1158,788 @@
     <t/>
   </si>
   <si>
-    <t>Emne</t>
-  </si>
-  <si>
-    <t>EmneNr</t>
-  </si>
-  <si>
-    <t>Noter</t>
-  </si>
-  <si>
     <t>SidstOpdatret</t>
   </si>
   <si>
-    <t>Topic 0</t>
-  </si>
-  <si>
-    <t>Topic 1</t>
-  </si>
-  <si>
-    <t>Topic 2</t>
-  </si>
-  <si>
-    <t>Topic 3</t>
-  </si>
-  <si>
-    <t>Topic 4</t>
-  </si>
-  <si>
-    <t>Regeringen overholder ikke de eksisterende indfødsretsaftaler</t>
-  </si>
-  <si>
-    <t>Ansøgerne har arbejdet hårdt for at opfylde de strenge krav og fortjener en "tillykke"</t>
-  </si>
-  <si>
-    <t>Der er forskellige tilføjelser/ændringsforslag under debatten</t>
-  </si>
-  <si>
-    <t>Nogle mener, at Danmark burde bryde med den internationale konvention om statsløse</t>
-  </si>
-  <si>
-    <t>Ingen flere korte bemærkninger inden afstemning</t>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>AutomatiskEmne</t>
+  </si>
+  <si>
+    <t>EmneGruppe</t>
+  </si>
+  <si>
+    <t>2004-E_Topic 0</t>
+  </si>
+  <si>
+    <t>Strammere krav til indfødsret: Behov for kulturel beskyttelse i Danmark</t>
+  </si>
+  <si>
+    <t>2004-E_Topic 1</t>
+  </si>
+  <si>
+    <t>Indvandringspolitik: Uenighed om lighed og statsborgerskab i Danmark</t>
+  </si>
+  <si>
+    <t>2004-E_Topic 2</t>
+  </si>
+  <si>
+    <t>Strammere krav til indfødsret er ikke løsningen for Danmark</t>
+  </si>
+  <si>
+    <t>2004-E_Topic 3</t>
+  </si>
+  <si>
+    <t>Kritik af danske uddannelseskrav som hindring for indvandrere</t>
+  </si>
+  <si>
+    <t>2005-E_Topic 0</t>
+  </si>
+  <si>
+    <t>Støtte til statsborgerskab med fokus på integration og sammenhængskraft</t>
+  </si>
+  <si>
+    <t>2005-E_Topic 1</t>
+  </si>
+  <si>
+    <t>Sprogkrav og indfødsret: En kritisk vurdering af dansk kulturpolitik</t>
+  </si>
+  <si>
+    <t>2005-E_Topic 2</t>
+  </si>
+  <si>
+    <t>Skærpelse af kravene til dansk indfødsret for at beskytte kultur og sikkerhed</t>
+  </si>
+  <si>
+    <t>2005-E_Topic 3</t>
+  </si>
+  <si>
+    <t>Retssikkerhed og inklusion i dansk statsborgerskabstildeling</t>
+  </si>
+  <si>
+    <t>2006-E_Topic 0</t>
+  </si>
+  <si>
+    <t>Krav om tilpasning og respekt for danske værdier ved nyborgerskab</t>
+  </si>
+  <si>
+    <t>2006-E_Topic 1</t>
+  </si>
+  <si>
+    <t>Retfærdighed i indfødsretslovgivningen for udsatte grupper i Danmark</t>
+  </si>
+  <si>
+    <t>2006-E_Topic 2</t>
+  </si>
+  <si>
+    <t>Børn fortjener dansk statsborgerskab trods fejlregistreringer</t>
+  </si>
+  <si>
+    <t>2006-E_Topic 3</t>
+  </si>
+  <si>
+    <t>Uenighed om indfødsret: Sygdom som berettigelse afvist</t>
+  </si>
+  <si>
+    <t>2006-F_Topic 0</t>
+  </si>
+  <si>
+    <t>"Det Radikale Venstre: Fornuftige krav til nye statsborgere med plads til dispensation"</t>
+  </si>
+  <si>
+    <t>2006-F_Topic 1</t>
+  </si>
+  <si>
+    <t>"Støtte til inkludering af flygtninge i det danske demokrati"</t>
+  </si>
+  <si>
+    <t>2006-F_Topic 2</t>
+  </si>
+  <si>
+    <t>Rimelige krav og anerkendelse af særlige dispensationer for statsborgerskab</t>
+  </si>
+  <si>
+    <t>2006-F_Topic 3</t>
+  </si>
+  <si>
+    <t>Krav om Dansk Sprogkundskab og Psykiske Lidelsers Hensyn i Indfødsret</t>
+  </si>
+  <si>
+    <t>2007-F_Topic 0</t>
+  </si>
+  <si>
+    <t>Socialdemokratiet arbejder for løsning af indfødsretsprøveproblematikken.</t>
+  </si>
+  <si>
+    <t>2007-F_Topic 1</t>
+  </si>
+  <si>
+    <t>Retfærdighed i indfødsretsprøven skal prioriteres højere</t>
+  </si>
+  <si>
+    <t>2007-F_Topic 2</t>
+  </si>
+  <si>
+    <t>Kritik af stramme regler for dansk statsborgerskab og integration</t>
+  </si>
+  <si>
+    <t>2008-E_Topic 0</t>
+  </si>
+  <si>
+    <t>Kritik af ændringer i indfødsret og afvisning af dobbelt statsborgerskab</t>
+  </si>
+  <si>
+    <t>2008-E_Topic 1</t>
+  </si>
+  <si>
+    <t>Kritik af skærpede krav til dansk statsborgerskab og betydningen af integration</t>
+  </si>
+  <si>
+    <t>2008-E_Topic 2</t>
+  </si>
+  <si>
+    <t>Vigtigheden af respekt for nye danske statsborgerskaber og integration</t>
+  </si>
+  <si>
+    <t>2008-F_Topic 2</t>
+  </si>
+  <si>
+    <t>Debat om krav og dispensation i indfødsretspolitik</t>
+  </si>
+  <si>
+    <t>2008-F_Topic 3</t>
+  </si>
+  <si>
+    <t>Understøttelse af indfødsret og forventninger til ministerens svar</t>
+  </si>
+  <si>
+    <t>2009-E_Topic 1</t>
+  </si>
+  <si>
+    <t>Støtte til indfødsret og integration for nye borgere i Danmark</t>
+  </si>
+  <si>
+    <t>2009-E_Topic 2</t>
+  </si>
+  <si>
+    <t>Kritik af regeringens stramninger i integrationsreglerne trods erkendte udfordringer.</t>
+  </si>
+  <si>
+    <t>2009-F_Topic 0</t>
+  </si>
+  <si>
+    <t>Indfødsretsprøven: En nødvendig garanti for dansk identitet</t>
+  </si>
+  <si>
+    <t>2009-F_Topic 1</t>
+  </si>
+  <si>
+    <t>Bevarelse af dansk identitet gennem strenge statsborgerskabsregler</t>
+  </si>
+  <si>
+    <t>2009-F_Topic 2</t>
+  </si>
+  <si>
+    <t>Fejring af nytilkomne danske statsborgere styrker demokratiet og rettighederne.</t>
+  </si>
+  <si>
+    <t>2009-F_Topic 3</t>
+  </si>
+  <si>
+    <t>Trygheden ved dansk statsborgerskab og nødvendigheden af én national identitet</t>
+  </si>
+  <si>
+    <t>2010-E_Topic 0</t>
+  </si>
+  <si>
+    <t>Kritik af ministerens påstand og støtte til Folketingets selvbestemmelse</t>
+  </si>
+  <si>
+    <t>2010-E_Topic 1</t>
+  </si>
+  <si>
+    <t>Forsvarsretter om grundlovens autoritet kontra FN-konventioner i indfødsretsspørgsmål</t>
+  </si>
+  <si>
+    <t>2010-E_Topic 2</t>
+  </si>
+  <si>
+    <t>Politisk debat om dansk indfødsret og statsborgerskabspraksis</t>
+  </si>
+  <si>
+    <t>2010-F_Topic 0</t>
+  </si>
+  <si>
+    <t>Statsborgerskab i Danmark: Vigtigheden af Loyalitet og Viden</t>
+  </si>
+  <si>
+    <t>2011-E_Topic 0</t>
+  </si>
+  <si>
+    <t>Demokratisk debat og retssikkerhed i statsborgerskabsreformer</t>
+  </si>
+  <si>
+    <t>2011-E_Topic 1</t>
+  </si>
+  <si>
+    <t>Prioritering af national sikkerhed i indfødsretsdebatten</t>
+  </si>
+  <si>
+    <t>2011-E_Topic 2</t>
+  </si>
+  <si>
+    <t>Kritik af Venstre og opfordring til ændring af sikkerhedskonventioner</t>
+  </si>
+  <si>
+    <t>2011-E_Topic 3</t>
+  </si>
+  <si>
+    <t>Venstre kræver reform af statsborgerskab ved kriminalitet og sikkerhed</t>
+  </si>
+  <si>
+    <t>2011-F_Topic 0</t>
+  </si>
+  <si>
+    <t>Kritik af sagsbehandling ved tildeling af dansk statsborgerskab</t>
+  </si>
+  <si>
+    <t>2011-F_Topic 1</t>
+  </si>
+  <si>
+    <t>Dansk Folkepartis modstand mod FN-konventionen om indfødsret</t>
+  </si>
+  <si>
+    <t>2012-E_Topic 0</t>
+  </si>
+  <si>
+    <t>Konservative støtter inklusion af statsborgerskab for kvalificerede ansøgere</t>
+  </si>
+  <si>
+    <t>2012-E_Topic 1</t>
+  </si>
+  <si>
+    <t>Kritik og støtte til lovgivning om statsborgerskab i Danmark</t>
+  </si>
+  <si>
+    <t>2012-E_Topic 2</t>
+  </si>
+  <si>
+    <t>Støtte til statsborgerskab som anerkendelse af tilknytning til Danmark</t>
+  </si>
+  <si>
+    <t>2012-F_Topic 0</t>
+  </si>
+  <si>
+    <t>Statsborgerskab: Udfordringer og Bekymringer ved Inkludering af Udlændinge</t>
+  </si>
+  <si>
+    <t>2012-F_Topic 1</t>
+  </si>
+  <si>
+    <t>"Støtte til rimelig indfødsret og ny dansk statsborgerskabspolitik"</t>
+  </si>
+  <si>
+    <t>2012-F_Topic 2</t>
+  </si>
+  <si>
+    <t>Kritik af statsborgerskab til kriminelle og sikkerhedstrusler</t>
+  </si>
+  <si>
+    <t>2012-F_Topic 3</t>
+  </si>
+  <si>
+    <t>Kritik af tildeling af dansk statsborgerskab til sikkerhedsrisici</t>
+  </si>
+  <si>
+    <t>2013-E_Topic 0</t>
+  </si>
+  <si>
+    <t>Dansk Folkepartis kritik af statsborgerskabspolitik og integrationstiltag</t>
+  </si>
+  <si>
+    <t>2013-E_Topic 1</t>
+  </si>
+  <si>
+    <t>Kritik af Dansk Folkepartis diskriminerende holdninger til statsborgerskab</t>
+  </si>
+  <si>
+    <t>2013-E_Topic 2</t>
+  </si>
+  <si>
+    <t>Statsborgerskab i Danmark: Balancen mellem krav og muligheder</t>
+  </si>
+  <si>
+    <t>2013-E_Topic 3</t>
+  </si>
+  <si>
+    <t>Modstand mod indvandring og statsborgerskab for muslimske lande</t>
+  </si>
+  <si>
+    <t>2013-F_Topic 0</t>
+  </si>
+  <si>
+    <t>Debatten om statsborgerskab, sikkerhed og politiske ansvarligheder i Danmark</t>
+  </si>
+  <si>
+    <t>2013-F_Topic 1</t>
+  </si>
+  <si>
+    <t>Offentlighedens Ret til Information vs. Fortrolighed og Strafansvar</t>
+  </si>
+  <si>
+    <t>2013-F_Topic 2</t>
+  </si>
+  <si>
+    <t>"Uenighed om statsborgerskab og fortrolighed i Folketinget"</t>
+  </si>
+  <si>
+    <t>2013-F_Topic 3</t>
+  </si>
+  <si>
+    <t>Kritik af regeringens håndtering af statsborgerskabs- og integrationspolitik</t>
+  </si>
+  <si>
+    <t>2014-E_Topic 0</t>
+  </si>
+  <si>
+    <t>Strammere krav til dansk statsborgerskab er nødvendige nu</t>
+  </si>
+  <si>
+    <t>2014-E_Topic 1</t>
+  </si>
+  <si>
+    <t>Statsborgerskab og integration: Vigtigheden af sprogkundskaber i Danmark</t>
+  </si>
+  <si>
+    <t>2014-E_Topic 3</t>
+  </si>
+  <si>
+    <t>Liberal Alliances støtte til problematisk lovforslag om statsborgerskab</t>
+  </si>
+  <si>
+    <t>2014-F_Topic 0</t>
+  </si>
+  <si>
+    <t>Positiv støtte til dansk statsborgerskab og traditionsbevarelse</t>
+  </si>
+  <si>
+    <t>2014-F_Topic 1</t>
+  </si>
+  <si>
+    <t>Anerkendelse af udfordringer for statsborgerskabssøgere i Danmark</t>
+  </si>
+  <si>
+    <t>2014-F_Topic 2</t>
+  </si>
+  <si>
+    <t>Forbedring af statsborgerskabsprocessen er nødvendig for familier.</t>
+  </si>
+  <si>
+    <t>2014-F_Topic 3</t>
+  </si>
+  <si>
+    <t>Støtte til flere statsborgerskaber fremmer dansk fællesskab og rettigheder.</t>
+  </si>
+  <si>
+    <t>2015-E_Topic 0</t>
+  </si>
+  <si>
+    <t>Politisk Anstændighed i Debatten om Indfødsret og Statsborgerskab</t>
+  </si>
+  <si>
+    <t>2015-E_Topic 1</t>
+  </si>
+  <si>
+    <t>"Vurdering af danske statsborgerskabsansøgere: Loyalitet og demokratisk accept"</t>
+  </si>
+  <si>
+    <t>2015-E_Topic 2</t>
+  </si>
+  <si>
+    <t>"Politisk debat om statsborgerskab og ytringsfrihed i Danmark"</t>
+  </si>
+  <si>
+    <t>2015-E_Topic 3</t>
+  </si>
+  <si>
+    <t>Fru Lotte Rod og Radikale Venstre: En Uendelig Tale om Demokrati</t>
+  </si>
+  <si>
+    <t>2016-E_Topic 0</t>
+  </si>
+  <si>
+    <t>Dansk Folkeparti ønsker strammere krav for dansk statsborgerskab.</t>
+  </si>
+  <si>
+    <t>2016-E_Topic 3</t>
+  </si>
+  <si>
+    <t>Fjern unødvendige forhindringer for dansk statsborgerskab for at styrke samfundet.</t>
+  </si>
+  <si>
+    <t>2016-F_Topic 0</t>
+  </si>
+  <si>
+    <t>Kritik af mangelfuld sagsbehandling i indfødsretssager</t>
+  </si>
+  <si>
+    <t>2016-F_Topic 2</t>
+  </si>
+  <si>
+    <t>Afstemning om ændringsforslag og politiske vurderinger af statsborgerskab</t>
+  </si>
+  <si>
+    <t>2016-F_Topic 3</t>
+  </si>
+  <si>
+    <t>Statsborgerskab: Krav om integration og retssikkerhed i Danmark</t>
+  </si>
+  <si>
+    <t>2017-E_Topic 0</t>
+  </si>
+  <si>
+    <t>Retssikkerhed for alle: Bekymringer ved dansk statsborgerskabslovgivning</t>
+  </si>
+  <si>
+    <t>2017-E_Topic 1</t>
+  </si>
+  <si>
+    <t>Kravene for dansk statsborgerskab som en vigtig privilegium</t>
+  </si>
+  <si>
+    <t>2017-E_Topic 2</t>
+  </si>
+  <si>
+    <t>Støtte til L 71: Anerkendelse af nye danskere som aktive samfundsborgere</t>
+  </si>
+  <si>
+    <t>2017-F_Topic 0</t>
+  </si>
+  <si>
+    <t>Afstemning om ændringsforslag vedrørende statsborgerskab og indvandringspolitik</t>
+  </si>
+  <si>
+    <t>2017-F_Topic 1</t>
+  </si>
+  <si>
+    <t>Dansk statsborgerskab: Udfordringer og muligheder for integration</t>
+  </si>
+  <si>
+    <t>2017-F_Topic 2</t>
+  </si>
+  <si>
+    <t>Støtte til statsborgerskab fremmer integration og demokratisk deltagelse</t>
+  </si>
+  <si>
+    <t>2017-F_Topic 3</t>
+  </si>
+  <si>
+    <t>Støtte til fru Laura Lindahl og Liberal Alliance's politikker.</t>
+  </si>
+  <si>
+    <t>2018-E_Topic 0</t>
+  </si>
+  <si>
+    <t>Krav om retfærdighed og inklusion i dansk statsborgerskabssystem</t>
+  </si>
+  <si>
+    <t>2018-E_Topic 1</t>
+  </si>
+  <si>
+    <t>Støtte til statsborgerskab med fokus på demokrati og værdier</t>
+  </si>
+  <si>
+    <t>2018-E_Topic 2</t>
+  </si>
+  <si>
+    <t>Statsborgerskab i Danmark: Behov for klare krav og integration</t>
+  </si>
+  <si>
+    <t>2018-E_Topic 3</t>
+  </si>
+  <si>
+    <t>Velkommen til nye danske statsborgere: Vigtigheden af inklusion i samfundet</t>
+  </si>
+  <si>
+    <t>2018-F_Topic 0</t>
+  </si>
+  <si>
+    <t>Fremme af statsborgerskab for bedre integration i Danmark</t>
+  </si>
+  <si>
+    <t>2018-F_Topic 1</t>
+  </si>
+  <si>
+    <t>Strammere krav til statsborgerskab for at beskytte dansk kultur</t>
+  </si>
+  <si>
+    <t>2018-F_Topic 3</t>
+  </si>
+  <si>
+    <t>Venstre støtter dansk statsborgerskab med krav om loyalitet og kulturforståelse</t>
+  </si>
+  <si>
+    <t>2019-E_Topic 0</t>
+  </si>
+  <si>
+    <t>Strengere krav til indfødsret for bedre integration i Danmark</t>
+  </si>
+  <si>
+    <t>2019-E_Topic 1</t>
+  </si>
+  <si>
+    <t>Lettere adgang til statsborgerskab: Enhedslistens forslag til reformer</t>
+  </si>
+  <si>
+    <t>2019-E_Topic 2</t>
+  </si>
+  <si>
+    <t>Krav til Statsborgerskab: Balancen mellem Integration og Kontrol</t>
+  </si>
+  <si>
+    <t>2019-E_Topic 3</t>
+  </si>
+  <si>
+    <t>Kritik af lovforslag L 41 og fokus på Danmarks sikkerhed</t>
+  </si>
+  <si>
+    <t>2020-E_Topic 0</t>
+  </si>
+  <si>
+    <t>Statsborgerskab: Gennemsigtighed, Retssikkerhed og Politisk Ansvarsbevidsthed</t>
+  </si>
+  <si>
+    <t>2020-E_Topic 1</t>
+  </si>
+  <si>
+    <t>Strammere regler for statsborgerskab og ansvarlighed i Danmark</t>
+  </si>
+  <si>
+    <t>2020-E_Topic 2</t>
+  </si>
+  <si>
+    <t>"Debat om dansk statsborgerskab og retssikkerhed for ansøgere"</t>
+  </si>
+  <si>
+    <t>2020-E_Topic 3</t>
+  </si>
+  <si>
+    <t>Strammere regler og individuel vurdering i dansk statsborgerskabspolitik</t>
+  </si>
+  <si>
+    <t>2020-F_Topic 0</t>
+  </si>
+  <si>
+    <t>Reform af danske statsborgerskabsregler: Retfærdighed og lighed for alle ansøgere</t>
+  </si>
+  <si>
+    <t>2020-F_Topic 1</t>
+  </si>
+  <si>
+    <t>Strammere krav til dansk statsborgerskab og respekt for kulturværdier</t>
+  </si>
+  <si>
+    <t>2020-F_Topic 2</t>
+  </si>
+  <si>
+    <t>Statsborgerskab i Danmark: Krav om tilpasning og håndtryk</t>
+  </si>
+  <si>
+    <t>2020-F_Topic 3</t>
+  </si>
+  <si>
+    <t>Strammere krav til indfødsret og statsborgerskab i Danmark</t>
+  </si>
+  <si>
+    <t>2021-E_Topic 0</t>
+  </si>
+  <si>
+    <t>Strengere krav til statsborgerskab: Fokus på fortjeneste og gennemsigtighed</t>
+  </si>
+  <si>
+    <t>2021-E_Topic 1</t>
+  </si>
+  <si>
+    <t>Kritik af ministerens håndtering af dansk statsborgerskabsspørgsmål</t>
+  </si>
+  <si>
+    <t>2021-E_Topic 2</t>
+  </si>
+  <si>
+    <t>Strenge krav og diskussioner om dansk statsborgerskab og værdier</t>
+  </si>
+  <si>
+    <t>2021-E_Topic 3</t>
+  </si>
+  <si>
+    <t>Retfærdig og objektiv behandling af statsborgerskab i Danmark</t>
+  </si>
+  <si>
+    <t>2021-F_Topic 0</t>
+  </si>
+  <si>
+    <t>Reform af statsborgerskabsregler for bedre inklusion i Danmark</t>
+  </si>
+  <si>
+    <t>2021-F_Topic 1</t>
+  </si>
+  <si>
+    <t>"Afstemning om lovforslag og grundlovens krav til skattepligt"</t>
+  </si>
+  <si>
+    <t>2021-F_Topic 2</t>
+  </si>
+  <si>
+    <t>Anerkendelse og kontrol i dansk statsborgerskabsdebat</t>
+  </si>
+  <si>
+    <t>2021-F_Topic 3</t>
+  </si>
+  <si>
+    <t>Kritik af statsborgerskabstildeling og krav til kommende danskere</t>
+  </si>
+  <si>
+    <t>2022-E_Topic 0</t>
+  </si>
+  <si>
+    <t>Balancen mellem strenge kriterier og retssikkerhed i dansk indfødsret</t>
+  </si>
+  <si>
+    <t>2022-E_Topic 1</t>
+  </si>
+  <si>
+    <t>Statsborgerskab og kriminalitet: En debat om ansvar og rettigheder</t>
+  </si>
+  <si>
+    <t>2022-E_Topic 2</t>
+  </si>
+  <si>
+    <t>Reform af danske statsborgerskabsregler for at sikre samfundsengagement</t>
+  </si>
+  <si>
+    <t>2022-E_Topic 3</t>
+  </si>
+  <si>
+    <t>Retfærdighed og ansvarlighed i dansk statsborgerskab og indfødsretssystemet</t>
+  </si>
+  <si>
+    <t>2022-F_Topic 0</t>
+  </si>
+  <si>
+    <t>Anerkendelse af mangfoldighed i indfødsretsaftalen er essentiel</t>
+  </si>
+  <si>
+    <t>2022-F_Topic 1</t>
+  </si>
+  <si>
+    <t>Kritik af massetildeling af statsborgerskaber i Danmark</t>
+  </si>
+  <si>
+    <t>2022-F_Topic 2</t>
+  </si>
+  <si>
+    <t>Statsborgerskab: Stolthed, Inklusion og Strenge Kriterier i Danmark</t>
+  </si>
+  <si>
+    <t>2022-F_Topic 3</t>
+  </si>
+  <si>
+    <t>Statsborgerskab som privilegium: Behov for værdige ansøgere</t>
+  </si>
+  <si>
+    <t>2023-E_Topic 0</t>
+  </si>
+  <si>
+    <t>Kritik af sikkerhed og kontrol i dansk statsborgerskabstildeling</t>
+  </si>
+  <si>
+    <t>2023-E_Topic 1</t>
+  </si>
+  <si>
+    <t>Restriktiv tilgang til dansk statsborgerskab og indvandreres værdier</t>
+  </si>
+  <si>
+    <t>2023-E_Topic 2</t>
+  </si>
+  <si>
+    <t>Retfærdighed og ansvarlighed i tildeling af dansk statsborgerskab</t>
+  </si>
+  <si>
+    <t>2023-E_Topic 3</t>
+  </si>
+  <si>
+    <t>Afstemning om ændringsforslag og lovforslagets vedtagelse i Folketinget</t>
+  </si>
+  <si>
+    <t>2023-F_Topic 0</t>
+  </si>
+  <si>
+    <t>Modstand mod ændringsforslag og lovgivning i dansk politik</t>
+  </si>
+  <si>
+    <t>2023-F_Topic 1</t>
+  </si>
+  <si>
+    <t>Kritik af Danmarks Indfødsretspraksis og Handicapdiskrimination</t>
+  </si>
+  <si>
+    <t>2024-F_Topic 0</t>
+  </si>
+  <si>
+    <t>Afstemning om ændringsforslag fra DF: En ensidig afvisning</t>
+  </si>
+  <si>
+    <t>2024-F_Topic 1</t>
+  </si>
+  <si>
+    <t>Strammere krav til dansk statsborgerskab for at beskytte samfundet</t>
+  </si>
+  <si>
+    <t>Kravene til indfødsret skal være stramme(re)</t>
+  </si>
+  <si>
+    <t>Ingen behov for at have strammere krav til indfødsret</t>
+  </si>
+  <si>
+    <t>De eksisterende krav til indfødsret er urimelige</t>
+  </si>
+  <si>
+    <t>Statsborgerskab er vejen til integration og lighed</t>
+  </si>
+  <si>
+    <t>Der er forskellige holdninger til at give dispensation fra reglerne</t>
+  </si>
+  <si>
+    <t>Dansk kultur og indentitet skal bevares som de er</t>
+  </si>
+  <si>
+    <t>Tildeling af statsborgerskaber påvirker nationalsikkerheden</t>
+  </si>
+  <si>
+    <t>Danmark har visse forpligtelser ifm. internationale konventioner</t>
+  </si>
+  <si>
+    <t>Den nuværende sagsbehandling af ansøgninger er ikke optimal</t>
+  </si>
+  <si>
+    <t>Der skal være balance mellem krav og virkelighed</t>
+  </si>
+  <si>
+    <t>Der er bekymringer om integration og/eller kriminalitet</t>
+  </si>
+  <si>
+    <t>Dansk statsborgerskab er en gave og et privilegium</t>
+  </si>
+  <si>
+    <t>Generel snak/procedure/debat mellem politiske modstandere</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1224,6 +1959,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1233,12 +1976,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1249,15 +2007,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1270,10 +2026,10 @@
       <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1340,15 +2096,15 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{2C1F5FC9-D397-455C-AEAF-D1763528A602}" name="Emner" displayName="Emner" ref="A1:D6" totalsRowShown="0" dataDxfId="0">
-  <autoFilter ref="A1:D6" xr:uid="{2C1F5FC9-D397-455C-AEAF-D1763528A602}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{2C1F5FC9-D397-455C-AEAF-D1763528A602}" name="Emner" displayName="Emner" ref="A1:D122" totalsRowShown="0" dataDxfId="4">
+  <autoFilter ref="A1:D122" xr:uid="{2C1F5FC9-D397-455C-AEAF-D1763528A602}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{6F47ADCF-7B5E-431B-8209-B52E2671F6C3}" name="EmneNr" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{625A89F7-2E0B-4AE9-8481-CBE8317B581F}" name="Emne" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{64403E5D-601B-4B88-B55D-4ECF3EA9DC38}" name="Noter" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{CF0732A2-488A-4A32-B356-40B8CE60F4B8}" name="SidstOpdatret" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{6F47ADCF-7B5E-431B-8209-B52E2671F6C3}" name="Id" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{625A89F7-2E0B-4AE9-8481-CBE8317B581F}" name="AutomatiskEmne" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{64403E5D-601B-4B88-B55D-4ECF3EA9DC38}" name="EmneGruppe" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{CF0732A2-488A-4A32-B356-40B8CE60F4B8}" name="SidstOpdatret" dataDxfId="0"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -4469,92 +5225,1726 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F1D6B43-84E6-4039-8D1A-0E6D941491BF}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="C122" sqref="C122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" customWidth="1"/>
-    <col min="2" max="2" width="50.21875" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="1" max="1" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>373</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="D1" t="s">
         <v>372</v>
       </c>
-      <c r="C1" t="s">
-        <v>374</v>
-      </c>
-      <c r="D1" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>376</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
+        <v>377</v>
+      </c>
+      <c r="C2" t="s">
+        <v>623</v>
+      </c>
+      <c r="D2" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>378</v>
+      </c>
+      <c r="B3" t="s">
+        <v>379</v>
+      </c>
+      <c r="C3" t="s">
+        <v>621</v>
+      </c>
+      <c r="D3" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>380</v>
+      </c>
+      <c r="B4" t="s">
         <v>381</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="5">
-        <v>45566</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="C4" t="s">
+        <v>619</v>
+      </c>
+      <c r="D4" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>382</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="5">
-        <v>45566</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>378</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="B5" t="s">
         <v>383</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5">
-        <v>45566</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" t="s">
+        <v>620</v>
+      </c>
+      <c r="D5" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>384</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5">
-        <v>45566</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>380</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>385</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5">
-        <v>45566</v>
+      <c r="C6" t="s">
+        <v>621</v>
+      </c>
+      <c r="D6" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>386</v>
+      </c>
+      <c r="B7" t="s">
+        <v>387</v>
+      </c>
+      <c r="C7" t="s">
+        <v>618</v>
+      </c>
+      <c r="D7" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>388</v>
+      </c>
+      <c r="B8" t="s">
+        <v>389</v>
+      </c>
+      <c r="C8" t="s">
+        <v>618</v>
+      </c>
+      <c r="D8" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>390</v>
+      </c>
+      <c r="B9" t="s">
+        <v>391</v>
+      </c>
+      <c r="C9" t="s">
+        <v>624</v>
+      </c>
+      <c r="D9" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>392</v>
+      </c>
+      <c r="B10" t="s">
+        <v>393</v>
+      </c>
+      <c r="C10" t="s">
+        <v>618</v>
+      </c>
+      <c r="D10" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>394</v>
+      </c>
+      <c r="B11" t="s">
+        <v>395</v>
+      </c>
+      <c r="C11" t="s">
+        <v>621</v>
+      </c>
+      <c r="D11" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>396</v>
+      </c>
+      <c r="B12" t="s">
+        <v>397</v>
+      </c>
+      <c r="C12" t="s">
+        <v>621</v>
+      </c>
+      <c r="D12" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>398</v>
+      </c>
+      <c r="B13" t="s">
+        <v>399</v>
+      </c>
+      <c r="C13" t="s">
+        <v>618</v>
+      </c>
+      <c r="D13" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>400</v>
+      </c>
+      <c r="B14" t="s">
+        <v>401</v>
+      </c>
+      <c r="C14" t="s">
+        <v>620</v>
+      </c>
+      <c r="D14" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>402</v>
+      </c>
+      <c r="B15" t="s">
+        <v>403</v>
+      </c>
+      <c r="C15" t="s">
+        <v>621</v>
+      </c>
+      <c r="D15" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>404</v>
+      </c>
+      <c r="B16" t="s">
+        <v>405</v>
+      </c>
+      <c r="C16" t="s">
+        <v>620</v>
+      </c>
+      <c r="D16" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>406</v>
+      </c>
+      <c r="B17" t="s">
+        <v>407</v>
+      </c>
+      <c r="C17" t="s">
+        <v>620</v>
+      </c>
+      <c r="D17" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>408</v>
+      </c>
+      <c r="B18" t="s">
+        <v>409</v>
+      </c>
+      <c r="C18" t="s">
+        <v>630</v>
+      </c>
+      <c r="D18" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>410</v>
+      </c>
+      <c r="B19" t="s">
+        <v>411</v>
+      </c>
+      <c r="C19" t="s">
+        <v>620</v>
+      </c>
+      <c r="D19" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>412</v>
+      </c>
+      <c r="B20" t="s">
+        <v>413</v>
+      </c>
+      <c r="C20" t="s">
+        <v>620</v>
+      </c>
+      <c r="D20" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>414</v>
+      </c>
+      <c r="B21" t="s">
+        <v>415</v>
+      </c>
+      <c r="C21" t="s">
+        <v>618</v>
+      </c>
+      <c r="D21" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>416</v>
+      </c>
+      <c r="B22" t="s">
+        <v>417</v>
+      </c>
+      <c r="C22" t="s">
+        <v>620</v>
+      </c>
+      <c r="D22" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>418</v>
+      </c>
+      <c r="B23" t="s">
+        <v>419</v>
+      </c>
+      <c r="C23" t="s">
+        <v>621</v>
+      </c>
+      <c r="D23" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>420</v>
+      </c>
+      <c r="B24" t="s">
+        <v>421</v>
+      </c>
+      <c r="C24" t="s">
+        <v>622</v>
+      </c>
+      <c r="D24" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>422</v>
+      </c>
+      <c r="B25" t="s">
+        <v>423</v>
+      </c>
+      <c r="C25" t="s">
+        <v>630</v>
+      </c>
+      <c r="D25" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>424</v>
+      </c>
+      <c r="B26" t="s">
+        <v>425</v>
+      </c>
+      <c r="C26" t="s">
+        <v>621</v>
+      </c>
+      <c r="D26" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>426</v>
+      </c>
+      <c r="B27" t="s">
+        <v>427</v>
+      </c>
+      <c r="C27" t="s">
+        <v>620</v>
+      </c>
+      <c r="D27" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>428</v>
+      </c>
+      <c r="B28" t="s">
+        <v>429</v>
+      </c>
+      <c r="C28" t="s">
+        <v>618</v>
+      </c>
+      <c r="D28" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>430</v>
+      </c>
+      <c r="B29" t="s">
+        <v>431</v>
+      </c>
+      <c r="C29" t="s">
+        <v>623</v>
+      </c>
+      <c r="D29" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>432</v>
+      </c>
+      <c r="B30" t="s">
+        <v>433</v>
+      </c>
+      <c r="C30" t="s">
+        <v>621</v>
+      </c>
+      <c r="D30" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>434</v>
+      </c>
+      <c r="B31" t="s">
+        <v>435</v>
+      </c>
+      <c r="C31" t="s">
+        <v>621</v>
+      </c>
+      <c r="D31" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>436</v>
+      </c>
+      <c r="B32" t="s">
+        <v>437</v>
+      </c>
+      <c r="C32" t="s">
+        <v>630</v>
+      </c>
+      <c r="D32" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>438</v>
+      </c>
+      <c r="B33" t="s">
+        <v>439</v>
+      </c>
+      <c r="C33" t="s">
+        <v>625</v>
+      </c>
+      <c r="D33" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>440</v>
+      </c>
+      <c r="B34" t="s">
+        <v>441</v>
+      </c>
+      <c r="C34" t="s">
+        <v>630</v>
+      </c>
+      <c r="D34" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>442</v>
+      </c>
+      <c r="B35" t="s">
+        <v>443</v>
+      </c>
+      <c r="C35" t="s">
+        <v>624</v>
+      </c>
+      <c r="D35" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>444</v>
+      </c>
+      <c r="B36" t="s">
+        <v>445</v>
+      </c>
+      <c r="C36" t="s">
+        <v>621</v>
+      </c>
+      <c r="D36" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>446</v>
+      </c>
+      <c r="B37" t="s">
+        <v>447</v>
+      </c>
+      <c r="C37" t="s">
+        <v>624</v>
+      </c>
+      <c r="D37" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>448</v>
+      </c>
+      <c r="B38" t="s">
+        <v>449</v>
+      </c>
+      <c r="C38" t="s">
+        <v>625</v>
+      </c>
+      <c r="D38" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>450</v>
+      </c>
+      <c r="B39" t="s">
+        <v>451</v>
+      </c>
+      <c r="C39" t="s">
+        <v>618</v>
+      </c>
+      <c r="D39" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>452</v>
+      </c>
+      <c r="B40" t="s">
+        <v>453</v>
+      </c>
+      <c r="C40" t="s">
+        <v>626</v>
+      </c>
+      <c r="D40" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>454</v>
+      </c>
+      <c r="B41" t="s">
+        <v>455</v>
+      </c>
+      <c r="C41" t="s">
+        <v>625</v>
+      </c>
+      <c r="D41" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>456</v>
+      </c>
+      <c r="B42" t="s">
+        <v>457</v>
+      </c>
+      <c r="C42" t="s">
+        <v>621</v>
+      </c>
+      <c r="D42" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>458</v>
+      </c>
+      <c r="B43" t="s">
+        <v>459</v>
+      </c>
+      <c r="C43" t="s">
+        <v>630</v>
+      </c>
+      <c r="D43" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>460</v>
+      </c>
+      <c r="B44" t="s">
+        <v>461</v>
+      </c>
+      <c r="C44" t="s">
+        <v>621</v>
+      </c>
+      <c r="D44" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>462</v>
+      </c>
+      <c r="B45" t="s">
+        <v>463</v>
+      </c>
+      <c r="C45" t="s">
+        <v>628</v>
+      </c>
+      <c r="D45" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>464</v>
+      </c>
+      <c r="B46" t="s">
+        <v>465</v>
+      </c>
+      <c r="C46" t="s">
+        <v>620</v>
+      </c>
+      <c r="D46" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>466</v>
+      </c>
+      <c r="B47" t="s">
+        <v>467</v>
+      </c>
+      <c r="C47" t="s">
+        <v>624</v>
+      </c>
+      <c r="D47" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>468</v>
+      </c>
+      <c r="B48" t="s">
+        <v>469</v>
+      </c>
+      <c r="C48" t="s">
+        <v>624</v>
+      </c>
+      <c r="D48" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>470</v>
+      </c>
+      <c r="B49" t="s">
+        <v>471</v>
+      </c>
+      <c r="C49" t="s">
+        <v>628</v>
+      </c>
+      <c r="D49" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>472</v>
+      </c>
+      <c r="B50" t="s">
+        <v>473</v>
+      </c>
+      <c r="C50" t="s">
+        <v>620</v>
+      </c>
+      <c r="D50" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>474</v>
+      </c>
+      <c r="B51" t="s">
+        <v>475</v>
+      </c>
+      <c r="C51" t="s">
+        <v>627</v>
+      </c>
+      <c r="D51" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>476</v>
+      </c>
+      <c r="B52" t="s">
+        <v>477</v>
+      </c>
+      <c r="C52" t="s">
+        <v>628</v>
+      </c>
+      <c r="D52" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>478</v>
+      </c>
+      <c r="B53" t="s">
+        <v>479</v>
+      </c>
+      <c r="C53" t="s">
+        <v>624</v>
+      </c>
+      <c r="D53" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>480</v>
+      </c>
+      <c r="B54" t="s">
+        <v>481</v>
+      </c>
+      <c r="C54" t="s">
+        <v>626</v>
+      </c>
+      <c r="D54" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>482</v>
+      </c>
+      <c r="B55" t="s">
+        <v>483</v>
+      </c>
+      <c r="C55" t="s">
+        <v>626</v>
+      </c>
+      <c r="D55" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>484</v>
+      </c>
+      <c r="B56" t="s">
+        <v>485</v>
+      </c>
+      <c r="C56" t="s">
+        <v>628</v>
+      </c>
+      <c r="D56" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>486</v>
+      </c>
+      <c r="B57" t="s">
+        <v>487</v>
+      </c>
+      <c r="C57" t="s">
+        <v>618</v>
+      </c>
+      <c r="D57" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>488</v>
+      </c>
+      <c r="B58" t="s">
+        <v>489</v>
+      </c>
+      <c r="C58" t="s">
+        <v>618</v>
+      </c>
+      <c r="D58" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>490</v>
+      </c>
+      <c r="B59" t="s">
+        <v>491</v>
+      </c>
+      <c r="C59" t="s">
+        <v>630</v>
+      </c>
+      <c r="D59" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>492</v>
+      </c>
+      <c r="B60" t="s">
+        <v>493</v>
+      </c>
+      <c r="C60" t="s">
+        <v>623</v>
+      </c>
+      <c r="D60" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>494</v>
+      </c>
+      <c r="B61" t="s">
+        <v>495</v>
+      </c>
+      <c r="C61" t="s">
+        <v>620</v>
+      </c>
+      <c r="D61" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>496</v>
+      </c>
+      <c r="B62" t="s">
+        <v>497</v>
+      </c>
+      <c r="C62" t="s">
+        <v>620</v>
+      </c>
+      <c r="D62" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>498</v>
+      </c>
+      <c r="B63" t="s">
+        <v>499</v>
+      </c>
+      <c r="C63" t="s">
+        <v>621</v>
+      </c>
+      <c r="D63" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>500</v>
+      </c>
+      <c r="B64" t="s">
+        <v>501</v>
+      </c>
+      <c r="C64" t="s">
+        <v>630</v>
+      </c>
+      <c r="D64" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>502</v>
+      </c>
+      <c r="B65" t="s">
+        <v>503</v>
+      </c>
+      <c r="C65" t="s">
+        <v>624</v>
+      </c>
+      <c r="D65" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>504</v>
+      </c>
+      <c r="B66" t="s">
+        <v>505</v>
+      </c>
+      <c r="C66" t="s">
+        <v>630</v>
+      </c>
+      <c r="D66" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>506</v>
+      </c>
+      <c r="B67" t="s">
+        <v>507</v>
+      </c>
+      <c r="C67" t="s">
+        <v>630</v>
+      </c>
+      <c r="D67" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>508</v>
+      </c>
+      <c r="B68" t="s">
+        <v>509</v>
+      </c>
+      <c r="C68" t="s">
+        <v>618</v>
+      </c>
+      <c r="D68" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>510</v>
+      </c>
+      <c r="B69" t="s">
+        <v>511</v>
+      </c>
+      <c r="C69" t="s">
+        <v>620</v>
+      </c>
+      <c r="D69" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>512</v>
+      </c>
+      <c r="B70" t="s">
+        <v>513</v>
+      </c>
+      <c r="C70" t="s">
+        <v>626</v>
+      </c>
+      <c r="D70" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>514</v>
+      </c>
+      <c r="B71" t="s">
+        <v>515</v>
+      </c>
+      <c r="C71" t="s">
+        <v>630</v>
+      </c>
+      <c r="D71" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>516</v>
+      </c>
+      <c r="B72" t="s">
+        <v>517</v>
+      </c>
+      <c r="C72" t="s">
+        <v>624</v>
+      </c>
+      <c r="D72" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>518</v>
+      </c>
+      <c r="B73" t="s">
+        <v>519</v>
+      </c>
+      <c r="C73" t="s">
+        <v>620</v>
+      </c>
+      <c r="D73" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>520</v>
+      </c>
+      <c r="B74" t="s">
+        <v>521</v>
+      </c>
+      <c r="C74" t="s">
+        <v>629</v>
+      </c>
+      <c r="D74" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>522</v>
+      </c>
+      <c r="B75" t="s">
+        <v>523</v>
+      </c>
+      <c r="C75" t="s">
+        <v>630</v>
+      </c>
+      <c r="D75" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>524</v>
+      </c>
+      <c r="B76" t="s">
+        <v>525</v>
+      </c>
+      <c r="C76" t="s">
+        <v>630</v>
+      </c>
+      <c r="D76" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>526</v>
+      </c>
+      <c r="B77" t="s">
+        <v>527</v>
+      </c>
+      <c r="C77" t="s">
+        <v>628</v>
+      </c>
+      <c r="D77" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>528</v>
+      </c>
+      <c r="B78" t="s">
+        <v>529</v>
+      </c>
+      <c r="C78" t="s">
+        <v>621</v>
+      </c>
+      <c r="D78" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>530</v>
+      </c>
+      <c r="B79" t="s">
+        <v>531</v>
+      </c>
+      <c r="C79" t="s">
+        <v>630</v>
+      </c>
+      <c r="D79" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>532</v>
+      </c>
+      <c r="B80" t="s">
+        <v>533</v>
+      </c>
+      <c r="C80" t="s">
+        <v>620</v>
+      </c>
+      <c r="D80" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>534</v>
+      </c>
+      <c r="B81" t="s">
+        <v>535</v>
+      </c>
+      <c r="C81" t="s">
+        <v>624</v>
+      </c>
+      <c r="D81" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>536</v>
+      </c>
+      <c r="B82" t="s">
+        <v>537</v>
+      </c>
+      <c r="C82" t="s">
+        <v>626</v>
+      </c>
+      <c r="D82" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>538</v>
+      </c>
+      <c r="B83" t="s">
+        <v>539</v>
+      </c>
+      <c r="C83" t="s">
+        <v>621</v>
+      </c>
+      <c r="D83" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>540</v>
+      </c>
+      <c r="B84" t="s">
+        <v>541</v>
+      </c>
+      <c r="C84" t="s">
+        <v>621</v>
+      </c>
+      <c r="D84" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>542</v>
+      </c>
+      <c r="B85" t="s">
+        <v>543</v>
+      </c>
+      <c r="C85" t="s">
+        <v>623</v>
+      </c>
+      <c r="D85" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>544</v>
+      </c>
+      <c r="B86" t="s">
+        <v>545</v>
+      </c>
+      <c r="C86" t="s">
+        <v>624</v>
+      </c>
+      <c r="D86" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>546</v>
+      </c>
+      <c r="B87" t="s">
+        <v>547</v>
+      </c>
+      <c r="C87" t="s">
+        <v>618</v>
+      </c>
+      <c r="D87" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>548</v>
+      </c>
+      <c r="B88" t="s">
+        <v>549</v>
+      </c>
+      <c r="C88" t="s">
+        <v>620</v>
+      </c>
+      <c r="D88" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>550</v>
+      </c>
+      <c r="B89" t="s">
+        <v>551</v>
+      </c>
+      <c r="C89" t="s">
+        <v>627</v>
+      </c>
+      <c r="D89" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>552</v>
+      </c>
+      <c r="B90" t="s">
+        <v>553</v>
+      </c>
+      <c r="C90" t="s">
+        <v>624</v>
+      </c>
+      <c r="D90" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>554</v>
+      </c>
+      <c r="B91" t="s">
+        <v>555</v>
+      </c>
+      <c r="C91" t="s">
+        <v>626</v>
+      </c>
+      <c r="D91" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>556</v>
+      </c>
+      <c r="B92" t="s">
+        <v>557</v>
+      </c>
+      <c r="C92" t="s">
+        <v>618</v>
+      </c>
+      <c r="D92" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>558</v>
+      </c>
+      <c r="B93" t="s">
+        <v>559</v>
+      </c>
+      <c r="C93" t="s">
+        <v>620</v>
+      </c>
+      <c r="D93" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>560</v>
+      </c>
+      <c r="B94" t="s">
+        <v>561</v>
+      </c>
+      <c r="C94" t="s">
+        <v>618</v>
+      </c>
+      <c r="D94" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>562</v>
+      </c>
+      <c r="B95" t="s">
+        <v>563</v>
+      </c>
+      <c r="C95" t="s">
+        <v>620</v>
+      </c>
+      <c r="D95" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>564</v>
+      </c>
+      <c r="B96" t="s">
+        <v>565</v>
+      </c>
+      <c r="C96" t="s">
+        <v>618</v>
+      </c>
+      <c r="D96" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>566</v>
+      </c>
+      <c r="B97" t="s">
+        <v>567</v>
+      </c>
+      <c r="C97" t="s">
+        <v>618</v>
+      </c>
+      <c r="D97" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>568</v>
+      </c>
+      <c r="B98" t="s">
+        <v>569</v>
+      </c>
+      <c r="C98" t="s">
+        <v>618</v>
+      </c>
+      <c r="D98" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>570</v>
+      </c>
+      <c r="B99" t="s">
+        <v>571</v>
+      </c>
+      <c r="C99" t="s">
+        <v>618</v>
+      </c>
+      <c r="D99" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>572</v>
+      </c>
+      <c r="B100" t="s">
+        <v>573</v>
+      </c>
+      <c r="C100" t="s">
+        <v>630</v>
+      </c>
+      <c r="D100" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>574</v>
+      </c>
+      <c r="B101" t="s">
+        <v>575</v>
+      </c>
+      <c r="C101" t="s">
+        <v>618</v>
+      </c>
+      <c r="D101" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>576</v>
+      </c>
+      <c r="B102" t="s">
+        <v>577</v>
+      </c>
+      <c r="C102" t="s">
+        <v>626</v>
+      </c>
+      <c r="D102" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>578</v>
+      </c>
+      <c r="B103" t="s">
+        <v>579</v>
+      </c>
+      <c r="C103" t="s">
+        <v>621</v>
+      </c>
+      <c r="D103" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>580</v>
+      </c>
+      <c r="B104" t="s">
+        <v>581</v>
+      </c>
+      <c r="C104" t="s">
+        <v>630</v>
+      </c>
+      <c r="D104" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>582</v>
+      </c>
+      <c r="B105" t="s">
+        <v>583</v>
+      </c>
+      <c r="C105" t="s">
+        <v>630</v>
+      </c>
+      <c r="D105" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>584</v>
+      </c>
+      <c r="B106" t="s">
+        <v>585</v>
+      </c>
+      <c r="C106" t="s">
+        <v>618</v>
+      </c>
+      <c r="D106" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>586</v>
+      </c>
+      <c r="B107" t="s">
+        <v>587</v>
+      </c>
+      <c r="C107" t="s">
+        <v>627</v>
+      </c>
+      <c r="D107" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>588</v>
+      </c>
+      <c r="B108" t="s">
+        <v>589</v>
+      </c>
+      <c r="C108" t="s">
+        <v>628</v>
+      </c>
+      <c r="D108" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>590</v>
+      </c>
+      <c r="B109" t="s">
+        <v>591</v>
+      </c>
+      <c r="C109" t="s">
+        <v>621</v>
+      </c>
+      <c r="D109" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>592</v>
+      </c>
+      <c r="B110" t="s">
+        <v>593</v>
+      </c>
+      <c r="C110" t="s">
+        <v>620</v>
+      </c>
+      <c r="D110" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>594</v>
+      </c>
+      <c r="B111" t="s">
+        <v>595</v>
+      </c>
+      <c r="C111" t="s">
+        <v>621</v>
+      </c>
+      <c r="D111" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>596</v>
+      </c>
+      <c r="B112" t="s">
+        <v>597</v>
+      </c>
+      <c r="C112" t="s">
+        <v>618</v>
+      </c>
+      <c r="D112" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>598</v>
+      </c>
+      <c r="B113" t="s">
+        <v>599</v>
+      </c>
+      <c r="C113" t="s">
+        <v>627</v>
+      </c>
+      <c r="D113" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>600</v>
+      </c>
+      <c r="B114" t="s">
+        <v>601</v>
+      </c>
+      <c r="C114" t="s">
+        <v>629</v>
+      </c>
+      <c r="D114" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>602</v>
+      </c>
+      <c r="B115" t="s">
+        <v>603</v>
+      </c>
+      <c r="C115" t="s">
+        <v>626</v>
+      </c>
+      <c r="D115" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>604</v>
+      </c>
+      <c r="B116" t="s">
+        <v>605</v>
+      </c>
+      <c r="C116" t="s">
+        <v>623</v>
+      </c>
+      <c r="D116" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>606</v>
+      </c>
+      <c r="B117" t="s">
+        <v>607</v>
+      </c>
+      <c r="C117" t="s">
+        <v>627</v>
+      </c>
+      <c r="D117" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>608</v>
+      </c>
+      <c r="B118" t="s">
+        <v>609</v>
+      </c>
+      <c r="C118" t="s">
+        <v>630</v>
+      </c>
+      <c r="D118" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>610</v>
+      </c>
+      <c r="B119" t="s">
+        <v>611</v>
+      </c>
+      <c r="C119" t="s">
+        <v>630</v>
+      </c>
+      <c r="D119" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>612</v>
+      </c>
+      <c r="B120" t="s">
+        <v>613</v>
+      </c>
+      <c r="C120" t="s">
+        <v>621</v>
+      </c>
+      <c r="D120" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>614</v>
+      </c>
+      <c r="B121" t="s">
+        <v>615</v>
+      </c>
+      <c r="C121" t="s">
+        <v>630</v>
+      </c>
+      <c r="D121" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>616</v>
+      </c>
+      <c r="B122" t="s">
+        <v>617</v>
+      </c>
+      <c r="C122" t="s">
+        <v>618</v>
+      </c>
+      <c r="D122" s="3">
+        <v>45622</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added latest party for party hoppers
A new helping table ensures a politicians who's switched parties is not counted as separate politicians. This approach assumes there are no two persons with the same identical name in a given season (e.g. 2024-E or 2024-F).
</commit_message>
<xml_diff>
--- a/input/mapping_tabeller.xlsx
+++ b/input/mapping_tabeller.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://maerskbroker-my.sharepoint.com/personal/kbo_mbshipbrokers_com/Documents/FTIND/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admkbo\Documents\FTIND\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="447" documentId="8_{6B022C61-D3E3-4D46-8183-99CFA6E77F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6AF65B6F-17D8-468D-A206-CE391679819A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB92151C-D627-4C25-BA1A-A16D848CDCC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{6B009A8E-40F0-41F8-8A22-826EDE827CF8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{6B009A8E-40F0-41F8-8A22-826EDE827CF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Lande" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Partigrupper" sheetId="3" r:id="rId3"/>
     <sheet name="Stopwords" sheetId="4" r:id="rId4"/>
     <sheet name="Emner" sheetId="5" r:id="rId5"/>
+    <sheet name="Partihoppere" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1902" uniqueCount="695">
   <si>
     <t>Albanien</t>
   </si>
@@ -1933,13 +1934,205 @@
   </si>
   <si>
     <t>Generel snak/procedure/debat mellem politiske modstandere</t>
+  </si>
+  <si>
+    <t>År</t>
+  </si>
+  <si>
+    <t>Sæson</t>
+  </si>
+  <si>
+    <t>Navn</t>
+  </si>
+  <si>
+    <t>AntalPartier</t>
+  </si>
+  <si>
+    <t>PartiHopper</t>
+  </si>
+  <si>
+    <t>SenestePartiGruppeKort</t>
+  </si>
+  <si>
+    <t>SenestePartiGruppe</t>
+  </si>
+  <si>
+    <t>Efterår</t>
+  </si>
+  <si>
+    <t>Aleqa Hammond</t>
+  </si>
+  <si>
+    <t>Forår</t>
+  </si>
+  <si>
+    <t>Anders Samuelsen</t>
+  </si>
+  <si>
+    <t>Astrid Krag</t>
+  </si>
+  <si>
+    <t>Bent Bøgsted</t>
+  </si>
+  <si>
+    <t>Britt Bager</t>
+  </si>
+  <si>
+    <t>Christian Friis Bach</t>
+  </si>
+  <si>
+    <t>Christian H. Hansen</t>
+  </si>
+  <si>
+    <t>Dennis Flydtkjær</t>
+  </si>
+  <si>
+    <t>Hans Kristian Skibby</t>
+  </si>
+  <si>
+    <t>Høgni Hoydal</t>
+  </si>
+  <si>
+    <t>Ida Auken</t>
+  </si>
+  <si>
+    <t>Inger Støjberg</t>
+  </si>
+  <si>
+    <t>Jakob Engel-Schmidt</t>
+  </si>
+  <si>
+    <t>Jens Henrik Thulesen Dahl</t>
+  </si>
+  <si>
+    <t>Jens Rohde</t>
+  </si>
+  <si>
+    <t>Jeppe Søe</t>
+  </si>
+  <si>
+    <t>Jesper Petersen</t>
+  </si>
+  <si>
+    <t>Jon Stephensen</t>
+  </si>
+  <si>
+    <t>Jørgen Poulsen</t>
+  </si>
+  <si>
+    <t>Karina Adsbøl</t>
+  </si>
+  <si>
+    <t>Kim Edberg Andersen</t>
+  </si>
+  <si>
+    <t>Lars Boje Mathiesen</t>
+  </si>
+  <si>
+    <t>Lars Løkke Rasmussen</t>
+  </si>
+  <si>
+    <t>Leif Mikkelsen</t>
+  </si>
+  <si>
+    <t>Lise Bech</t>
+  </si>
+  <si>
+    <t>Liselott Blixt</t>
+  </si>
+  <si>
+    <t>Louise Frevert</t>
+  </si>
+  <si>
+    <t>Mads Fuglede</t>
+  </si>
+  <si>
+    <t>Marcus Knuth</t>
+  </si>
+  <si>
+    <t>Marie Krarup</t>
+  </si>
+  <si>
+    <t>Marlene Harpsøe</t>
+  </si>
+  <si>
+    <t>Mette Thiesen</t>
+  </si>
+  <si>
+    <t>Mike Villa Fonseca</t>
+  </si>
+  <si>
+    <t>Morten Messerschmidt</t>
+  </si>
+  <si>
+    <t>Naser Khader</t>
+  </si>
+  <si>
+    <t>Ole Sohn</t>
+  </si>
+  <si>
+    <t>Orla Østerby</t>
+  </si>
+  <si>
+    <t>Per Ørum Jørgensen</t>
+  </si>
+  <si>
+    <t>Pernille Rosenkrantz-Theil</t>
+  </si>
+  <si>
+    <t>Pernille Schnoor</t>
+  </si>
+  <si>
+    <t>Pernille Vermund</t>
+  </si>
+  <si>
+    <t>Peter Seier Christensen</t>
+  </si>
+  <si>
+    <t>Peter Skaarup</t>
+  </si>
+  <si>
+    <t>Pia Christmas-Møller</t>
+  </si>
+  <si>
+    <t>Rasmus Nordqvist</t>
+  </si>
+  <si>
+    <t>Sikandar Siddique</t>
+  </si>
+  <si>
+    <t>Simon Emil Ammitzbøll</t>
+  </si>
+  <si>
+    <t>Simon Emil Ammitzbøll-Bille</t>
+  </si>
+  <si>
+    <t>Sjúrður Skaale</t>
+  </si>
+  <si>
+    <t>Susanne Zimmer</t>
+  </si>
+  <si>
+    <t>Søren Espersen</t>
+  </si>
+  <si>
+    <t>Theresa Scavenius</t>
+  </si>
+  <si>
+    <t>Uffe Elbæk</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Bekræftet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1967,6 +2160,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1976,7 +2176,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1999,11 +2199,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2014,11 +2227,56 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
     <dxf>
       <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2089,20 +2347,39 @@
   <autoFilter ref="A1:B27" xr:uid="{D929CE4D-DE0E-4371-9D74-DAF23F806F68}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{703DE216-50CE-4E57-B997-17634E591F71}" name="Ord"/>
-    <tableColumn id="2" xr3:uid="{A35AE28A-3BB9-4161-A171-35C527B7C143}" name="DatoTilføjet" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{A35AE28A-3BB9-4161-A171-35C527B7C143}" name="DatoTilføjet" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{2C1F5FC9-D397-455C-AEAF-D1763528A602}" name="Emner" displayName="Emner" ref="A1:D122" totalsRowShown="0" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{2C1F5FC9-D397-455C-AEAF-D1763528A602}" name="Emner" displayName="Emner" ref="A1:D122" totalsRowShown="0" dataDxfId="7">
   <autoFilter ref="A1:D122" xr:uid="{2C1F5FC9-D397-455C-AEAF-D1763528A602}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{6F47ADCF-7B5E-431B-8209-B52E2671F6C3}" name="Id" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{625A89F7-2E0B-4AE9-8481-CBE8317B581F}" name="AutomatiskEmne" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{64403E5D-601B-4B88-B55D-4ECF3EA9DC38}" name="EmneGruppe" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{CF0732A2-488A-4A32-B356-40B8CE60F4B8}" name="SidstOpdatret" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{6F47ADCF-7B5E-431B-8209-B52E2671F6C3}" name="Id" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{625A89F7-2E0B-4AE9-8481-CBE8317B581F}" name="AutomatiskEmne" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{64403E5D-601B-4B88-B55D-4ECF3EA9DC38}" name="EmneGruppe" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{CF0732A2-488A-4A32-B356-40B8CE60F4B8}" name="SidstOpdatret" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{74B9B96F-B2B9-4B1F-B795-88782D08D518}" name="Partihoppere" displayName="Partihoppere" ref="A1:J125" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+  <autoFilter ref="A1:J125" xr:uid="{74B9B96F-B2B9-4B1F-B795-88782D08D518}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{89FDB6DF-DC04-4A62-9FBD-A480D176D728}" name="År"/>
+    <tableColumn id="2" xr3:uid="{EB522542-B3BD-40F0-8289-5655B16459AE}" name="Sæson"/>
+    <tableColumn id="3" xr3:uid="{DD683865-656E-456C-A587-7AFD5AB293CB}" name="Navn"/>
+    <tableColumn id="4" xr3:uid="{69D80B71-FDB5-4AA5-982D-3A0D21DC5D89}" name="PartiGruppe"/>
+    <tableColumn id="5" xr3:uid="{6BDDA968-0B25-4E7D-B3EE-CC8488C58BF4}" name="PartiGruppeKort"/>
+    <tableColumn id="6" xr3:uid="{0179A0FF-38D0-4422-820D-DF57338451A3}" name="AntalPartier"/>
+    <tableColumn id="7" xr3:uid="{6A259891-D6DE-49C6-8FAC-BA6E7A3A1363}" name="PartiHopper"/>
+    <tableColumn id="8" xr3:uid="{228D6916-AAE3-40F9-BFC4-75F3B3F5B34C}" name="SenestePartiGruppeKort"/>
+    <tableColumn id="9" xr3:uid="{1F6983D8-24DE-41FF-93E7-C6D5A7FAB00B}" name="SenestePartiGruppe"/>
+    <tableColumn id="10" xr3:uid="{BFA45AB6-6DC4-4C73-B5DD-866E4B2BC0E5}" name="Status"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5227,7 +5504,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F1D6B43-84E6-4039-8D1A-0E6D941491BF}">
   <dimension ref="A1:D122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+    <sheetView topLeftCell="A103" workbookViewId="0">
       <selection activeCell="C122" sqref="C122"/>
     </sheetView>
   </sheetViews>
@@ -6955,4 +7232,4034 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92098685-FF19-46AD-A7A9-F4030AB9C8B1}">
+  <dimension ref="A1:J125"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>631</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>632</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>633</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>634</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>635</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>636</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>637</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2018</v>
+      </c>
+      <c r="B2" t="s">
+        <v>638</v>
+      </c>
+      <c r="C2" t="s">
+        <v>639</v>
+      </c>
+      <c r="D2" t="s">
+        <v>334</v>
+      </c>
+      <c r="E2" t="s">
+        <v>337</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>337</v>
+      </c>
+      <c r="I2" t="s">
+        <v>334</v>
+      </c>
+      <c r="J2" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2017</v>
+      </c>
+      <c r="B3" t="s">
+        <v>638</v>
+      </c>
+      <c r="C3" t="s">
+        <v>639</v>
+      </c>
+      <c r="D3" t="s">
+        <v>320</v>
+      </c>
+      <c r="E3" t="s">
+        <v>298</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>337</v>
+      </c>
+      <c r="I3" t="s">
+        <v>334</v>
+      </c>
+      <c r="J3" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2016</v>
+      </c>
+      <c r="B4" t="s">
+        <v>640</v>
+      </c>
+      <c r="C4" t="s">
+        <v>639</v>
+      </c>
+      <c r="D4" t="s">
+        <v>327</v>
+      </c>
+      <c r="E4" t="s">
+        <v>338</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>337</v>
+      </c>
+      <c r="I4" t="s">
+        <v>334</v>
+      </c>
+      <c r="J4" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2018</v>
+      </c>
+      <c r="B5" t="s">
+        <v>638</v>
+      </c>
+      <c r="C5" t="s">
+        <v>641</v>
+      </c>
+      <c r="D5" t="s">
+        <v>318</v>
+      </c>
+      <c r="E5" t="s">
+        <v>291</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>291</v>
+      </c>
+      <c r="I5" t="s">
+        <v>318</v>
+      </c>
+      <c r="J5" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2008</v>
+      </c>
+      <c r="B6" t="s">
+        <v>640</v>
+      </c>
+      <c r="C6" t="s">
+        <v>641</v>
+      </c>
+      <c r="D6" t="s">
+        <v>331</v>
+      </c>
+      <c r="E6" t="s">
+        <v>342</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>291</v>
+      </c>
+      <c r="I6" t="s">
+        <v>318</v>
+      </c>
+      <c r="J6" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2024</v>
+      </c>
+      <c r="B7" t="s">
+        <v>638</v>
+      </c>
+      <c r="C7" t="s">
+        <v>642</v>
+      </c>
+      <c r="D7" t="s">
+        <v>311</v>
+      </c>
+      <c r="E7" t="s">
+        <v>282</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>282</v>
+      </c>
+      <c r="I7" t="s">
+        <v>311</v>
+      </c>
+      <c r="J7" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2013</v>
+      </c>
+      <c r="B8" t="s">
+        <v>638</v>
+      </c>
+      <c r="C8" t="s">
+        <v>642</v>
+      </c>
+      <c r="D8" t="s">
+        <v>314</v>
+      </c>
+      <c r="E8" t="s">
+        <v>286</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I8" t="s">
+        <v>311</v>
+      </c>
+      <c r="J8" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>2022</v>
+      </c>
+      <c r="B9" t="s">
+        <v>640</v>
+      </c>
+      <c r="C9" t="s">
+        <v>643</v>
+      </c>
+      <c r="D9" t="s">
+        <v>320</v>
+      </c>
+      <c r="E9" t="s">
+        <v>298</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>298</v>
+      </c>
+      <c r="I9" t="s">
+        <v>320</v>
+      </c>
+      <c r="J9" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>2021</v>
+      </c>
+      <c r="B10" t="s">
+        <v>638</v>
+      </c>
+      <c r="C10" t="s">
+        <v>643</v>
+      </c>
+      <c r="D10" t="s">
+        <v>313</v>
+      </c>
+      <c r="E10" t="s">
+        <v>283</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>298</v>
+      </c>
+      <c r="I10" t="s">
+        <v>320</v>
+      </c>
+      <c r="J10" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>2022</v>
+      </c>
+      <c r="B11" t="s">
+        <v>640</v>
+      </c>
+      <c r="C11" t="s">
+        <v>644</v>
+      </c>
+      <c r="D11" t="s">
+        <v>316</v>
+      </c>
+      <c r="E11" t="s">
+        <v>287</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>287</v>
+      </c>
+      <c r="I11" t="s">
+        <v>316</v>
+      </c>
+      <c r="J11" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>2020</v>
+      </c>
+      <c r="B12" t="s">
+        <v>638</v>
+      </c>
+      <c r="C12" t="s">
+        <v>644</v>
+      </c>
+      <c r="D12" t="s">
+        <v>312</v>
+      </c>
+      <c r="E12" t="s">
+        <v>284</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>287</v>
+      </c>
+      <c r="I12" t="s">
+        <v>316</v>
+      </c>
+      <c r="J12" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>2024</v>
+      </c>
+      <c r="B13" t="s">
+        <v>638</v>
+      </c>
+      <c r="C13" t="s">
+        <v>645</v>
+      </c>
+      <c r="D13" t="s">
+        <v>312</v>
+      </c>
+      <c r="E13" t="s">
+        <v>284</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" t="s">
+        <v>284</v>
+      </c>
+      <c r="I13" t="s">
+        <v>312</v>
+      </c>
+      <c r="J13" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>2024</v>
+      </c>
+      <c r="B14" t="s">
+        <v>640</v>
+      </c>
+      <c r="C14" t="s">
+        <v>645</v>
+      </c>
+      <c r="D14" t="s">
+        <v>315</v>
+      </c>
+      <c r="E14" t="s">
+        <v>285</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
+        <v>284</v>
+      </c>
+      <c r="I14" t="s">
+        <v>312</v>
+      </c>
+      <c r="J14" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>2011</v>
+      </c>
+      <c r="B15" t="s">
+        <v>640</v>
+      </c>
+      <c r="C15" t="s">
+        <v>646</v>
+      </c>
+      <c r="D15" t="s">
+        <v>320</v>
+      </c>
+      <c r="E15" t="s">
+        <v>298</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" t="s">
+        <v>298</v>
+      </c>
+      <c r="I15" t="s">
+        <v>320</v>
+      </c>
+      <c r="J15" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>2008</v>
+      </c>
+      <c r="B16" t="s">
+        <v>640</v>
+      </c>
+      <c r="C16" t="s">
+        <v>646</v>
+      </c>
+      <c r="D16" t="s">
+        <v>313</v>
+      </c>
+      <c r="E16" t="s">
+        <v>283</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>298</v>
+      </c>
+      <c r="I16" t="s">
+        <v>320</v>
+      </c>
+      <c r="J16" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>2024</v>
+      </c>
+      <c r="B17" t="s">
+        <v>638</v>
+      </c>
+      <c r="C17" t="s">
+        <v>647</v>
+      </c>
+      <c r="D17" t="s">
+        <v>325</v>
+      </c>
+      <c r="E17" t="s">
+        <v>290</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" t="s">
+        <v>290</v>
+      </c>
+      <c r="I17" t="s">
+        <v>325</v>
+      </c>
+      <c r="J17" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>2022</v>
+      </c>
+      <c r="B18" t="s">
+        <v>640</v>
+      </c>
+      <c r="C18" t="s">
+        <v>647</v>
+      </c>
+      <c r="D18" t="s">
+        <v>313</v>
+      </c>
+      <c r="E18" t="s">
+        <v>283</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
+        <v>290</v>
+      </c>
+      <c r="I18" t="s">
+        <v>325</v>
+      </c>
+      <c r="J18" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>2024</v>
+      </c>
+      <c r="B19" t="s">
+        <v>638</v>
+      </c>
+      <c r="C19" t="s">
+        <v>648</v>
+      </c>
+      <c r="D19" t="s">
+        <v>325</v>
+      </c>
+      <c r="E19" t="s">
+        <v>290</v>
+      </c>
+      <c r="F19">
+        <v>3</v>
+      </c>
+      <c r="G19" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" t="s">
+        <v>290</v>
+      </c>
+      <c r="I19" t="s">
+        <v>325</v>
+      </c>
+      <c r="J19" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>2022</v>
+      </c>
+      <c r="B20" t="s">
+        <v>640</v>
+      </c>
+      <c r="C20" t="s">
+        <v>648</v>
+      </c>
+      <c r="D20" t="s">
+        <v>320</v>
+      </c>
+      <c r="E20" t="s">
+        <v>298</v>
+      </c>
+      <c r="F20">
+        <v>3</v>
+      </c>
+      <c r="G20" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" t="s">
+        <v>290</v>
+      </c>
+      <c r="I20" t="s">
+        <v>325</v>
+      </c>
+      <c r="J20" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>2021</v>
+      </c>
+      <c r="B21" t="s">
+        <v>638</v>
+      </c>
+      <c r="C21" t="s">
+        <v>648</v>
+      </c>
+      <c r="D21" t="s">
+        <v>313</v>
+      </c>
+      <c r="E21" t="s">
+        <v>283</v>
+      </c>
+      <c r="F21">
+        <v>3</v>
+      </c>
+      <c r="G21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H21" t="s">
+        <v>290</v>
+      </c>
+      <c r="I21" t="s">
+        <v>325</v>
+      </c>
+      <c r="J21" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>2016</v>
+      </c>
+      <c r="B22" t="s">
+        <v>638</v>
+      </c>
+      <c r="C22" t="s">
+        <v>649</v>
+      </c>
+      <c r="D22" t="s">
+        <v>333</v>
+      </c>
+      <c r="E22" t="s">
+        <v>336</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="G22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H22" t="s">
+        <v>336</v>
+      </c>
+      <c r="I22" t="s">
+        <v>333</v>
+      </c>
+      <c r="J22" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>2010</v>
+      </c>
+      <c r="B23" t="s">
+        <v>638</v>
+      </c>
+      <c r="C23" t="s">
+        <v>649</v>
+      </c>
+      <c r="D23" t="s">
+        <v>328</v>
+      </c>
+      <c r="E23" t="s">
+        <v>339</v>
+      </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
+      <c r="G23" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23" t="s">
+        <v>336</v>
+      </c>
+      <c r="I23" t="s">
+        <v>333</v>
+      </c>
+      <c r="J23" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>2024</v>
+      </c>
+      <c r="B24" t="s">
+        <v>638</v>
+      </c>
+      <c r="C24" t="s">
+        <v>650</v>
+      </c>
+      <c r="D24" t="s">
+        <v>311</v>
+      </c>
+      <c r="E24" t="s">
+        <v>282</v>
+      </c>
+      <c r="F24">
+        <v>3</v>
+      </c>
+      <c r="G24" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24" t="s">
+        <v>282</v>
+      </c>
+      <c r="I24" t="s">
+        <v>311</v>
+      </c>
+      <c r="J24" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>2019</v>
+      </c>
+      <c r="B25" t="s">
+        <v>638</v>
+      </c>
+      <c r="C25" t="s">
+        <v>650</v>
+      </c>
+      <c r="D25" t="s">
+        <v>315</v>
+      </c>
+      <c r="E25" t="s">
+        <v>285</v>
+      </c>
+      <c r="F25">
+        <v>3</v>
+      </c>
+      <c r="G25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H25" t="s">
+        <v>282</v>
+      </c>
+      <c r="I25" t="s">
+        <v>311</v>
+      </c>
+      <c r="J25" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>2013</v>
+      </c>
+      <c r="B26" t="s">
+        <v>638</v>
+      </c>
+      <c r="C26" t="s">
+        <v>650</v>
+      </c>
+      <c r="D26" t="s">
+        <v>314</v>
+      </c>
+      <c r="E26" t="s">
+        <v>286</v>
+      </c>
+      <c r="F26">
+        <v>3</v>
+      </c>
+      <c r="G26" t="b">
+        <v>1</v>
+      </c>
+      <c r="H26" t="s">
+        <v>282</v>
+      </c>
+      <c r="I26" t="s">
+        <v>311</v>
+      </c>
+      <c r="J26" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>2024</v>
+      </c>
+      <c r="B27" t="s">
+        <v>638</v>
+      </c>
+      <c r="C27" t="s">
+        <v>651</v>
+      </c>
+      <c r="D27" t="s">
+        <v>325</v>
+      </c>
+      <c r="E27" t="s">
+        <v>290</v>
+      </c>
+      <c r="F27">
+        <v>3</v>
+      </c>
+      <c r="G27" t="b">
+        <v>1</v>
+      </c>
+      <c r="H27" t="s">
+        <v>290</v>
+      </c>
+      <c r="I27" t="s">
+        <v>325</v>
+      </c>
+      <c r="J27" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>2021</v>
+      </c>
+      <c r="B28" t="s">
+        <v>638</v>
+      </c>
+      <c r="C28" t="s">
+        <v>651</v>
+      </c>
+      <c r="D28" t="s">
+        <v>320</v>
+      </c>
+      <c r="E28" t="s">
+        <v>298</v>
+      </c>
+      <c r="F28">
+        <v>3</v>
+      </c>
+      <c r="G28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H28" t="s">
+        <v>290</v>
+      </c>
+      <c r="I28" t="s">
+        <v>325</v>
+      </c>
+      <c r="J28" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>2020</v>
+      </c>
+      <c r="B29" t="s">
+        <v>638</v>
+      </c>
+      <c r="C29" t="s">
+        <v>651</v>
+      </c>
+      <c r="D29" t="s">
+        <v>312</v>
+      </c>
+      <c r="E29" t="s">
+        <v>284</v>
+      </c>
+      <c r="F29">
+        <v>3</v>
+      </c>
+      <c r="G29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H29" t="s">
+        <v>290</v>
+      </c>
+      <c r="I29" t="s">
+        <v>325</v>
+      </c>
+      <c r="J29" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>2024</v>
+      </c>
+      <c r="B30" t="s">
+        <v>638</v>
+      </c>
+      <c r="C30" t="s">
+        <v>652</v>
+      </c>
+      <c r="D30" t="s">
+        <v>324</v>
+      </c>
+      <c r="E30" t="s">
+        <v>289</v>
+      </c>
+      <c r="F30">
+        <v>2</v>
+      </c>
+      <c r="G30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H30" t="s">
+        <v>289</v>
+      </c>
+      <c r="I30" t="s">
+        <v>324</v>
+      </c>
+      <c r="J30" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>2017</v>
+      </c>
+      <c r="B31" t="s">
+        <v>640</v>
+      </c>
+      <c r="C31" t="s">
+        <v>652</v>
+      </c>
+      <c r="D31" t="s">
+        <v>312</v>
+      </c>
+      <c r="E31" t="s">
+        <v>284</v>
+      </c>
+      <c r="F31">
+        <v>2</v>
+      </c>
+      <c r="G31" t="b">
+        <v>1</v>
+      </c>
+      <c r="H31" t="s">
+        <v>289</v>
+      </c>
+      <c r="I31" t="s">
+        <v>324</v>
+      </c>
+      <c r="J31" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>2024</v>
+      </c>
+      <c r="B32" t="s">
+        <v>638</v>
+      </c>
+      <c r="C32" t="s">
+        <v>653</v>
+      </c>
+      <c r="D32" t="s">
+        <v>325</v>
+      </c>
+      <c r="E32" t="s">
+        <v>290</v>
+      </c>
+      <c r="F32">
+        <v>2</v>
+      </c>
+      <c r="G32" t="b">
+        <v>1</v>
+      </c>
+      <c r="H32" t="s">
+        <v>290</v>
+      </c>
+      <c r="I32" t="s">
+        <v>325</v>
+      </c>
+      <c r="J32" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>2022</v>
+      </c>
+      <c r="B33" t="s">
+        <v>640</v>
+      </c>
+      <c r="C33" t="s">
+        <v>653</v>
+      </c>
+      <c r="D33" t="s">
+        <v>313</v>
+      </c>
+      <c r="E33" t="s">
+        <v>283</v>
+      </c>
+      <c r="F33">
+        <v>2</v>
+      </c>
+      <c r="G33" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" t="s">
+        <v>290</v>
+      </c>
+      <c r="I33" t="s">
+        <v>325</v>
+      </c>
+      <c r="J33" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>2022</v>
+      </c>
+      <c r="B34" t="s">
+        <v>640</v>
+      </c>
+      <c r="C34" t="s">
+        <v>654</v>
+      </c>
+      <c r="D34" t="s">
+        <v>319</v>
+      </c>
+      <c r="E34" t="s">
+        <v>301</v>
+      </c>
+      <c r="F34">
+        <v>3</v>
+      </c>
+      <c r="G34" t="b">
+        <v>1</v>
+      </c>
+      <c r="H34" t="s">
+        <v>301</v>
+      </c>
+      <c r="I34" t="s">
+        <v>319</v>
+      </c>
+      <c r="J34" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>2020</v>
+      </c>
+      <c r="B35" t="s">
+        <v>638</v>
+      </c>
+      <c r="C35" t="s">
+        <v>654</v>
+      </c>
+      <c r="D35" t="s">
+        <v>315</v>
+      </c>
+      <c r="E35" t="s">
+        <v>285</v>
+      </c>
+      <c r="F35">
+        <v>3</v>
+      </c>
+      <c r="G35" t="b">
+        <v>1</v>
+      </c>
+      <c r="H35" t="s">
+        <v>301</v>
+      </c>
+      <c r="I35" t="s">
+        <v>319</v>
+      </c>
+      <c r="J35" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>2006</v>
+      </c>
+      <c r="B36" t="s">
+        <v>638</v>
+      </c>
+      <c r="C36" t="s">
+        <v>654</v>
+      </c>
+      <c r="D36" t="s">
+        <v>312</v>
+      </c>
+      <c r="E36" t="s">
+        <v>284</v>
+      </c>
+      <c r="F36">
+        <v>3</v>
+      </c>
+      <c r="G36" t="b">
+        <v>1</v>
+      </c>
+      <c r="H36" t="s">
+        <v>301</v>
+      </c>
+      <c r="I36" t="s">
+        <v>319</v>
+      </c>
+      <c r="J36" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>2024</v>
+      </c>
+      <c r="B37" t="s">
+        <v>638</v>
+      </c>
+      <c r="C37" t="s">
+        <v>655</v>
+      </c>
+      <c r="D37" t="s">
+        <v>320</v>
+      </c>
+      <c r="E37" t="s">
+        <v>298</v>
+      </c>
+      <c r="F37">
+        <v>2</v>
+      </c>
+      <c r="G37" t="b">
+        <v>1</v>
+      </c>
+      <c r="H37" t="s">
+        <v>298</v>
+      </c>
+      <c r="I37" t="s">
+        <v>320</v>
+      </c>
+      <c r="J37" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>2024</v>
+      </c>
+      <c r="B38" t="s">
+        <v>640</v>
+      </c>
+      <c r="C38" t="s">
+        <v>655</v>
+      </c>
+      <c r="D38" t="s">
+        <v>324</v>
+      </c>
+      <c r="E38" t="s">
+        <v>289</v>
+      </c>
+      <c r="F38">
+        <v>2</v>
+      </c>
+      <c r="G38" t="b">
+        <v>1</v>
+      </c>
+      <c r="H38" t="s">
+        <v>298</v>
+      </c>
+      <c r="I38" t="s">
+        <v>320</v>
+      </c>
+      <c r="J38" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>2024</v>
+      </c>
+      <c r="B39" t="s">
+        <v>638</v>
+      </c>
+      <c r="C39" t="s">
+        <v>656</v>
+      </c>
+      <c r="D39" t="s">
+        <v>311</v>
+      </c>
+      <c r="E39" t="s">
+        <v>282</v>
+      </c>
+      <c r="F39">
+        <v>2</v>
+      </c>
+      <c r="G39" t="b">
+        <v>1</v>
+      </c>
+      <c r="H39" t="s">
+        <v>282</v>
+      </c>
+      <c r="I39" t="s">
+        <v>311</v>
+      </c>
+      <c r="J39" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>2012</v>
+      </c>
+      <c r="B40" t="s">
+        <v>638</v>
+      </c>
+      <c r="C40" t="s">
+        <v>656</v>
+      </c>
+      <c r="D40" t="s">
+        <v>314</v>
+      </c>
+      <c r="E40" t="s">
+        <v>286</v>
+      </c>
+      <c r="F40">
+        <v>2</v>
+      </c>
+      <c r="G40" t="b">
+        <v>1</v>
+      </c>
+      <c r="H40" t="s">
+        <v>282</v>
+      </c>
+      <c r="I40" t="s">
+        <v>311</v>
+      </c>
+      <c r="J40" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>2024</v>
+      </c>
+      <c r="B41" t="s">
+        <v>638</v>
+      </c>
+      <c r="C41" t="s">
+        <v>657</v>
+      </c>
+      <c r="D41" t="s">
+        <v>320</v>
+      </c>
+      <c r="E41" t="s">
+        <v>298</v>
+      </c>
+      <c r="F41">
+        <v>2</v>
+      </c>
+      <c r="G41" t="b">
+        <v>1</v>
+      </c>
+      <c r="H41" t="s">
+        <v>298</v>
+      </c>
+      <c r="I41" t="s">
+        <v>320</v>
+      </c>
+      <c r="J41" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>2022</v>
+      </c>
+      <c r="B42" t="s">
+        <v>638</v>
+      </c>
+      <c r="C42" t="s">
+        <v>657</v>
+      </c>
+      <c r="D42" t="s">
+        <v>324</v>
+      </c>
+      <c r="E42" t="s">
+        <v>289</v>
+      </c>
+      <c r="F42">
+        <v>2</v>
+      </c>
+      <c r="G42" t="b">
+        <v>1</v>
+      </c>
+      <c r="H42" t="s">
+        <v>298</v>
+      </c>
+      <c r="I42" t="s">
+        <v>320</v>
+      </c>
+      <c r="J42" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>2011</v>
+      </c>
+      <c r="B43" t="s">
+        <v>640</v>
+      </c>
+      <c r="C43" t="s">
+        <v>658</v>
+      </c>
+      <c r="D43" t="s">
+        <v>315</v>
+      </c>
+      <c r="E43" t="s">
+        <v>285</v>
+      </c>
+      <c r="F43">
+        <v>2</v>
+      </c>
+      <c r="G43" t="b">
+        <v>1</v>
+      </c>
+      <c r="H43" t="s">
+        <v>285</v>
+      </c>
+      <c r="I43" t="s">
+        <v>315</v>
+      </c>
+      <c r="J43" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>2008</v>
+      </c>
+      <c r="B44" t="s">
+        <v>640</v>
+      </c>
+      <c r="C44" t="s">
+        <v>658</v>
+      </c>
+      <c r="D44" t="s">
+        <v>331</v>
+      </c>
+      <c r="E44" t="s">
+        <v>342</v>
+      </c>
+      <c r="F44">
+        <v>2</v>
+      </c>
+      <c r="G44" t="b">
+        <v>1</v>
+      </c>
+      <c r="H44" t="s">
+        <v>285</v>
+      </c>
+      <c r="I44" t="s">
+        <v>315</v>
+      </c>
+      <c r="J44" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>2024</v>
+      </c>
+      <c r="B45" t="s">
+        <v>638</v>
+      </c>
+      <c r="C45" t="s">
+        <v>659</v>
+      </c>
+      <c r="D45" t="s">
+        <v>325</v>
+      </c>
+      <c r="E45" t="s">
+        <v>290</v>
+      </c>
+      <c r="F45">
+        <v>3</v>
+      </c>
+      <c r="G45" t="b">
+        <v>1</v>
+      </c>
+      <c r="H45" t="s">
+        <v>290</v>
+      </c>
+      <c r="I45" t="s">
+        <v>325</v>
+      </c>
+      <c r="J45" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>2022</v>
+      </c>
+      <c r="B46" t="s">
+        <v>640</v>
+      </c>
+      <c r="C46" t="s">
+        <v>659</v>
+      </c>
+      <c r="D46" t="s">
+        <v>320</v>
+      </c>
+      <c r="E46" t="s">
+        <v>298</v>
+      </c>
+      <c r="F46">
+        <v>3</v>
+      </c>
+      <c r="G46" t="b">
+        <v>1</v>
+      </c>
+      <c r="H46" t="s">
+        <v>290</v>
+      </c>
+      <c r="I46" t="s">
+        <v>325</v>
+      </c>
+      <c r="J46" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>2021</v>
+      </c>
+      <c r="B47" t="s">
+        <v>638</v>
+      </c>
+      <c r="C47" t="s">
+        <v>659</v>
+      </c>
+      <c r="D47" t="s">
+        <v>313</v>
+      </c>
+      <c r="E47" t="s">
+        <v>283</v>
+      </c>
+      <c r="F47">
+        <v>3</v>
+      </c>
+      <c r="G47" t="b">
+        <v>1</v>
+      </c>
+      <c r="H47" t="s">
+        <v>290</v>
+      </c>
+      <c r="I47" t="s">
+        <v>325</v>
+      </c>
+      <c r="J47" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>2024</v>
+      </c>
+      <c r="B48" t="s">
+        <v>638</v>
+      </c>
+      <c r="C48" t="s">
+        <v>660</v>
+      </c>
+      <c r="D48" t="s">
+        <v>325</v>
+      </c>
+      <c r="E48" t="s">
+        <v>290</v>
+      </c>
+      <c r="F48">
+        <v>2</v>
+      </c>
+      <c r="G48" t="b">
+        <v>1</v>
+      </c>
+      <c r="H48" t="s">
+        <v>290</v>
+      </c>
+      <c r="I48" t="s">
+        <v>325</v>
+      </c>
+      <c r="J48" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>2023</v>
+      </c>
+      <c r="B49" t="s">
+        <v>638</v>
+      </c>
+      <c r="C49" t="s">
+        <v>660</v>
+      </c>
+      <c r="D49" t="s">
+        <v>322</v>
+      </c>
+      <c r="E49" t="s">
+        <v>294</v>
+      </c>
+      <c r="F49">
+        <v>2</v>
+      </c>
+      <c r="G49" t="b">
+        <v>1</v>
+      </c>
+      <c r="H49" t="s">
+        <v>290</v>
+      </c>
+      <c r="I49" t="s">
+        <v>325</v>
+      </c>
+      <c r="J49" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>2024</v>
+      </c>
+      <c r="B50" t="s">
+        <v>638</v>
+      </c>
+      <c r="C50" t="s">
+        <v>661</v>
+      </c>
+      <c r="D50" t="s">
+        <v>320</v>
+      </c>
+      <c r="E50" t="s">
+        <v>298</v>
+      </c>
+      <c r="F50">
+        <v>2</v>
+      </c>
+      <c r="G50" t="b">
+        <v>1</v>
+      </c>
+      <c r="H50" t="s">
+        <v>298</v>
+      </c>
+      <c r="I50" t="s">
+        <v>320</v>
+      </c>
+      <c r="J50" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>2022</v>
+      </c>
+      <c r="B51" t="s">
+        <v>640</v>
+      </c>
+      <c r="C51" t="s">
+        <v>661</v>
+      </c>
+      <c r="D51" t="s">
+        <v>322</v>
+      </c>
+      <c r="E51" t="s">
+        <v>294</v>
+      </c>
+      <c r="F51">
+        <v>2</v>
+      </c>
+      <c r="G51" t="b">
+        <v>1</v>
+      </c>
+      <c r="H51" t="s">
+        <v>298</v>
+      </c>
+      <c r="I51" t="s">
+        <v>320</v>
+      </c>
+      <c r="J51" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>2024</v>
+      </c>
+      <c r="B52" t="s">
+        <v>638</v>
+      </c>
+      <c r="C52" t="s">
+        <v>662</v>
+      </c>
+      <c r="D52" t="s">
+        <v>324</v>
+      </c>
+      <c r="E52" t="s">
+        <v>289</v>
+      </c>
+      <c r="F52">
+        <v>3</v>
+      </c>
+      <c r="G52" t="b">
+        <v>1</v>
+      </c>
+      <c r="H52" t="s">
+        <v>289</v>
+      </c>
+      <c r="I52" t="s">
+        <v>324</v>
+      </c>
+      <c r="J52" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>2021</v>
+      </c>
+      <c r="B53" t="s">
+        <v>638</v>
+      </c>
+      <c r="C53" t="s">
+        <v>662</v>
+      </c>
+      <c r="D53" t="s">
+        <v>320</v>
+      </c>
+      <c r="E53" t="s">
+        <v>298</v>
+      </c>
+      <c r="F53">
+        <v>3</v>
+      </c>
+      <c r="G53" t="b">
+        <v>1</v>
+      </c>
+      <c r="H53" t="s">
+        <v>289</v>
+      </c>
+      <c r="I53" t="s">
+        <v>324</v>
+      </c>
+      <c r="J53" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>2020</v>
+      </c>
+      <c r="B54" t="s">
+        <v>638</v>
+      </c>
+      <c r="C54" t="s">
+        <v>662</v>
+      </c>
+      <c r="D54" t="s">
+        <v>312</v>
+      </c>
+      <c r="E54" t="s">
+        <v>284</v>
+      </c>
+      <c r="F54">
+        <v>3</v>
+      </c>
+      <c r="G54" t="b">
+        <v>1</v>
+      </c>
+      <c r="H54" t="s">
+        <v>289</v>
+      </c>
+      <c r="I54" t="s">
+        <v>324</v>
+      </c>
+      <c r="J54" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>2018</v>
+      </c>
+      <c r="B55" t="s">
+        <v>638</v>
+      </c>
+      <c r="C55" t="s">
+        <v>663</v>
+      </c>
+      <c r="D55" t="s">
+        <v>318</v>
+      </c>
+      <c r="E55" t="s">
+        <v>291</v>
+      </c>
+      <c r="F55">
+        <v>3</v>
+      </c>
+      <c r="G55" t="b">
+        <v>1</v>
+      </c>
+      <c r="H55" t="s">
+        <v>291</v>
+      </c>
+      <c r="I55" t="s">
+        <v>318</v>
+      </c>
+      <c r="J55" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>2007</v>
+      </c>
+      <c r="B56" t="s">
+        <v>640</v>
+      </c>
+      <c r="C56" t="s">
+        <v>663</v>
+      </c>
+      <c r="D56" t="s">
+        <v>320</v>
+      </c>
+      <c r="E56" t="s">
+        <v>298</v>
+      </c>
+      <c r="F56">
+        <v>3</v>
+      </c>
+      <c r="G56" t="b">
+        <v>1</v>
+      </c>
+      <c r="H56" t="s">
+        <v>291</v>
+      </c>
+      <c r="I56" t="s">
+        <v>318</v>
+      </c>
+      <c r="J56" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>2006</v>
+      </c>
+      <c r="B57" t="s">
+        <v>638</v>
+      </c>
+      <c r="C57" t="s">
+        <v>663</v>
+      </c>
+      <c r="D57" t="s">
+        <v>312</v>
+      </c>
+      <c r="E57" t="s">
+        <v>284</v>
+      </c>
+      <c r="F57">
+        <v>3</v>
+      </c>
+      <c r="G57" t="b">
+        <v>1</v>
+      </c>
+      <c r="H57" t="s">
+        <v>291</v>
+      </c>
+      <c r="I57" t="s">
+        <v>318</v>
+      </c>
+      <c r="J57" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>2024</v>
+      </c>
+      <c r="B58" t="s">
+        <v>638</v>
+      </c>
+      <c r="C58" t="s">
+        <v>664</v>
+      </c>
+      <c r="D58" t="s">
+        <v>325</v>
+      </c>
+      <c r="E58" t="s">
+        <v>290</v>
+      </c>
+      <c r="F58">
+        <v>3</v>
+      </c>
+      <c r="G58" t="b">
+        <v>1</v>
+      </c>
+      <c r="H58" t="s">
+        <v>290</v>
+      </c>
+      <c r="I58" t="s">
+        <v>325</v>
+      </c>
+      <c r="J58" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>2022</v>
+      </c>
+      <c r="B59" t="s">
+        <v>640</v>
+      </c>
+      <c r="C59" t="s">
+        <v>664</v>
+      </c>
+      <c r="D59" t="s">
+        <v>320</v>
+      </c>
+      <c r="E59" t="s">
+        <v>298</v>
+      </c>
+      <c r="F59">
+        <v>3</v>
+      </c>
+      <c r="G59" t="b">
+        <v>1</v>
+      </c>
+      <c r="H59" t="s">
+        <v>290</v>
+      </c>
+      <c r="I59" t="s">
+        <v>325</v>
+      </c>
+      <c r="J59" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>2021</v>
+      </c>
+      <c r="B60" t="s">
+        <v>638</v>
+      </c>
+      <c r="C60" t="s">
+        <v>664</v>
+      </c>
+      <c r="D60" t="s">
+        <v>313</v>
+      </c>
+      <c r="E60" t="s">
+        <v>283</v>
+      </c>
+      <c r="F60">
+        <v>3</v>
+      </c>
+      <c r="G60" t="b">
+        <v>1</v>
+      </c>
+      <c r="H60" t="s">
+        <v>290</v>
+      </c>
+      <c r="I60" t="s">
+        <v>325</v>
+      </c>
+      <c r="J60" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>2022</v>
+      </c>
+      <c r="B61" t="s">
+        <v>640</v>
+      </c>
+      <c r="C61" t="s">
+        <v>665</v>
+      </c>
+      <c r="D61" t="s">
+        <v>320</v>
+      </c>
+      <c r="E61" t="s">
+        <v>298</v>
+      </c>
+      <c r="F61">
+        <v>2</v>
+      </c>
+      <c r="G61" t="b">
+        <v>1</v>
+      </c>
+      <c r="H61" t="s">
+        <v>298</v>
+      </c>
+      <c r="I61" t="s">
+        <v>320</v>
+      </c>
+      <c r="J61" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>2021</v>
+      </c>
+      <c r="B62" t="s">
+        <v>638</v>
+      </c>
+      <c r="C62" t="s">
+        <v>665</v>
+      </c>
+      <c r="D62" t="s">
+        <v>313</v>
+      </c>
+      <c r="E62" t="s">
+        <v>283</v>
+      </c>
+      <c r="F62">
+        <v>2</v>
+      </c>
+      <c r="G62" t="b">
+        <v>1</v>
+      </c>
+      <c r="H62" t="s">
+        <v>298</v>
+      </c>
+      <c r="I62" t="s">
+        <v>320</v>
+      </c>
+      <c r="J62" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>2007</v>
+      </c>
+      <c r="B63" t="s">
+        <v>640</v>
+      </c>
+      <c r="C63" t="s">
+        <v>666</v>
+      </c>
+      <c r="D63" t="s">
+        <v>320</v>
+      </c>
+      <c r="E63" t="s">
+        <v>298</v>
+      </c>
+      <c r="F63">
+        <v>2</v>
+      </c>
+      <c r="G63" t="b">
+        <v>1</v>
+      </c>
+      <c r="H63" t="s">
+        <v>298</v>
+      </c>
+      <c r="I63" t="s">
+        <v>320</v>
+      </c>
+      <c r="J63" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>2006</v>
+      </c>
+      <c r="B64" t="s">
+        <v>638</v>
+      </c>
+      <c r="C64" t="s">
+        <v>666</v>
+      </c>
+      <c r="D64" t="s">
+        <v>313</v>
+      </c>
+      <c r="E64" t="s">
+        <v>283</v>
+      </c>
+      <c r="F64">
+        <v>2</v>
+      </c>
+      <c r="G64" t="b">
+        <v>1</v>
+      </c>
+      <c r="H64" t="s">
+        <v>298</v>
+      </c>
+      <c r="I64" t="s">
+        <v>320</v>
+      </c>
+      <c r="J64" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>2024</v>
+      </c>
+      <c r="B65" t="s">
+        <v>640</v>
+      </c>
+      <c r="C65" t="s">
+        <v>667</v>
+      </c>
+      <c r="D65" t="s">
+        <v>325</v>
+      </c>
+      <c r="E65" t="s">
+        <v>290</v>
+      </c>
+      <c r="F65">
+        <v>2</v>
+      </c>
+      <c r="G65" t="b">
+        <v>1</v>
+      </c>
+      <c r="H65" t="s">
+        <v>290</v>
+      </c>
+      <c r="I65" t="s">
+        <v>325</v>
+      </c>
+      <c r="J65" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>2023</v>
+      </c>
+      <c r="B66" t="s">
+        <v>638</v>
+      </c>
+      <c r="C66" t="s">
+        <v>667</v>
+      </c>
+      <c r="D66" t="s">
+        <v>312</v>
+      </c>
+      <c r="E66" t="s">
+        <v>284</v>
+      </c>
+      <c r="F66">
+        <v>2</v>
+      </c>
+      <c r="G66" t="b">
+        <v>1</v>
+      </c>
+      <c r="H66" t="s">
+        <v>290</v>
+      </c>
+      <c r="I66" t="s">
+        <v>325</v>
+      </c>
+      <c r="J66" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>2022</v>
+      </c>
+      <c r="B67" t="s">
+        <v>640</v>
+      </c>
+      <c r="C67" t="s">
+        <v>668</v>
+      </c>
+      <c r="D67" t="s">
+        <v>316</v>
+      </c>
+      <c r="E67" t="s">
+        <v>287</v>
+      </c>
+      <c r="F67">
+        <v>2</v>
+      </c>
+      <c r="G67" t="b">
+        <v>1</v>
+      </c>
+      <c r="H67" t="s">
+        <v>287</v>
+      </c>
+      <c r="I67" t="s">
+        <v>316</v>
+      </c>
+      <c r="J67" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>2018</v>
+      </c>
+      <c r="B68" t="s">
+        <v>638</v>
+      </c>
+      <c r="C68" t="s">
+        <v>668</v>
+      </c>
+      <c r="D68" t="s">
+        <v>312</v>
+      </c>
+      <c r="E68" t="s">
+        <v>284</v>
+      </c>
+      <c r="F68">
+        <v>2</v>
+      </c>
+      <c r="G68" t="b">
+        <v>1</v>
+      </c>
+      <c r="H68" t="s">
+        <v>287</v>
+      </c>
+      <c r="I68" t="s">
+        <v>316</v>
+      </c>
+      <c r="J68" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>2022</v>
+      </c>
+      <c r="B69" t="s">
+        <v>640</v>
+      </c>
+      <c r="C69" t="s">
+        <v>669</v>
+      </c>
+      <c r="D69" t="s">
+        <v>320</v>
+      </c>
+      <c r="E69" t="s">
+        <v>298</v>
+      </c>
+      <c r="F69">
+        <v>2</v>
+      </c>
+      <c r="G69" t="b">
+        <v>1</v>
+      </c>
+      <c r="H69" t="s">
+        <v>298</v>
+      </c>
+      <c r="I69" t="s">
+        <v>320</v>
+      </c>
+      <c r="J69" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>2021</v>
+      </c>
+      <c r="B70" t="s">
+        <v>638</v>
+      </c>
+      <c r="C70" t="s">
+        <v>669</v>
+      </c>
+      <c r="D70" t="s">
+        <v>313</v>
+      </c>
+      <c r="E70" t="s">
+        <v>283</v>
+      </c>
+      <c r="F70">
+        <v>2</v>
+      </c>
+      <c r="G70" t="b">
+        <v>1</v>
+      </c>
+      <c r="H70" t="s">
+        <v>298</v>
+      </c>
+      <c r="I70" t="s">
+        <v>320</v>
+      </c>
+      <c r="J70" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>2024</v>
+      </c>
+      <c r="B71" t="s">
+        <v>638</v>
+      </c>
+      <c r="C71" t="s">
+        <v>670</v>
+      </c>
+      <c r="D71" t="s">
+        <v>325</v>
+      </c>
+      <c r="E71" t="s">
+        <v>290</v>
+      </c>
+      <c r="F71">
+        <v>2</v>
+      </c>
+      <c r="G71" t="b">
+        <v>1</v>
+      </c>
+      <c r="H71" t="s">
+        <v>290</v>
+      </c>
+      <c r="I71" t="s">
+        <v>325</v>
+      </c>
+      <c r="J71" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>2018</v>
+      </c>
+      <c r="B72" t="s">
+        <v>638</v>
+      </c>
+      <c r="C72" t="s">
+        <v>670</v>
+      </c>
+      <c r="D72" t="s">
+        <v>313</v>
+      </c>
+      <c r="E72" t="s">
+        <v>283</v>
+      </c>
+      <c r="F72">
+        <v>2</v>
+      </c>
+      <c r="G72" t="b">
+        <v>1</v>
+      </c>
+      <c r="H72" t="s">
+        <v>290</v>
+      </c>
+      <c r="I72" t="s">
+        <v>325</v>
+      </c>
+      <c r="J72" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>2024</v>
+      </c>
+      <c r="B73" t="s">
+        <v>638</v>
+      </c>
+      <c r="C73" t="s">
+        <v>671</v>
+      </c>
+      <c r="D73" t="s">
+        <v>313</v>
+      </c>
+      <c r="E73" t="s">
+        <v>283</v>
+      </c>
+      <c r="F73">
+        <v>2</v>
+      </c>
+      <c r="G73" t="b">
+        <v>1</v>
+      </c>
+      <c r="H73" t="s">
+        <v>283</v>
+      </c>
+      <c r="I73" t="s">
+        <v>313</v>
+      </c>
+      <c r="J73" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>2022</v>
+      </c>
+      <c r="B74" t="s">
+        <v>640</v>
+      </c>
+      <c r="C74" t="s">
+        <v>671</v>
+      </c>
+      <c r="D74" t="s">
+        <v>322</v>
+      </c>
+      <c r="E74" t="s">
+        <v>294</v>
+      </c>
+      <c r="F74">
+        <v>2</v>
+      </c>
+      <c r="G74" t="b">
+        <v>1</v>
+      </c>
+      <c r="H74" t="s">
+        <v>283</v>
+      </c>
+      <c r="I74" t="s">
+        <v>313</v>
+      </c>
+      <c r="J74" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>2024</v>
+      </c>
+      <c r="B75" t="s">
+        <v>638</v>
+      </c>
+      <c r="C75" t="s">
+        <v>672</v>
+      </c>
+      <c r="D75" t="s">
+        <v>320</v>
+      </c>
+      <c r="E75" t="s">
+        <v>298</v>
+      </c>
+      <c r="F75">
+        <v>2</v>
+      </c>
+      <c r="G75" t="b">
+        <v>1</v>
+      </c>
+      <c r="H75" t="s">
+        <v>298</v>
+      </c>
+      <c r="I75" t="s">
+        <v>320</v>
+      </c>
+      <c r="J75" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>2023</v>
+      </c>
+      <c r="B76" t="s">
+        <v>640</v>
+      </c>
+      <c r="C76" t="s">
+        <v>672</v>
+      </c>
+      <c r="D76" t="s">
+        <v>324</v>
+      </c>
+      <c r="E76" t="s">
+        <v>289</v>
+      </c>
+      <c r="F76">
+        <v>2</v>
+      </c>
+      <c r="G76" t="b">
+        <v>1</v>
+      </c>
+      <c r="H76" t="s">
+        <v>298</v>
+      </c>
+      <c r="I76" t="s">
+        <v>320</v>
+      </c>
+      <c r="J76" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>2024</v>
+      </c>
+      <c r="B77" t="s">
+        <v>638</v>
+      </c>
+      <c r="C77" t="s">
+        <v>673</v>
+      </c>
+      <c r="D77" t="s">
+        <v>313</v>
+      </c>
+      <c r="E77" t="s">
+        <v>283</v>
+      </c>
+      <c r="F77">
+        <v>2</v>
+      </c>
+      <c r="G77" t="b">
+        <v>1</v>
+      </c>
+      <c r="H77" t="s">
+        <v>283</v>
+      </c>
+      <c r="I77" t="s">
+        <v>313</v>
+      </c>
+      <c r="J77" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>2007</v>
+      </c>
+      <c r="B78" t="s">
+        <v>640</v>
+      </c>
+      <c r="C78" t="s">
+        <v>673</v>
+      </c>
+      <c r="D78" t="s">
+        <v>320</v>
+      </c>
+      <c r="E78" t="s">
+        <v>298</v>
+      </c>
+      <c r="F78">
+        <v>2</v>
+      </c>
+      <c r="G78" t="b">
+        <v>1</v>
+      </c>
+      <c r="H78" t="s">
+        <v>283</v>
+      </c>
+      <c r="I78" t="s">
+        <v>313</v>
+      </c>
+      <c r="J78" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>2022</v>
+      </c>
+      <c r="B79" t="s">
+        <v>640</v>
+      </c>
+      <c r="C79" t="s">
+        <v>674</v>
+      </c>
+      <c r="D79" t="s">
+        <v>320</v>
+      </c>
+      <c r="E79" t="s">
+        <v>298</v>
+      </c>
+      <c r="F79">
+        <v>5</v>
+      </c>
+      <c r="G79" t="b">
+        <v>1</v>
+      </c>
+      <c r="H79" t="s">
+        <v>298</v>
+      </c>
+      <c r="I79" t="s">
+        <v>320</v>
+      </c>
+      <c r="J79" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>2020</v>
+      </c>
+      <c r="B80" t="s">
+        <v>638</v>
+      </c>
+      <c r="C80" t="s">
+        <v>674</v>
+      </c>
+      <c r="D80" t="s">
+        <v>316</v>
+      </c>
+      <c r="E80" t="s">
+        <v>287</v>
+      </c>
+      <c r="F80">
+        <v>5</v>
+      </c>
+      <c r="G80" t="b">
+        <v>1</v>
+      </c>
+      <c r="H80" t="s">
+        <v>298</v>
+      </c>
+      <c r="I80" t="s">
+        <v>320</v>
+      </c>
+      <c r="J80" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>2008</v>
+      </c>
+      <c r="B81" t="s">
+        <v>638</v>
+      </c>
+      <c r="C81" t="s">
+        <v>674</v>
+      </c>
+      <c r="D81" t="s">
+        <v>318</v>
+      </c>
+      <c r="E81" t="s">
+        <v>291</v>
+      </c>
+      <c r="F81">
+        <v>5</v>
+      </c>
+      <c r="G81" t="b">
+        <v>1</v>
+      </c>
+      <c r="H81" t="s">
+        <v>298</v>
+      </c>
+      <c r="I81" t="s">
+        <v>320</v>
+      </c>
+      <c r="J81" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>2008</v>
+      </c>
+      <c r="B82" t="s">
+        <v>640</v>
+      </c>
+      <c r="C82" t="s">
+        <v>674</v>
+      </c>
+      <c r="D82" t="s">
+        <v>331</v>
+      </c>
+      <c r="E82" t="s">
+        <v>342</v>
+      </c>
+      <c r="F82">
+        <v>5</v>
+      </c>
+      <c r="G82" t="b">
+        <v>1</v>
+      </c>
+      <c r="H82" t="s">
+        <v>298</v>
+      </c>
+      <c r="I82" t="s">
+        <v>320</v>
+      </c>
+      <c r="J82" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>2006</v>
+      </c>
+      <c r="B83" t="s">
+        <v>638</v>
+      </c>
+      <c r="C83" t="s">
+        <v>674</v>
+      </c>
+      <c r="D83" t="s">
+        <v>315</v>
+      </c>
+      <c r="E83" t="s">
+        <v>285</v>
+      </c>
+      <c r="F83">
+        <v>5</v>
+      </c>
+      <c r="G83" t="b">
+        <v>1</v>
+      </c>
+      <c r="H83" t="s">
+        <v>298</v>
+      </c>
+      <c r="I83" t="s">
+        <v>320</v>
+      </c>
+      <c r="J83" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>2014</v>
+      </c>
+      <c r="B84" t="s">
+        <v>638</v>
+      </c>
+      <c r="C84" t="s">
+        <v>675</v>
+      </c>
+      <c r="D84" t="s">
+        <v>311</v>
+      </c>
+      <c r="E84" t="s">
+        <v>282</v>
+      </c>
+      <c r="F84">
+        <v>2</v>
+      </c>
+      <c r="G84" t="b">
+        <v>1</v>
+      </c>
+      <c r="H84" t="s">
+        <v>282</v>
+      </c>
+      <c r="I84" t="s">
+        <v>311</v>
+      </c>
+      <c r="J84" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>2013</v>
+      </c>
+      <c r="B85" t="s">
+        <v>638</v>
+      </c>
+      <c r="C85" t="s">
+        <v>675</v>
+      </c>
+      <c r="D85" t="s">
+        <v>314</v>
+      </c>
+      <c r="E85" t="s">
+        <v>286</v>
+      </c>
+      <c r="F85">
+        <v>2</v>
+      </c>
+      <c r="G85" t="b">
+        <v>1</v>
+      </c>
+      <c r="H85" t="s">
+        <v>282</v>
+      </c>
+      <c r="I85" t="s">
+        <v>311</v>
+      </c>
+      <c r="J85" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>2022</v>
+      </c>
+      <c r="B86" t="s">
+        <v>640</v>
+      </c>
+      <c r="C86" t="s">
+        <v>676</v>
+      </c>
+      <c r="D86" t="s">
+        <v>320</v>
+      </c>
+      <c r="E86" t="s">
+        <v>298</v>
+      </c>
+      <c r="F86">
+        <v>2</v>
+      </c>
+      <c r="G86" t="b">
+        <v>1</v>
+      </c>
+      <c r="H86" t="s">
+        <v>298</v>
+      </c>
+      <c r="I86" t="s">
+        <v>320</v>
+      </c>
+      <c r="J86" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>2019</v>
+      </c>
+      <c r="B87" t="s">
+        <v>638</v>
+      </c>
+      <c r="C87" t="s">
+        <v>676</v>
+      </c>
+      <c r="D87" t="s">
+        <v>316</v>
+      </c>
+      <c r="E87" t="s">
+        <v>287</v>
+      </c>
+      <c r="F87">
+        <v>2</v>
+      </c>
+      <c r="G87" t="b">
+        <v>1</v>
+      </c>
+      <c r="H87" t="s">
+        <v>298</v>
+      </c>
+      <c r="I87" t="s">
+        <v>320</v>
+      </c>
+      <c r="J87" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>2011</v>
+      </c>
+      <c r="B88" t="s">
+        <v>640</v>
+      </c>
+      <c r="C88" t="s">
+        <v>677</v>
+      </c>
+      <c r="D88" t="s">
+        <v>319</v>
+      </c>
+      <c r="E88" t="s">
+        <v>301</v>
+      </c>
+      <c r="F88">
+        <v>3</v>
+      </c>
+      <c r="G88" t="b">
+        <v>1</v>
+      </c>
+      <c r="H88" t="s">
+        <v>301</v>
+      </c>
+      <c r="I88" t="s">
+        <v>319</v>
+      </c>
+      <c r="J88" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>2010</v>
+      </c>
+      <c r="B89" t="s">
+        <v>640</v>
+      </c>
+      <c r="C89" t="s">
+        <v>677</v>
+      </c>
+      <c r="D89" t="s">
+        <v>320</v>
+      </c>
+      <c r="E89" t="s">
+        <v>298</v>
+      </c>
+      <c r="F89">
+        <v>3</v>
+      </c>
+      <c r="G89" t="b">
+        <v>1</v>
+      </c>
+      <c r="H89" t="s">
+        <v>301</v>
+      </c>
+      <c r="I89" t="s">
+        <v>319</v>
+      </c>
+      <c r="J89" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>2009</v>
+      </c>
+      <c r="B90" t="s">
+        <v>638</v>
+      </c>
+      <c r="C90" t="s">
+        <v>677</v>
+      </c>
+      <c r="D90" t="s">
+        <v>316</v>
+      </c>
+      <c r="E90" t="s">
+        <v>287</v>
+      </c>
+      <c r="F90">
+        <v>3</v>
+      </c>
+      <c r="G90" t="b">
+        <v>1</v>
+      </c>
+      <c r="H90" t="s">
+        <v>301</v>
+      </c>
+      <c r="I90" t="s">
+        <v>319</v>
+      </c>
+      <c r="J90" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>2024</v>
+      </c>
+      <c r="B91" t="s">
+        <v>638</v>
+      </c>
+      <c r="C91" t="s">
+        <v>678</v>
+      </c>
+      <c r="D91" t="s">
+        <v>311</v>
+      </c>
+      <c r="E91" t="s">
+        <v>282</v>
+      </c>
+      <c r="F91">
+        <v>2</v>
+      </c>
+      <c r="G91" t="b">
+        <v>1</v>
+      </c>
+      <c r="H91" t="s">
+        <v>282</v>
+      </c>
+      <c r="I91" t="s">
+        <v>311</v>
+      </c>
+      <c r="J91" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>2007</v>
+      </c>
+      <c r="B92" t="s">
+        <v>640</v>
+      </c>
+      <c r="C92" t="s">
+        <v>678</v>
+      </c>
+      <c r="D92" t="s">
+        <v>317</v>
+      </c>
+      <c r="E92" t="s">
+        <v>288</v>
+      </c>
+      <c r="F92">
+        <v>2</v>
+      </c>
+      <c r="G92" t="b">
+        <v>1</v>
+      </c>
+      <c r="H92" t="s">
+        <v>282</v>
+      </c>
+      <c r="I92" t="s">
+        <v>311</v>
+      </c>
+      <c r="J92" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>2018</v>
+      </c>
+      <c r="B93" t="s">
+        <v>638</v>
+      </c>
+      <c r="C93" t="s">
+        <v>679</v>
+      </c>
+      <c r="D93" t="s">
+        <v>321</v>
+      </c>
+      <c r="E93" t="s">
+        <v>293</v>
+      </c>
+      <c r="F93">
+        <v>2</v>
+      </c>
+      <c r="G93" t="b">
+        <v>1</v>
+      </c>
+      <c r="H93" t="s">
+        <v>293</v>
+      </c>
+      <c r="I93" t="s">
+        <v>321</v>
+      </c>
+      <c r="J93" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>2016</v>
+      </c>
+      <c r="B94" t="s">
+        <v>640</v>
+      </c>
+      <c r="C94" t="s">
+        <v>679</v>
+      </c>
+      <c r="D94" t="s">
+        <v>311</v>
+      </c>
+      <c r="E94" t="s">
+        <v>282</v>
+      </c>
+      <c r="F94">
+        <v>2</v>
+      </c>
+      <c r="G94" t="b">
+        <v>1</v>
+      </c>
+      <c r="H94" t="s">
+        <v>293</v>
+      </c>
+      <c r="I94" t="s">
+        <v>321</v>
+      </c>
+      <c r="J94" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>2024</v>
+      </c>
+      <c r="B95" t="s">
+        <v>638</v>
+      </c>
+      <c r="C95" t="s">
+        <v>680</v>
+      </c>
+      <c r="D95" t="s">
+        <v>318</v>
+      </c>
+      <c r="E95" t="s">
+        <v>291</v>
+      </c>
+      <c r="F95">
+        <v>2</v>
+      </c>
+      <c r="G95" t="b">
+        <v>1</v>
+      </c>
+      <c r="H95" t="s">
+        <v>291</v>
+      </c>
+      <c r="I95" t="s">
+        <v>318</v>
+      </c>
+      <c r="J95" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>2023</v>
+      </c>
+      <c r="B96" t="s">
+        <v>638</v>
+      </c>
+      <c r="C96" t="s">
+        <v>680</v>
+      </c>
+      <c r="D96" t="s">
+        <v>322</v>
+      </c>
+      <c r="E96" t="s">
+        <v>294</v>
+      </c>
+      <c r="F96">
+        <v>2</v>
+      </c>
+      <c r="G96" t="b">
+        <v>1</v>
+      </c>
+      <c r="H96" t="s">
+        <v>291</v>
+      </c>
+      <c r="I96" t="s">
+        <v>318</v>
+      </c>
+      <c r="J96" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>2024</v>
+      </c>
+      <c r="B97" t="s">
+        <v>638</v>
+      </c>
+      <c r="C97" t="s">
+        <v>681</v>
+      </c>
+      <c r="D97" t="s">
+        <v>320</v>
+      </c>
+      <c r="E97" t="s">
+        <v>298</v>
+      </c>
+      <c r="F97">
+        <v>2</v>
+      </c>
+      <c r="G97" t="b">
+        <v>1</v>
+      </c>
+      <c r="H97" t="s">
+        <v>298</v>
+      </c>
+      <c r="I97" t="s">
+        <v>320</v>
+      </c>
+      <c r="J97" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>2023</v>
+      </c>
+      <c r="B98" t="s">
+        <v>638</v>
+      </c>
+      <c r="C98" t="s">
+        <v>681</v>
+      </c>
+      <c r="D98" t="s">
+        <v>322</v>
+      </c>
+      <c r="E98" t="s">
+        <v>294</v>
+      </c>
+      <c r="F98">
+        <v>2</v>
+      </c>
+      <c r="G98" t="b">
+        <v>1</v>
+      </c>
+      <c r="H98" t="s">
+        <v>298</v>
+      </c>
+      <c r="I98" t="s">
+        <v>320</v>
+      </c>
+      <c r="J98" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>2024</v>
+      </c>
+      <c r="B99" t="s">
+        <v>638</v>
+      </c>
+      <c r="C99" t="s">
+        <v>682</v>
+      </c>
+      <c r="D99" t="s">
+        <v>325</v>
+      </c>
+      <c r="E99" t="s">
+        <v>290</v>
+      </c>
+      <c r="F99">
+        <v>2</v>
+      </c>
+      <c r="G99" t="b">
+        <v>1</v>
+      </c>
+      <c r="H99" t="s">
+        <v>290</v>
+      </c>
+      <c r="I99" t="s">
+        <v>325</v>
+      </c>
+      <c r="J99" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>2022</v>
+      </c>
+      <c r="B100" t="s">
+        <v>640</v>
+      </c>
+      <c r="C100" t="s">
+        <v>682</v>
+      </c>
+      <c r="D100" t="s">
+        <v>313</v>
+      </c>
+      <c r="E100" t="s">
+        <v>283</v>
+      </c>
+      <c r="F100">
+        <v>2</v>
+      </c>
+      <c r="G100" t="b">
+        <v>1</v>
+      </c>
+      <c r="H100" t="s">
+        <v>290</v>
+      </c>
+      <c r="I100" t="s">
+        <v>325</v>
+      </c>
+      <c r="J100" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>2011</v>
+      </c>
+      <c r="B101" t="s">
+        <v>640</v>
+      </c>
+      <c r="C101" t="s">
+        <v>683</v>
+      </c>
+      <c r="D101" t="s">
+        <v>320</v>
+      </c>
+      <c r="E101" t="s">
+        <v>298</v>
+      </c>
+      <c r="F101">
+        <v>2</v>
+      </c>
+      <c r="G101" t="b">
+        <v>1</v>
+      </c>
+      <c r="H101" t="s">
+        <v>298</v>
+      </c>
+      <c r="I101" t="s">
+        <v>320</v>
+      </c>
+      <c r="J101" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>2007</v>
+      </c>
+      <c r="B102" t="s">
+        <v>640</v>
+      </c>
+      <c r="C102" t="s">
+        <v>683</v>
+      </c>
+      <c r="D102" t="s">
+        <v>316</v>
+      </c>
+      <c r="E102" t="s">
+        <v>287</v>
+      </c>
+      <c r="F102">
+        <v>2</v>
+      </c>
+      <c r="G102" t="b">
+        <v>1</v>
+      </c>
+      <c r="H102" t="s">
+        <v>298</v>
+      </c>
+      <c r="I102" t="s">
+        <v>320</v>
+      </c>
+      <c r="J102" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>2022</v>
+      </c>
+      <c r="B103" t="s">
+        <v>640</v>
+      </c>
+      <c r="C103" t="s">
+        <v>684</v>
+      </c>
+      <c r="D103" t="s">
+        <v>314</v>
+      </c>
+      <c r="E103" t="s">
+        <v>286</v>
+      </c>
+      <c r="F103">
+        <v>2</v>
+      </c>
+      <c r="G103" t="b">
+        <v>1</v>
+      </c>
+      <c r="H103" t="s">
+        <v>286</v>
+      </c>
+      <c r="I103" t="s">
+        <v>314</v>
+      </c>
+      <c r="J103" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>2019</v>
+      </c>
+      <c r="B104" t="s">
+        <v>638</v>
+      </c>
+      <c r="C104" t="s">
+        <v>684</v>
+      </c>
+      <c r="D104" t="s">
+        <v>321</v>
+      </c>
+      <c r="E104" t="s">
+        <v>293</v>
+      </c>
+      <c r="F104">
+        <v>2</v>
+      </c>
+      <c r="G104" t="b">
+        <v>1</v>
+      </c>
+      <c r="H104" t="s">
+        <v>286</v>
+      </c>
+      <c r="I104" t="s">
+        <v>314</v>
+      </c>
+      <c r="J104" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>2022</v>
+      </c>
+      <c r="B105" t="s">
+        <v>640</v>
+      </c>
+      <c r="C105" t="s">
+        <v>685</v>
+      </c>
+      <c r="D105" t="s">
+        <v>323</v>
+      </c>
+      <c r="E105" t="s">
+        <v>302</v>
+      </c>
+      <c r="F105">
+        <v>3</v>
+      </c>
+      <c r="G105" t="b">
+        <v>1</v>
+      </c>
+      <c r="H105" t="s">
+        <v>302</v>
+      </c>
+      <c r="I105" t="s">
+        <v>323</v>
+      </c>
+      <c r="J105" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <v>2021</v>
+      </c>
+      <c r="B106" t="s">
+        <v>640</v>
+      </c>
+      <c r="C106" t="s">
+        <v>685</v>
+      </c>
+      <c r="D106" t="s">
+        <v>320</v>
+      </c>
+      <c r="E106" t="s">
+        <v>298</v>
+      </c>
+      <c r="F106">
+        <v>3</v>
+      </c>
+      <c r="G106" t="b">
+        <v>1</v>
+      </c>
+      <c r="H106" t="s">
+        <v>302</v>
+      </c>
+      <c r="I106" t="s">
+        <v>323</v>
+      </c>
+      <c r="J106" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <v>2019</v>
+      </c>
+      <c r="B107" t="s">
+        <v>638</v>
+      </c>
+      <c r="C107" t="s">
+        <v>685</v>
+      </c>
+      <c r="D107" t="s">
+        <v>321</v>
+      </c>
+      <c r="E107" t="s">
+        <v>293</v>
+      </c>
+      <c r="F107">
+        <v>3</v>
+      </c>
+      <c r="G107" t="b">
+        <v>1</v>
+      </c>
+      <c r="H107" t="s">
+        <v>302</v>
+      </c>
+      <c r="I107" t="s">
+        <v>323</v>
+      </c>
+      <c r="J107" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <v>2017</v>
+      </c>
+      <c r="B108" t="s">
+        <v>640</v>
+      </c>
+      <c r="C108" t="s">
+        <v>686</v>
+      </c>
+      <c r="D108" t="s">
+        <v>318</v>
+      </c>
+      <c r="E108" t="s">
+        <v>291</v>
+      </c>
+      <c r="F108">
+        <v>3</v>
+      </c>
+      <c r="G108" t="b">
+        <v>1</v>
+      </c>
+      <c r="H108" t="s">
+        <v>291</v>
+      </c>
+      <c r="I108" t="s">
+        <v>318</v>
+      </c>
+      <c r="J108" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <v>2009</v>
+      </c>
+      <c r="B109" t="s">
+        <v>640</v>
+      </c>
+      <c r="C109" t="s">
+        <v>686</v>
+      </c>
+      <c r="D109" t="s">
+        <v>320</v>
+      </c>
+      <c r="E109" t="s">
+        <v>298</v>
+      </c>
+      <c r="F109">
+        <v>3</v>
+      </c>
+      <c r="G109" t="b">
+        <v>1</v>
+      </c>
+      <c r="H109" t="s">
+        <v>291</v>
+      </c>
+      <c r="I109" t="s">
+        <v>318</v>
+      </c>
+      <c r="J109" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <v>2008</v>
+      </c>
+      <c r="B110" t="s">
+        <v>640</v>
+      </c>
+      <c r="C110" t="s">
+        <v>686</v>
+      </c>
+      <c r="D110" t="s">
+        <v>315</v>
+      </c>
+      <c r="E110" t="s">
+        <v>285</v>
+      </c>
+      <c r="F110">
+        <v>3</v>
+      </c>
+      <c r="G110" t="b">
+        <v>1</v>
+      </c>
+      <c r="H110" t="s">
+        <v>291</v>
+      </c>
+      <c r="I110" t="s">
+        <v>318</v>
+      </c>
+      <c r="J110" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <v>2022</v>
+      </c>
+      <c r="B111" t="s">
+        <v>640</v>
+      </c>
+      <c r="C111" t="s">
+        <v>687</v>
+      </c>
+      <c r="D111" t="s">
+        <v>320</v>
+      </c>
+      <c r="E111" t="s">
+        <v>298</v>
+      </c>
+      <c r="F111">
+        <v>2</v>
+      </c>
+      <c r="G111" t="b">
+        <v>1</v>
+      </c>
+      <c r="H111" t="s">
+        <v>298</v>
+      </c>
+      <c r="I111" t="s">
+        <v>320</v>
+      </c>
+      <c r="J111" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A112">
+        <v>2018</v>
+      </c>
+      <c r="B112" t="s">
+        <v>638</v>
+      </c>
+      <c r="C112" t="s">
+        <v>687</v>
+      </c>
+      <c r="D112" t="s">
+        <v>318</v>
+      </c>
+      <c r="E112" t="s">
+        <v>291</v>
+      </c>
+      <c r="F112">
+        <v>2</v>
+      </c>
+      <c r="G112" t="b">
+        <v>1</v>
+      </c>
+      <c r="H112" t="s">
+        <v>298</v>
+      </c>
+      <c r="I112" t="s">
+        <v>320</v>
+      </c>
+      <c r="J112" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A113">
+        <v>2024</v>
+      </c>
+      <c r="B113" t="s">
+        <v>638</v>
+      </c>
+      <c r="C113" t="s">
+        <v>688</v>
+      </c>
+      <c r="D113" t="s">
+        <v>332</v>
+      </c>
+      <c r="E113" t="s">
+        <v>343</v>
+      </c>
+      <c r="F113">
+        <v>2</v>
+      </c>
+      <c r="G113" t="b">
+        <v>1</v>
+      </c>
+      <c r="H113" t="s">
+        <v>343</v>
+      </c>
+      <c r="I113" t="s">
+        <v>332</v>
+      </c>
+      <c r="J113" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A114">
+        <v>2008</v>
+      </c>
+      <c r="B114" t="s">
+        <v>640</v>
+      </c>
+      <c r="C114" t="s">
+        <v>688</v>
+      </c>
+      <c r="D114" t="s">
+        <v>328</v>
+      </c>
+      <c r="E114" t="s">
+        <v>339</v>
+      </c>
+      <c r="F114">
+        <v>2</v>
+      </c>
+      <c r="G114" t="b">
+        <v>1</v>
+      </c>
+      <c r="H114" t="s">
+        <v>343</v>
+      </c>
+      <c r="I114" t="s">
+        <v>332</v>
+      </c>
+      <c r="J114" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A115">
+        <v>2022</v>
+      </c>
+      <c r="B115" t="s">
+        <v>640</v>
+      </c>
+      <c r="C115" t="s">
+        <v>689</v>
+      </c>
+      <c r="D115" t="s">
+        <v>323</v>
+      </c>
+      <c r="E115" t="s">
+        <v>302</v>
+      </c>
+      <c r="F115">
+        <v>3</v>
+      </c>
+      <c r="G115" t="b">
+        <v>1</v>
+      </c>
+      <c r="H115" t="s">
+        <v>302</v>
+      </c>
+      <c r="I115" t="s">
+        <v>323</v>
+      </c>
+      <c r="J115" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A116">
+        <v>2021</v>
+      </c>
+      <c r="B116" t="s">
+        <v>640</v>
+      </c>
+      <c r="C116" t="s">
+        <v>689</v>
+      </c>
+      <c r="D116" t="s">
+        <v>320</v>
+      </c>
+      <c r="E116" t="s">
+        <v>298</v>
+      </c>
+      <c r="F116">
+        <v>3</v>
+      </c>
+      <c r="G116" t="b">
+        <v>1</v>
+      </c>
+      <c r="H116" t="s">
+        <v>302</v>
+      </c>
+      <c r="I116" t="s">
+        <v>323</v>
+      </c>
+      <c r="J116" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A117">
+        <v>2019</v>
+      </c>
+      <c r="B117" t="s">
+        <v>638</v>
+      </c>
+      <c r="C117" t="s">
+        <v>689</v>
+      </c>
+      <c r="D117" t="s">
+        <v>321</v>
+      </c>
+      <c r="E117" t="s">
+        <v>293</v>
+      </c>
+      <c r="F117">
+        <v>3</v>
+      </c>
+      <c r="G117" t="b">
+        <v>1</v>
+      </c>
+      <c r="H117" t="s">
+        <v>302</v>
+      </c>
+      <c r="I117" t="s">
+        <v>323</v>
+      </c>
+      <c r="J117" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A118">
+        <v>2024</v>
+      </c>
+      <c r="B118" t="s">
+        <v>638</v>
+      </c>
+      <c r="C118" t="s">
+        <v>690</v>
+      </c>
+      <c r="D118" t="s">
+        <v>325</v>
+      </c>
+      <c r="E118" t="s">
+        <v>290</v>
+      </c>
+      <c r="F118">
+        <v>2</v>
+      </c>
+      <c r="G118" t="b">
+        <v>1</v>
+      </c>
+      <c r="H118" t="s">
+        <v>290</v>
+      </c>
+      <c r="I118" t="s">
+        <v>325</v>
+      </c>
+      <c r="J118" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A119">
+        <v>2022</v>
+      </c>
+      <c r="B119" t="s">
+        <v>640</v>
+      </c>
+      <c r="C119" t="s">
+        <v>690</v>
+      </c>
+      <c r="D119" t="s">
+        <v>313</v>
+      </c>
+      <c r="E119" t="s">
+        <v>283</v>
+      </c>
+      <c r="F119">
+        <v>2</v>
+      </c>
+      <c r="G119" t="b">
+        <v>1</v>
+      </c>
+      <c r="H119" t="s">
+        <v>290</v>
+      </c>
+      <c r="I119" t="s">
+        <v>325</v>
+      </c>
+      <c r="J119" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A120">
+        <v>2024</v>
+      </c>
+      <c r="B120" t="s">
+        <v>638</v>
+      </c>
+      <c r="C120" t="s">
+        <v>691</v>
+      </c>
+      <c r="D120" t="s">
+        <v>320</v>
+      </c>
+      <c r="E120" t="s">
+        <v>298</v>
+      </c>
+      <c r="F120">
+        <v>2</v>
+      </c>
+      <c r="G120" t="b">
+        <v>1</v>
+      </c>
+      <c r="H120" t="s">
+        <v>298</v>
+      </c>
+      <c r="I120" t="s">
+        <v>320</v>
+      </c>
+      <c r="J120" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A121">
+        <v>2023</v>
+      </c>
+      <c r="B121" t="s">
+        <v>640</v>
+      </c>
+      <c r="C121" t="s">
+        <v>691</v>
+      </c>
+      <c r="D121" t="s">
+        <v>321</v>
+      </c>
+      <c r="E121" t="s">
+        <v>293</v>
+      </c>
+      <c r="F121">
+        <v>2</v>
+      </c>
+      <c r="G121" t="b">
+        <v>1</v>
+      </c>
+      <c r="H121" t="s">
+        <v>298</v>
+      </c>
+      <c r="I121" t="s">
+        <v>320</v>
+      </c>
+      <c r="J121" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A122">
+        <v>2022</v>
+      </c>
+      <c r="B122" t="s">
+        <v>640</v>
+      </c>
+      <c r="C122" t="s">
+        <v>692</v>
+      </c>
+      <c r="D122" t="s">
+        <v>323</v>
+      </c>
+      <c r="E122" t="s">
+        <v>302</v>
+      </c>
+      <c r="F122">
+        <v>4</v>
+      </c>
+      <c r="G122" t="b">
+        <v>1</v>
+      </c>
+      <c r="H122" t="s">
+        <v>302</v>
+      </c>
+      <c r="I122" t="s">
+        <v>323</v>
+      </c>
+      <c r="J122" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A123">
+        <v>2021</v>
+      </c>
+      <c r="B123" t="s">
+        <v>640</v>
+      </c>
+      <c r="C123" t="s">
+        <v>692</v>
+      </c>
+      <c r="D123" t="s">
+        <v>320</v>
+      </c>
+      <c r="E123" t="s">
+        <v>298</v>
+      </c>
+      <c r="F123">
+        <v>4</v>
+      </c>
+      <c r="G123" t="b">
+        <v>1</v>
+      </c>
+      <c r="H123" t="s">
+        <v>302</v>
+      </c>
+      <c r="I123" t="s">
+        <v>323</v>
+      </c>
+      <c r="J123" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A124">
+        <v>2019</v>
+      </c>
+      <c r="B124" t="s">
+        <v>638</v>
+      </c>
+      <c r="C124" t="s">
+        <v>692</v>
+      </c>
+      <c r="D124" t="s">
+        <v>321</v>
+      </c>
+      <c r="E124" t="s">
+        <v>293</v>
+      </c>
+      <c r="F124">
+        <v>4</v>
+      </c>
+      <c r="G124" t="b">
+        <v>1</v>
+      </c>
+      <c r="H124" t="s">
+        <v>302</v>
+      </c>
+      <c r="I124" t="s">
+        <v>323</v>
+      </c>
+      <c r="J124" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A125">
+        <v>2013</v>
+      </c>
+      <c r="B125" t="s">
+        <v>640</v>
+      </c>
+      <c r="C125" t="s">
+        <v>692</v>
+      </c>
+      <c r="D125" t="s">
+        <v>315</v>
+      </c>
+      <c r="E125" t="s">
+        <v>285</v>
+      </c>
+      <c r="F125">
+        <v>4</v>
+      </c>
+      <c r="G125" t="b">
+        <v>1</v>
+      </c>
+      <c r="H125" t="s">
+        <v>302</v>
+      </c>
+      <c r="I125" t="s">
+        <v>323</v>
+      </c>
+      <c r="J125" t="s">
+        <v>694</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated mapping of LDA-LLM topics
</commit_message>
<xml_diff>
--- a/input/mapping_tabeller.xlsx
+++ b/input/mapping_tabeller.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admkbo\Documents\FTIND\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C624DF16-41F5-49BC-9F06-1AE62CEDF1A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B80A27E5-486B-4D9C-BC50-D0E16B24A79B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{6B009A8E-40F0-41F8-8A22-826EDE827CF8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{6B009A8E-40F0-41F8-8A22-826EDE827CF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Lande" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,9 @@
     <sheet name="Partigrupper" sheetId="3" r:id="rId3"/>
     <sheet name="Stopwords" sheetId="4" r:id="rId4"/>
     <sheet name="Emner" sheetId="5" r:id="rId5"/>
-    <sheet name="Partihoppere" sheetId="6" r:id="rId6"/>
+    <sheet name="EmnerOLD_Unikke" sheetId="8" r:id="rId6"/>
+    <sheet name="EmnerOLD" sheetId="7" r:id="rId7"/>
+    <sheet name="Partihoppere" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2131" uniqueCount="709">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2197" uniqueCount="744">
   <si>
     <t>Albanien</t>
   </si>
@@ -2168,6 +2170,111 @@
   </si>
   <si>
     <t>BP</t>
+  </si>
+  <si>
+    <t>2025-F_Topic 0</t>
+  </si>
+  <si>
+    <t>Politisk debat om indfødsret og statsborgerskab i Danmark</t>
+  </si>
+  <si>
+    <t>2025-F_Topic 1</t>
+  </si>
+  <si>
+    <t>Debat om statsborgerskab og integrationspolitik i Danmark</t>
+  </si>
+  <si>
+    <t>2025-F_Topic 2</t>
+  </si>
+  <si>
+    <t>Debatten om statsborgerskab og indvandringspolitik i Danmark</t>
+  </si>
+  <si>
+    <t>2025-F_Topic 3</t>
+  </si>
+  <si>
+    <t>Politisk Debat om Udlændingepolitik og Identitet i Danmark</t>
+  </si>
+  <si>
+    <t>Topics to choose from</t>
+  </si>
+  <si>
+    <t>De eksisterende krav til indfødsret burde strammes</t>
+  </si>
+  <si>
+    <t>Der er enighed om behovet for klare og konsekvente regler for tildeling af dansk statsborgerskab og bekymringer over ændringer af betingelserne efter ansøgninger, hvilket underminerer tilliden til systemet. Diskussionen om statsborgerskab omfatter også spørgsmål om diskrimination baseret på oprindelse, økonomiske kriterier og beskyttelse af grundlæggende frihedsrettigheder. Flere partier ønsker at sikre, at borgere, der opfylder kravene, behandles retfærdigt og ikke bliver påvirket af politiske skift eller fordomme.</t>
+  </si>
+  <si>
+    <t>At opnå dansk statsborgerskab kræver opfyldelse af strenge krav, herunder sprogkundskaber, selvforsørgelse og kendskab til danske værdier, hvilket anerkendes som et stort privilegium. Fejringen af de nye statsborgere understreger vigtigheden af deres bidrag til samfundet og muligheden for at deltage aktivt i demokratiet. Der er en generel enighed om, at statsborgerskab fremmer integration og tilhørsforhold, samtidig med at der er ønsker om at lette betingelserne for at gøre det lettere for flere at blive en del af det danske fællesskab.</t>
+  </si>
+  <si>
+    <t>Der anerkendes udfordringer forbundet med islamisme og sharialov i visse ghettoer, samt problemer relateret til ikkevestlig indvandring.</t>
+  </si>
+  <si>
+    <t>Der er behov for, at politikere træffer beslutninger baseret på deres overbevisninger for at sikre Danmarks fremtid og velfærd. Regeringen anerkender forskellige synspunkter og har oprettet en ekspertgruppe for at forbedre borgerbehandlingen, men der er bekymringer om, at sindelagssamtaler kan overtræde retsstatsprincipperne. Der appelleres til ministeren om at sikre, at disse principper respekteres i statsborgerskabsansøgninger.</t>
+  </si>
+  <si>
+    <t>Indlægget kritiserer Hr. Jesper Langballes udtalelser som perfide og faktuelt mangelfulde, samtidig med at der påpeges, at direkte tiltale ikke må anvendes i debatten.</t>
+  </si>
+  <si>
+    <t>Der er behov for at nedsætte en ekspertgruppe for at opnå resultater, men der er usikkerhed om tidshorisonten. Der søges klarhed over Venstres støtte til den tidligere beslutning om en undersøgelseskommission.</t>
+  </si>
+  <si>
+    <t>Der afholdes en række taler og bemærkninger fra forskellige ordførere i Folketinget, hvor der udveksles synspunkter om udlændingepolitik, kontrol af ansøgere til statsborgerskab og politiske holdninger. Flere parter udtrykker bekymringer over håndteringen af emner såsom kriminalitet og integration, samt behovet for klarhed og ansvarlighed i lovgivningen. Der er også et fokus på samarbejde mellem partierne i den politiske debat.</t>
+  </si>
+  <si>
+    <t>Der er en stigende politisk debat om indfødsret i Danmark, med fokus på at sikre, at statsborgerskab kun tildeles personer, der har vist loyalitet og tilknytning til landet. Der er bekymring over tildelingen af statsborgerskab til personer med kriminel baggrund og et ønske om strammere kriterier og individuel vurdering af ansøgere. Partier som Dansk Folkeparti presser på for at ændre procedurerne, hvilket skaber en kompleks diskussion om balance mellem integration, sikkerhed og danske værdier.</t>
+  </si>
+  <si>
+    <t>Der har været en række afstemninger om forskellige ændringsforslag, hvor mange blev forkastet med stor margin. Lovforslaget er blevet vedtaget til direkte behandling uden fornyet udvalgsbehandling, og der er flere ændringsforslag, der er blevet betragtet som vedtaget uden afstemning, når ingen har gjort indsigelse. Generelt set har ændringsforslag fra mindretal, især fra DF, ofte ikke fået støtte fra flertallet.</t>
+  </si>
+  <si>
+    <t>Der er en fælles opfattelse af, at Socialdemokratiet lider under utilstrækkelig intern kommunikation.</t>
+  </si>
+  <si>
+    <t>Der er enighed blandt partierne om at stramme reglerne for dansk statsborgerskab, herunder krav om, at ansøgere skal dele grundlæggende demokratiske værdier og udelukkelse af personer med kriminel baggrund. Liberal Alliance og andre partier understreger behovet for at håndhæve disse stramninger og prioritere kvalificerede ansøgere.</t>
+  </si>
+  <si>
+    <t>Der er en igangværende debat om statsborgerskabslovgivning, hvor forskellige partier stiller spørgsmålstegn ved hinandens holdninger og forslag, herunder håndtering af statsløse personer og krav til ansøgere om statsborgerskab. Der er bekymring for, at massetildeling af statsborgerskaber uden tilstrækkelig kontrol kan have negative konsekvenser for samfundet, samtidig med at der er behov for at balancere demokratiske værdier med sikkerhed og integration. Diskussionen omfatter også hvordan kriminalitet påvirker tildeling af statsborgerskab og hvordan forskellige partier forholder sig til dette emne.</t>
+  </si>
+  <si>
+    <t>To personer med kriminel baggrund er blevet forpligtet til at optages på statsborgerskabslovforslaget på grund af sagsbehandlingsfejl, hvilket rejser spørgsmål om lovens anvendelse.</t>
+  </si>
+  <si>
+    <t>Der er en udbredt bekymring over indvandring og tildeling af dansk statsborgerskab, især til personer med kriminel baggrund, hvilket fører til uenighed mellem politiske partier om stramning af reglerne. Mange parter ønsker at sikre, at statsborgerskab kun gives til dem, der bidrager positivt til samfundet, og der efterlyses bedre kontrol med ansøgeres baggrund og rettigheder. Diskussionen om indvandringens omfang og dens indvirkning på det danske samfund er central, med krav om klare kriterier for tildeling af statsborgerskab.</t>
+  </si>
+  <si>
+    <t>Forhandlingen er afsluttet, da ingen ønsker at udtale sig, og der er indkaldt til afstemning. Der er stillet ændringsforslag, men ingen har ønsket at kommentere dem.</t>
+  </si>
+  <si>
+    <t>Folketinget står over for en debat om indfødsret, hvor der stilles spørgsmål ved, om internationale konventioner skal have indflydelse på beslutninger om statsborgerskab, især i forhold til personer, der kan udgøre en sikkerhedsrisiko. Der er også bekymringer om, hvordan sager behandles og beslutninger træffes i Indfødsretsudvalget, samt om det er acceptabelt at inkludere personer med problematiske baggrunde i lovforslag. Der er enighed om, at grundloven har forrang over konventionerne, og Folketinget har ret til at fastlægge betingelserne for indfødsret.</t>
+  </si>
+  <si>
+    <t>Der er en generel enighed blandt partierne om behovet for strammere kriterier for tildeling af dansk statsborgerskab, især i forhold til personer med kriminel baggrund. Der stilles spørgsmål ved, hvordan indfødsretsprocessen skal håndteres, herunder behovet for individuel behandling og objektive kriterier, samt bekymringer om politisk indflydelse på beslutningerne. Derudover er der en åbenhed for dialog og forhandlinger mellem partierne, selvom der er uenigheder om specifikke tilgange og holdninger til statsborgerskab.</t>
+  </si>
+  <si>
+    <t>Der rejses kritik af, at partier som Alternativet og Radikale Venstre ikke deltager i behandlingen af et vigtigt forslag, hvilket stiller spørgsmål ved deres seriøsitet. Liberal Alliance repræsenterer en ændring i tilgang ved at fokusere på ansøgeres værdier, hvilket skaber debat om partiets tidligere holdninger. Forhandlingen om lovforslaget er afsluttet, og det er vedtaget at henvise det til Indfødsretsudvalget.</t>
+  </si>
+  <si>
+    <t>Der er behov for tydeligere regler og retssikkerhed i ansøgningsprocessen</t>
+  </si>
+  <si>
+    <t>Statsborgerskab fremmer integration og belønner ansøgernes bidrag til samfundet</t>
+  </si>
+  <si>
+    <t>Der er problemer med kulturelle forskelle ifm. ikke-vestlig indvandring</t>
+  </si>
+  <si>
+    <t>Ren procedure snak/politiker peger fingre på hinanden</t>
+  </si>
+  <si>
+    <t>Diskussion af politiske tiltag fra regeringen/partiernes side ifm. indfødsretsprocessen</t>
+  </si>
+  <si>
+    <t>Der er bekymringer for utilstrækkelig integration og kriminalitet blandt dem, som tildeles indfødsret</t>
+  </si>
+  <si>
+    <t>Reglerne for opnåelsen af dansk statsborgerskab bør strammes</t>
   </si>
 </sst>
 </file>
@@ -2258,7 +2365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2278,11 +2385,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="16">
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <border outline="0">
         <top style="thin">
@@ -2341,6 +2463,21 @@
       <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
   </dxfs>
@@ -2354,6 +2491,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2395,27 +2536,50 @@
   <autoFilter ref="A1:B27" xr:uid="{D929CE4D-DE0E-4371-9D74-DAF23F806F68}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{703DE216-50CE-4E57-B997-17634E591F71}" name="Ord"/>
-    <tableColumn id="2" xr3:uid="{A35AE28A-3BB9-4161-A171-35C527B7C143}" name="DatoTilføjet" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{A35AE28A-3BB9-4161-A171-35C527B7C143}" name="DatoTilføjet" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{2C1F5FC9-D397-455C-AEAF-D1763528A602}" name="Emner" displayName="Emner" ref="A1:D126" totalsRowShown="0" dataDxfId="7">
-  <autoFilter ref="A1:D126" xr:uid="{2C1F5FC9-D397-455C-AEAF-D1763528A602}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{2C1F5FC9-D397-455C-AEAF-D1763528A602}" name="Emner" displayName="Emner" ref="A1:D19" totalsRowShown="0" dataDxfId="14">
+  <autoFilter ref="A1:D19" xr:uid="{2C1F5FC9-D397-455C-AEAF-D1763528A602}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{6F47ADCF-7B5E-431B-8209-B52E2671F6C3}" name="Id" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{625A89F7-2E0B-4AE9-8481-CBE8317B581F}" name="AutomatiskEmne" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{64403E5D-601B-4B88-B55D-4ECF3EA9DC38}" name="EmneGruppe" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{CF0732A2-488A-4A32-B356-40B8CE60F4B8}" name="SidstOpdatret" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{6F47ADCF-7B5E-431B-8209-B52E2671F6C3}" name="Id" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{625A89F7-2E0B-4AE9-8481-CBE8317B581F}" name="AutomatiskEmne" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{64403E5D-601B-4B88-B55D-4ECF3EA9DC38}" name="EmneGruppe" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{CF0732A2-488A-4A32-B356-40B8CE60F4B8}" name="SidstOpdatret" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{74B9B96F-B2B9-4B1F-B795-88782D08D518}" name="Partihoppere" displayName="Partihoppere" ref="A1:J156" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{ACEBC73D-D5CB-474D-A08E-341527931D76}" name="Table8" displayName="Table8" ref="A1:A14" totalsRowShown="0" dataDxfId="11">
+  <autoFilter ref="A1:A14" xr:uid="{ACEBC73D-D5CB-474D-A08E-341527931D76}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{3D760C71-CA3D-4682-AB2E-A98C0BA67482}" name="Topics to choose from" dataDxfId="10"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{204A3821-716B-47DA-873B-31C8C0CEF80B}" name="EmnerOLD" displayName="EmnerOLD" ref="A1:D130" totalsRowShown="0" dataDxfId="9">
+  <autoFilter ref="A1:D130" xr:uid="{2C1F5FC9-D397-455C-AEAF-D1763528A602}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{94BA0EB3-0C75-479D-9BD6-7C6FB84F78EE}" name="Id" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{A5450B2C-F4C6-4F5C-9C58-5034F7F7DA04}" name="AutomatiskEmne" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{27DD0F04-ABC0-4A1C-BD5A-95A66D0F1812}" name="EmneGruppe" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{DD14152F-048A-4656-8E38-362FA4F4752D}" name="SidstOpdatret" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{74B9B96F-B2B9-4B1F-B795-88782D08D518}" name="Partihoppere" displayName="Partihoppere" ref="A1:J156" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2">
   <autoFilter ref="A1:J156" xr:uid="{74B9B96F-B2B9-4B1F-B795-88782D08D518}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J156">
     <sortCondition ref="C1:C156"/>
@@ -5553,10 +5717,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F1D6B43-84E6-4039-8D1A-0E6D941491BF}">
-  <dimension ref="A1:D126"/>
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="B127" sqref="B127"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5574,1762 +5741,228 @@
       <c r="B1" s="4" t="s">
         <v>374</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>375</v>
       </c>
       <c r="D1" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>376</v>
-      </c>
-      <c r="B2" t="s">
-        <v>377</v>
-      </c>
-      <c r="C2" t="s">
-        <v>623</v>
-      </c>
-      <c r="D2" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>378</v>
-      </c>
-      <c r="B3" t="s">
-        <v>379</v>
-      </c>
-      <c r="C3" t="s">
-        <v>621</v>
-      </c>
-      <c r="D3" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>380</v>
-      </c>
-      <c r="B4" t="s">
-        <v>381</v>
-      </c>
-      <c r="C4" t="s">
-        <v>619</v>
-      </c>
-      <c r="D4" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>382</v>
-      </c>
-      <c r="B5" t="s">
-        <v>383</v>
-      </c>
-      <c r="C5" t="s">
-        <v>620</v>
-      </c>
-      <c r="D5" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>384</v>
-      </c>
-      <c r="B6" t="s">
-        <v>385</v>
-      </c>
-      <c r="C6" t="s">
-        <v>621</v>
-      </c>
-      <c r="D6" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>386</v>
-      </c>
-      <c r="B7" t="s">
-        <v>387</v>
-      </c>
-      <c r="C7" t="s">
-        <v>618</v>
-      </c>
-      <c r="D7" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>388</v>
-      </c>
-      <c r="B8" t="s">
-        <v>389</v>
-      </c>
-      <c r="C8" t="s">
-        <v>618</v>
-      </c>
-      <c r="D8" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>390</v>
-      </c>
-      <c r="B9" t="s">
-        <v>391</v>
-      </c>
-      <c r="C9" t="s">
-        <v>624</v>
-      </c>
-      <c r="D9" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>392</v>
-      </c>
-      <c r="B10" t="s">
-        <v>393</v>
-      </c>
-      <c r="C10" t="s">
-        <v>618</v>
-      </c>
-      <c r="D10" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>394</v>
-      </c>
-      <c r="B11" t="s">
-        <v>395</v>
-      </c>
-      <c r="C11" t="s">
-        <v>621</v>
-      </c>
-      <c r="D11" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>396</v>
-      </c>
-      <c r="B12" t="s">
-        <v>397</v>
-      </c>
-      <c r="C12" t="s">
-        <v>621</v>
-      </c>
-      <c r="D12" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>398</v>
-      </c>
-      <c r="B13" t="s">
-        <v>399</v>
-      </c>
-      <c r="C13" t="s">
-        <v>618</v>
-      </c>
-      <c r="D13" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>400</v>
-      </c>
-      <c r="B14" t="s">
-        <v>401</v>
-      </c>
-      <c r="C14" t="s">
-        <v>620</v>
-      </c>
-      <c r="D14" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>402</v>
-      </c>
-      <c r="B15" t="s">
-        <v>403</v>
-      </c>
-      <c r="C15" t="s">
-        <v>621</v>
-      </c>
-      <c r="D15" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>404</v>
-      </c>
-      <c r="B16" t="s">
-        <v>405</v>
-      </c>
-      <c r="C16" t="s">
-        <v>620</v>
-      </c>
-      <c r="D16" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>406</v>
-      </c>
-      <c r="B17" t="s">
-        <v>407</v>
-      </c>
-      <c r="C17" t="s">
-        <v>620</v>
-      </c>
-      <c r="D17" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>408</v>
-      </c>
-      <c r="B18" t="s">
-        <v>409</v>
-      </c>
-      <c r="C18" t="s">
-        <v>630</v>
-      </c>
-      <c r="D18" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>410</v>
-      </c>
-      <c r="B19" t="s">
-        <v>411</v>
-      </c>
-      <c r="C19" t="s">
-        <v>620</v>
-      </c>
-      <c r="D19" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>412</v>
-      </c>
-      <c r="B20" t="s">
-        <v>413</v>
-      </c>
-      <c r="C20" t="s">
-        <v>620</v>
-      </c>
-      <c r="D20" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>414</v>
-      </c>
-      <c r="B21" t="s">
-        <v>415</v>
-      </c>
-      <c r="C21" t="s">
-        <v>618</v>
-      </c>
-      <c r="D21" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>416</v>
-      </c>
-      <c r="B22" t="s">
-        <v>417</v>
-      </c>
-      <c r="C22" t="s">
-        <v>620</v>
-      </c>
-      <c r="D22" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>418</v>
-      </c>
-      <c r="B23" t="s">
-        <v>419</v>
-      </c>
-      <c r="C23" t="s">
-        <v>621</v>
-      </c>
-      <c r="D23" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>420</v>
-      </c>
-      <c r="B24" t="s">
-        <v>421</v>
-      </c>
-      <c r="C24" t="s">
-        <v>622</v>
-      </c>
-      <c r="D24" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>422</v>
-      </c>
-      <c r="B25" t="s">
-        <v>423</v>
-      </c>
-      <c r="C25" t="s">
-        <v>630</v>
-      </c>
-      <c r="D25" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>424</v>
-      </c>
-      <c r="B26" t="s">
-        <v>425</v>
-      </c>
-      <c r="C26" t="s">
-        <v>621</v>
-      </c>
-      <c r="D26" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>426</v>
-      </c>
-      <c r="B27" t="s">
-        <v>427</v>
-      </c>
-      <c r="C27" t="s">
-        <v>620</v>
-      </c>
-      <c r="D27" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>428</v>
-      </c>
-      <c r="B28" t="s">
-        <v>429</v>
-      </c>
-      <c r="C28" t="s">
-        <v>618</v>
-      </c>
-      <c r="D28" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>430</v>
-      </c>
-      <c r="B29" t="s">
-        <v>431</v>
-      </c>
-      <c r="C29" t="s">
-        <v>623</v>
-      </c>
-      <c r="D29" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>432</v>
-      </c>
-      <c r="B30" t="s">
-        <v>433</v>
-      </c>
-      <c r="C30" t="s">
-        <v>621</v>
-      </c>
-      <c r="D30" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>434</v>
-      </c>
-      <c r="B31" t="s">
-        <v>435</v>
-      </c>
-      <c r="C31" t="s">
-        <v>621</v>
-      </c>
-      <c r="D31" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>436</v>
-      </c>
-      <c r="B32" t="s">
-        <v>437</v>
-      </c>
-      <c r="C32" t="s">
-        <v>630</v>
-      </c>
-      <c r="D32" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>438</v>
-      </c>
-      <c r="B33" t="s">
-        <v>439</v>
-      </c>
-      <c r="C33" t="s">
-        <v>625</v>
-      </c>
-      <c r="D33" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>440</v>
-      </c>
-      <c r="B34" t="s">
-        <v>441</v>
-      </c>
-      <c r="C34" t="s">
-        <v>630</v>
-      </c>
-      <c r="D34" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>442</v>
-      </c>
-      <c r="B35" t="s">
-        <v>443</v>
-      </c>
-      <c r="C35" t="s">
-        <v>624</v>
-      </c>
-      <c r="D35" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>444</v>
-      </c>
-      <c r="B36" t="s">
-        <v>445</v>
-      </c>
-      <c r="C36" t="s">
-        <v>621</v>
-      </c>
-      <c r="D36" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>446</v>
-      </c>
-      <c r="B37" t="s">
-        <v>447</v>
-      </c>
-      <c r="C37" t="s">
-        <v>624</v>
-      </c>
-      <c r="D37" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>448</v>
-      </c>
-      <c r="B38" t="s">
-        <v>449</v>
-      </c>
-      <c r="C38" t="s">
-        <v>625</v>
-      </c>
-      <c r="D38" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>450</v>
-      </c>
-      <c r="B39" t="s">
-        <v>451</v>
-      </c>
-      <c r="C39" t="s">
-        <v>618</v>
-      </c>
-      <c r="D39" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>452</v>
-      </c>
-      <c r="B40" t="s">
-        <v>453</v>
-      </c>
-      <c r="C40" t="s">
-        <v>626</v>
-      </c>
-      <c r="D40" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>454</v>
-      </c>
-      <c r="B41" t="s">
-        <v>455</v>
-      </c>
-      <c r="C41" t="s">
-        <v>625</v>
-      </c>
-      <c r="D41" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>456</v>
-      </c>
-      <c r="B42" t="s">
-        <v>457</v>
-      </c>
-      <c r="C42" t="s">
-        <v>621</v>
-      </c>
-      <c r="D42" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>458</v>
-      </c>
-      <c r="B43" t="s">
-        <v>459</v>
-      </c>
-      <c r="C43" t="s">
-        <v>630</v>
-      </c>
-      <c r="D43" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>460</v>
-      </c>
-      <c r="B44" t="s">
-        <v>461</v>
-      </c>
-      <c r="C44" t="s">
-        <v>621</v>
-      </c>
-      <c r="D44" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>462</v>
-      </c>
-      <c r="B45" t="s">
-        <v>463</v>
-      </c>
-      <c r="C45" t="s">
-        <v>628</v>
-      </c>
-      <c r="D45" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>464</v>
-      </c>
-      <c r="B46" t="s">
-        <v>465</v>
-      </c>
-      <c r="C46" t="s">
-        <v>620</v>
-      </c>
-      <c r="D46" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>466</v>
-      </c>
-      <c r="B47" t="s">
-        <v>467</v>
-      </c>
-      <c r="C47" t="s">
-        <v>624</v>
-      </c>
-      <c r="D47" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>468</v>
-      </c>
-      <c r="B48" t="s">
-        <v>469</v>
-      </c>
-      <c r="C48" t="s">
-        <v>624</v>
-      </c>
-      <c r="D48" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>470</v>
-      </c>
-      <c r="B49" t="s">
-        <v>471</v>
-      </c>
-      <c r="C49" t="s">
-        <v>628</v>
-      </c>
-      <c r="D49" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>472</v>
-      </c>
-      <c r="B50" t="s">
-        <v>473</v>
-      </c>
-      <c r="C50" t="s">
-        <v>620</v>
-      </c>
-      <c r="D50" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>474</v>
-      </c>
-      <c r="B51" t="s">
-        <v>475</v>
-      </c>
-      <c r="C51" t="s">
-        <v>627</v>
-      </c>
-      <c r="D51" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>476</v>
-      </c>
-      <c r="B52" t="s">
-        <v>477</v>
-      </c>
-      <c r="C52" t="s">
-        <v>628</v>
-      </c>
-      <c r="D52" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>478</v>
-      </c>
-      <c r="B53" t="s">
-        <v>479</v>
-      </c>
-      <c r="C53" t="s">
-        <v>624</v>
-      </c>
-      <c r="D53" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>480</v>
-      </c>
-      <c r="B54" t="s">
-        <v>481</v>
-      </c>
-      <c r="C54" t="s">
-        <v>626</v>
-      </c>
-      <c r="D54" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>482</v>
-      </c>
-      <c r="B55" t="s">
-        <v>483</v>
-      </c>
-      <c r="C55" t="s">
-        <v>626</v>
-      </c>
-      <c r="D55" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>484</v>
-      </c>
-      <c r="B56" t="s">
-        <v>485</v>
-      </c>
-      <c r="C56" t="s">
-        <v>628</v>
-      </c>
-      <c r="D56" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>486</v>
-      </c>
-      <c r="B57" t="s">
-        <v>487</v>
-      </c>
-      <c r="C57" t="s">
-        <v>618</v>
-      </c>
-      <c r="D57" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>488</v>
-      </c>
-      <c r="B58" t="s">
-        <v>489</v>
-      </c>
-      <c r="C58" t="s">
-        <v>618</v>
-      </c>
-      <c r="D58" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>490</v>
-      </c>
-      <c r="B59" t="s">
-        <v>491</v>
-      </c>
-      <c r="C59" t="s">
-        <v>630</v>
-      </c>
-      <c r="D59" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>492</v>
-      </c>
-      <c r="B60" t="s">
-        <v>493</v>
-      </c>
-      <c r="C60" t="s">
-        <v>623</v>
-      </c>
-      <c r="D60" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>494</v>
-      </c>
-      <c r="B61" t="s">
-        <v>495</v>
-      </c>
-      <c r="C61" t="s">
-        <v>620</v>
-      </c>
-      <c r="D61" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>496</v>
-      </c>
-      <c r="B62" t="s">
-        <v>497</v>
-      </c>
-      <c r="C62" t="s">
-        <v>620</v>
-      </c>
-      <c r="D62" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>498</v>
-      </c>
-      <c r="B63" t="s">
-        <v>499</v>
-      </c>
-      <c r="C63" t="s">
-        <v>621</v>
-      </c>
-      <c r="D63" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>500</v>
-      </c>
-      <c r="B64" t="s">
-        <v>501</v>
-      </c>
-      <c r="C64" t="s">
-        <v>630</v>
-      </c>
-      <c r="D64" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>502</v>
-      </c>
-      <c r="B65" t="s">
-        <v>503</v>
-      </c>
-      <c r="C65" t="s">
-        <v>624</v>
-      </c>
-      <c r="D65" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>504</v>
-      </c>
-      <c r="B66" t="s">
-        <v>505</v>
-      </c>
-      <c r="C66" t="s">
-        <v>630</v>
-      </c>
-      <c r="D66" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>506</v>
-      </c>
-      <c r="B67" t="s">
-        <v>507</v>
-      </c>
-      <c r="C67" t="s">
-        <v>630</v>
-      </c>
-      <c r="D67" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>508</v>
-      </c>
-      <c r="B68" t="s">
-        <v>509</v>
-      </c>
-      <c r="C68" t="s">
-        <v>618</v>
-      </c>
-      <c r="D68" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
-        <v>510</v>
-      </c>
-      <c r="B69" t="s">
-        <v>511</v>
-      </c>
-      <c r="C69" t="s">
-        <v>620</v>
-      </c>
-      <c r="D69" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
-        <v>512</v>
-      </c>
-      <c r="B70" t="s">
-        <v>513</v>
-      </c>
-      <c r="C70" t="s">
-        <v>626</v>
-      </c>
-      <c r="D70" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>514</v>
-      </c>
-      <c r="B71" t="s">
-        <v>515</v>
-      </c>
-      <c r="C71" t="s">
-        <v>630</v>
-      </c>
-      <c r="D71" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>516</v>
-      </c>
-      <c r="B72" t="s">
-        <v>517</v>
-      </c>
-      <c r="C72" t="s">
-        <v>624</v>
-      </c>
-      <c r="D72" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>518</v>
-      </c>
-      <c r="B73" t="s">
-        <v>519</v>
-      </c>
-      <c r="C73" t="s">
-        <v>620</v>
-      </c>
-      <c r="D73" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>520</v>
-      </c>
-      <c r="B74" t="s">
-        <v>521</v>
-      </c>
-      <c r="C74" t="s">
-        <v>629</v>
-      </c>
-      <c r="D74" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>522</v>
-      </c>
-      <c r="B75" t="s">
-        <v>523</v>
-      </c>
-      <c r="C75" t="s">
-        <v>630</v>
-      </c>
-      <c r="D75" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>524</v>
-      </c>
-      <c r="B76" t="s">
-        <v>525</v>
-      </c>
-      <c r="C76" t="s">
-        <v>630</v>
-      </c>
-      <c r="D76" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
-        <v>526</v>
-      </c>
-      <c r="B77" t="s">
-        <v>527</v>
-      </c>
-      <c r="C77" t="s">
-        <v>628</v>
-      </c>
-      <c r="D77" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>528</v>
-      </c>
-      <c r="B78" t="s">
-        <v>529</v>
-      </c>
-      <c r="C78" t="s">
-        <v>621</v>
-      </c>
-      <c r="D78" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
-        <v>530</v>
-      </c>
-      <c r="B79" t="s">
-        <v>531</v>
-      </c>
-      <c r="C79" t="s">
-        <v>630</v>
-      </c>
-      <c r="D79" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>532</v>
-      </c>
-      <c r="B80" t="s">
-        <v>533</v>
-      </c>
-      <c r="C80" t="s">
-        <v>620</v>
-      </c>
-      <c r="D80" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
-        <v>534</v>
-      </c>
-      <c r="B81" t="s">
-        <v>535</v>
-      </c>
-      <c r="C81" t="s">
-        <v>624</v>
-      </c>
-      <c r="D81" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
-        <v>536</v>
-      </c>
-      <c r="B82" t="s">
-        <v>537</v>
-      </c>
-      <c r="C82" t="s">
-        <v>626</v>
-      </c>
-      <c r="D82" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
-        <v>538</v>
-      </c>
-      <c r="B83" t="s">
-        <v>539</v>
-      </c>
-      <c r="C83" t="s">
-        <v>621</v>
-      </c>
-      <c r="D83" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
-        <v>540</v>
-      </c>
-      <c r="B84" t="s">
-        <v>541</v>
-      </c>
-      <c r="C84" t="s">
-        <v>621</v>
-      </c>
-      <c r="D84" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
-        <v>542</v>
-      </c>
-      <c r="B85" t="s">
-        <v>543</v>
-      </c>
-      <c r="C85" t="s">
-        <v>623</v>
-      </c>
-      <c r="D85" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>544</v>
-      </c>
-      <c r="B86" t="s">
-        <v>545</v>
-      </c>
-      <c r="C86" t="s">
-        <v>624</v>
-      </c>
-      <c r="D86" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>546</v>
-      </c>
-      <c r="B87" t="s">
-        <v>547</v>
-      </c>
-      <c r="C87" t="s">
-        <v>618</v>
-      </c>
-      <c r="D87" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>548</v>
-      </c>
-      <c r="B88" t="s">
-        <v>549</v>
-      </c>
-      <c r="C88" t="s">
-        <v>620</v>
-      </c>
-      <c r="D88" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
-        <v>550</v>
-      </c>
-      <c r="B89" t="s">
-        <v>551</v>
-      </c>
-      <c r="C89" t="s">
-        <v>627</v>
-      </c>
-      <c r="D89" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
-        <v>552</v>
-      </c>
-      <c r="B90" t="s">
-        <v>553</v>
-      </c>
-      <c r="C90" t="s">
-        <v>624</v>
-      </c>
-      <c r="D90" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
-        <v>554</v>
-      </c>
-      <c r="B91" t="s">
-        <v>555</v>
-      </c>
-      <c r="C91" t="s">
-        <v>626</v>
-      </c>
-      <c r="D91" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
-        <v>556</v>
-      </c>
-      <c r="B92" t="s">
-        <v>557</v>
-      </c>
-      <c r="C92" t="s">
-        <v>618</v>
-      </c>
-      <c r="D92" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
-        <v>558</v>
-      </c>
-      <c r="B93" t="s">
-        <v>559</v>
-      </c>
-      <c r="C93" t="s">
-        <v>620</v>
-      </c>
-      <c r="D93" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
-        <v>560</v>
-      </c>
-      <c r="B94" t="s">
-        <v>561</v>
-      </c>
-      <c r="C94" t="s">
-        <v>618</v>
-      </c>
-      <c r="D94" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
-        <v>562</v>
-      </c>
-      <c r="B95" t="s">
-        <v>563</v>
-      </c>
-      <c r="C95" t="s">
-        <v>620</v>
-      </c>
-      <c r="D95" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
-        <v>564</v>
-      </c>
-      <c r="B96" t="s">
-        <v>565</v>
-      </c>
-      <c r="C96" t="s">
-        <v>618</v>
-      </c>
-      <c r="D96" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
-        <v>566</v>
-      </c>
-      <c r="B97" t="s">
-        <v>567</v>
-      </c>
-      <c r="C97" t="s">
-        <v>618</v>
-      </c>
-      <c r="D97" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
-        <v>568</v>
-      </c>
-      <c r="B98" t="s">
-        <v>569</v>
-      </c>
-      <c r="C98" t="s">
-        <v>618</v>
-      </c>
-      <c r="D98" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
-        <v>570</v>
-      </c>
-      <c r="B99" t="s">
-        <v>571</v>
-      </c>
-      <c r="C99" t="s">
-        <v>618</v>
-      </c>
-      <c r="D99" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
-        <v>572</v>
-      </c>
-      <c r="B100" t="s">
-        <v>573</v>
-      </c>
-      <c r="C100" t="s">
-        <v>630</v>
-      </c>
-      <c r="D100" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
-        <v>574</v>
-      </c>
-      <c r="B101" t="s">
-        <v>575</v>
-      </c>
-      <c r="C101" t="s">
-        <v>618</v>
-      </c>
-      <c r="D101" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
-        <v>576</v>
-      </c>
-      <c r="B102" t="s">
-        <v>577</v>
-      </c>
-      <c r="C102" t="s">
-        <v>626</v>
-      </c>
-      <c r="D102" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
-        <v>578</v>
-      </c>
-      <c r="B103" t="s">
-        <v>579</v>
-      </c>
-      <c r="C103" t="s">
-        <v>621</v>
-      </c>
-      <c r="D103" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
-        <v>580</v>
-      </c>
-      <c r="B104" t="s">
-        <v>581</v>
-      </c>
-      <c r="C104" t="s">
-        <v>630</v>
-      </c>
-      <c r="D104" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
-        <v>582</v>
-      </c>
-      <c r="B105" t="s">
-        <v>583</v>
-      </c>
-      <c r="C105" t="s">
-        <v>630</v>
-      </c>
-      <c r="D105" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
-        <v>584</v>
-      </c>
-      <c r="B106" t="s">
-        <v>585</v>
-      </c>
-      <c r="C106" t="s">
-        <v>618</v>
-      </c>
-      <c r="D106" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
-        <v>586</v>
-      </c>
-      <c r="B107" t="s">
-        <v>587</v>
-      </c>
-      <c r="C107" t="s">
-        <v>627</v>
-      </c>
-      <c r="D107" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
-        <v>588</v>
-      </c>
-      <c r="B108" t="s">
-        <v>589</v>
-      </c>
-      <c r="C108" t="s">
-        <v>628</v>
-      </c>
-      <c r="D108" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
-        <v>590</v>
-      </c>
-      <c r="B109" t="s">
-        <v>591</v>
-      </c>
-      <c r="C109" t="s">
-        <v>621</v>
-      </c>
-      <c r="D109" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
-        <v>592</v>
-      </c>
-      <c r="B110" t="s">
-        <v>593</v>
-      </c>
-      <c r="C110" t="s">
-        <v>620</v>
-      </c>
-      <c r="D110" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A111" t="s">
-        <v>594</v>
-      </c>
-      <c r="B111" t="s">
-        <v>595</v>
-      </c>
-      <c r="C111" t="s">
-        <v>621</v>
-      </c>
-      <c r="D111" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A112" t="s">
-        <v>596</v>
-      </c>
-      <c r="B112" t="s">
-        <v>597</v>
-      </c>
-      <c r="C112" t="s">
-        <v>618</v>
-      </c>
-      <c r="D112" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A113" t="s">
-        <v>598</v>
-      </c>
-      <c r="B113" t="s">
-        <v>599</v>
-      </c>
-      <c r="C113" t="s">
-        <v>627</v>
-      </c>
-      <c r="D113" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A114" t="s">
-        <v>600</v>
-      </c>
-      <c r="B114" t="s">
-        <v>601</v>
-      </c>
-      <c r="C114" t="s">
-        <v>629</v>
-      </c>
-      <c r="D114" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
-        <v>602</v>
-      </c>
-      <c r="B115" t="s">
-        <v>603</v>
-      </c>
-      <c r="C115" t="s">
-        <v>626</v>
-      </c>
-      <c r="D115" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A116" t="s">
-        <v>604</v>
-      </c>
-      <c r="B116" t="s">
-        <v>605</v>
-      </c>
-      <c r="C116" t="s">
-        <v>623</v>
-      </c>
-      <c r="D116" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A117" t="s">
-        <v>606</v>
-      </c>
-      <c r="B117" t="s">
-        <v>607</v>
-      </c>
-      <c r="C117" t="s">
-        <v>627</v>
-      </c>
-      <c r="D117" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A118" t="s">
-        <v>608</v>
-      </c>
-      <c r="B118" t="s">
-        <v>609</v>
-      </c>
-      <c r="C118" t="s">
-        <v>630</v>
-      </c>
-      <c r="D118" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A119" t="s">
-        <v>610</v>
-      </c>
-      <c r="B119" t="s">
-        <v>611</v>
-      </c>
-      <c r="C119" t="s">
-        <v>630</v>
-      </c>
-      <c r="D119" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A120" t="s">
-        <v>612</v>
-      </c>
-      <c r="B120" t="s">
-        <v>613</v>
-      </c>
-      <c r="C120" t="s">
-        <v>621</v>
-      </c>
-      <c r="D120" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A121" t="s">
-        <v>614</v>
-      </c>
-      <c r="B121" t="s">
-        <v>615</v>
-      </c>
-      <c r="C121" t="s">
-        <v>630</v>
-      </c>
-      <c r="D121" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A122" t="s">
-        <v>616</v>
-      </c>
-      <c r="B122" t="s">
-        <v>617</v>
-      </c>
-      <c r="C122" t="s">
-        <v>618</v>
-      </c>
-      <c r="D122" s="3">
-        <v>45622</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A123" s="7" t="s">
-        <v>695</v>
-      </c>
-      <c r="B123" s="8" t="s">
-        <v>696</v>
-      </c>
-      <c r="C123" t="s">
-        <v>618</v>
-      </c>
-      <c r="D123" s="3">
-        <v>45666</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A124" s="7" t="s">
-        <v>697</v>
-      </c>
-      <c r="B124" s="8" t="s">
-        <v>698</v>
-      </c>
-      <c r="C124" t="s">
-        <v>630</v>
-      </c>
-      <c r="D124" s="3">
-        <v>45666</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A125" s="7" t="s">
-        <v>699</v>
-      </c>
-      <c r="B125" s="8" t="s">
-        <v>700</v>
-      </c>
-      <c r="C125" t="s">
-        <v>618</v>
-      </c>
-      <c r="D125" s="3">
-        <v>45666</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A126" s="7" t="s">
-        <v>701</v>
-      </c>
-      <c r="B126" s="8" t="s">
-        <v>702</v>
-      </c>
-      <c r="C126" s="7" t="s">
-        <v>623</v>
-      </c>
-      <c r="D126" s="3">
-        <v>45666</v>
-      </c>
+    <row r="2" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="11">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>719</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>737</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="11">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>720</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>738</v>
+      </c>
+      <c r="D3" s="10"/>
+    </row>
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="11">
+        <v>3</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>721</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>739</v>
+      </c>
+      <c r="D4" s="10"/>
+    </row>
+    <row r="5" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="11">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>722</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>737</v>
+      </c>
+      <c r="D5" s="10"/>
+    </row>
+    <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="11">
+        <v>5</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>723</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>740</v>
+      </c>
+      <c r="D6" s="10"/>
+    </row>
+    <row r="7" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="11">
+        <v>7</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>724</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>741</v>
+      </c>
+      <c r="D7" s="10"/>
+    </row>
+    <row r="8" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="11">
+        <v>8</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>725</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>742</v>
+      </c>
+      <c r="D8" s="10"/>
+    </row>
+    <row r="9" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="11">
+        <v>9</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>726</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>740</v>
+      </c>
+      <c r="D9" s="10"/>
+    </row>
+    <row r="10" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A10" s="11">
+        <v>10</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>727</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>740</v>
+      </c>
+      <c r="D10" s="10"/>
+    </row>
+    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="11">
+        <v>11</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>728</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>740</v>
+      </c>
+      <c r="D11" s="10"/>
+    </row>
+    <row r="12" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A12" s="11">
+        <v>12</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>729</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>743</v>
+      </c>
+      <c r="D12" s="10"/>
+    </row>
+    <row r="13" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="11">
+        <v>13</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>730</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>742</v>
+      </c>
+      <c r="D13" s="10"/>
+    </row>
+    <row r="14" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="11">
+        <v>14</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>731</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>742</v>
+      </c>
+      <c r="D14" s="10"/>
+    </row>
+    <row r="15" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="11">
+        <v>15</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>732</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>742</v>
+      </c>
+      <c r="D15" s="10"/>
+    </row>
+    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="11">
+        <v>16</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>733</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>740</v>
+      </c>
+      <c r="D16" s="10"/>
+    </row>
+    <row r="17" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="11">
+        <v>17</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>734</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>742</v>
+      </c>
+      <c r="D17" s="9"/>
+    </row>
+    <row r="18" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="11">
+        <v>18</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>735</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>743</v>
+      </c>
+      <c r="D18" s="9"/>
+    </row>
+    <row r="19" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A19" s="11">
+        <v>19</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>736</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>740</v>
+      </c>
+      <c r="D19" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -7342,10 +5975,1953 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BADE879A-7EC1-495C-9E50-902B8DD0A077}">
+  <dimension ref="A1:A14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="53.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>624</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A129">
+    <sortCondition ref="A1:A129"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33BE4AF1-62F2-48C7-9858-4347997C7FE3}">
+  <sheetPr>
+    <tabColor rgb="FFEE0000"/>
+  </sheetPr>
+  <dimension ref="A1:D130"/>
+  <sheetViews>
+    <sheetView topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C130"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="D1" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>376</v>
+      </c>
+      <c r="B2" t="s">
+        <v>377</v>
+      </c>
+      <c r="C2" t="s">
+        <v>623</v>
+      </c>
+      <c r="D2" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>378</v>
+      </c>
+      <c r="B3" t="s">
+        <v>379</v>
+      </c>
+      <c r="C3" t="s">
+        <v>621</v>
+      </c>
+      <c r="D3" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>380</v>
+      </c>
+      <c r="B4" t="s">
+        <v>381</v>
+      </c>
+      <c r="C4" t="s">
+        <v>619</v>
+      </c>
+      <c r="D4" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>382</v>
+      </c>
+      <c r="B5" t="s">
+        <v>383</v>
+      </c>
+      <c r="C5" t="s">
+        <v>620</v>
+      </c>
+      <c r="D5" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>384</v>
+      </c>
+      <c r="B6" t="s">
+        <v>385</v>
+      </c>
+      <c r="C6" t="s">
+        <v>621</v>
+      </c>
+      <c r="D6" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>386</v>
+      </c>
+      <c r="B7" t="s">
+        <v>387</v>
+      </c>
+      <c r="C7" t="s">
+        <v>618</v>
+      </c>
+      <c r="D7" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>388</v>
+      </c>
+      <c r="B8" t="s">
+        <v>389</v>
+      </c>
+      <c r="C8" t="s">
+        <v>618</v>
+      </c>
+      <c r="D8" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>390</v>
+      </c>
+      <c r="B9" t="s">
+        <v>391</v>
+      </c>
+      <c r="C9" t="s">
+        <v>624</v>
+      </c>
+      <c r="D9" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>392</v>
+      </c>
+      <c r="B10" t="s">
+        <v>393</v>
+      </c>
+      <c r="C10" t="s">
+        <v>618</v>
+      </c>
+      <c r="D10" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>394</v>
+      </c>
+      <c r="B11" t="s">
+        <v>395</v>
+      </c>
+      <c r="C11" t="s">
+        <v>621</v>
+      </c>
+      <c r="D11" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>396</v>
+      </c>
+      <c r="B12" t="s">
+        <v>397</v>
+      </c>
+      <c r="C12" t="s">
+        <v>621</v>
+      </c>
+      <c r="D12" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>398</v>
+      </c>
+      <c r="B13" t="s">
+        <v>399</v>
+      </c>
+      <c r="C13" t="s">
+        <v>618</v>
+      </c>
+      <c r="D13" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>400</v>
+      </c>
+      <c r="B14" t="s">
+        <v>401</v>
+      </c>
+      <c r="C14" t="s">
+        <v>620</v>
+      </c>
+      <c r="D14" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>402</v>
+      </c>
+      <c r="B15" t="s">
+        <v>403</v>
+      </c>
+      <c r="C15" t="s">
+        <v>621</v>
+      </c>
+      <c r="D15" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>404</v>
+      </c>
+      <c r="B16" t="s">
+        <v>405</v>
+      </c>
+      <c r="C16" t="s">
+        <v>620</v>
+      </c>
+      <c r="D16" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>406</v>
+      </c>
+      <c r="B17" t="s">
+        <v>407</v>
+      </c>
+      <c r="C17" t="s">
+        <v>620</v>
+      </c>
+      <c r="D17" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>408</v>
+      </c>
+      <c r="B18" t="s">
+        <v>409</v>
+      </c>
+      <c r="C18" t="s">
+        <v>630</v>
+      </c>
+      <c r="D18" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>410</v>
+      </c>
+      <c r="B19" t="s">
+        <v>411</v>
+      </c>
+      <c r="C19" t="s">
+        <v>620</v>
+      </c>
+      <c r="D19" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>412</v>
+      </c>
+      <c r="B20" t="s">
+        <v>413</v>
+      </c>
+      <c r="C20" t="s">
+        <v>620</v>
+      </c>
+      <c r="D20" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>414</v>
+      </c>
+      <c r="B21" t="s">
+        <v>415</v>
+      </c>
+      <c r="C21" t="s">
+        <v>618</v>
+      </c>
+      <c r="D21" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>416</v>
+      </c>
+      <c r="B22" t="s">
+        <v>417</v>
+      </c>
+      <c r="C22" t="s">
+        <v>620</v>
+      </c>
+      <c r="D22" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>418</v>
+      </c>
+      <c r="B23" t="s">
+        <v>419</v>
+      </c>
+      <c r="C23" t="s">
+        <v>621</v>
+      </c>
+      <c r="D23" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>420</v>
+      </c>
+      <c r="B24" t="s">
+        <v>421</v>
+      </c>
+      <c r="C24" t="s">
+        <v>622</v>
+      </c>
+      <c r="D24" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>422</v>
+      </c>
+      <c r="B25" t="s">
+        <v>423</v>
+      </c>
+      <c r="C25" t="s">
+        <v>630</v>
+      </c>
+      <c r="D25" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>424</v>
+      </c>
+      <c r="B26" t="s">
+        <v>425</v>
+      </c>
+      <c r="C26" t="s">
+        <v>621</v>
+      </c>
+      <c r="D26" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>426</v>
+      </c>
+      <c r="B27" t="s">
+        <v>427</v>
+      </c>
+      <c r="C27" t="s">
+        <v>620</v>
+      </c>
+      <c r="D27" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>428</v>
+      </c>
+      <c r="B28" t="s">
+        <v>429</v>
+      </c>
+      <c r="C28" t="s">
+        <v>618</v>
+      </c>
+      <c r="D28" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>430</v>
+      </c>
+      <c r="B29" t="s">
+        <v>431</v>
+      </c>
+      <c r="C29" t="s">
+        <v>623</v>
+      </c>
+      <c r="D29" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>432</v>
+      </c>
+      <c r="B30" t="s">
+        <v>433</v>
+      </c>
+      <c r="C30" t="s">
+        <v>621</v>
+      </c>
+      <c r="D30" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>434</v>
+      </c>
+      <c r="B31" t="s">
+        <v>435</v>
+      </c>
+      <c r="C31" t="s">
+        <v>621</v>
+      </c>
+      <c r="D31" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>436</v>
+      </c>
+      <c r="B32" t="s">
+        <v>437</v>
+      </c>
+      <c r="C32" t="s">
+        <v>630</v>
+      </c>
+      <c r="D32" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>438</v>
+      </c>
+      <c r="B33" t="s">
+        <v>439</v>
+      </c>
+      <c r="C33" t="s">
+        <v>625</v>
+      </c>
+      <c r="D33" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>440</v>
+      </c>
+      <c r="B34" t="s">
+        <v>441</v>
+      </c>
+      <c r="C34" t="s">
+        <v>630</v>
+      </c>
+      <c r="D34" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>442</v>
+      </c>
+      <c r="B35" t="s">
+        <v>443</v>
+      </c>
+      <c r="C35" t="s">
+        <v>624</v>
+      </c>
+      <c r="D35" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>444</v>
+      </c>
+      <c r="B36" t="s">
+        <v>445</v>
+      </c>
+      <c r="C36" t="s">
+        <v>621</v>
+      </c>
+      <c r="D36" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>446</v>
+      </c>
+      <c r="B37" t="s">
+        <v>447</v>
+      </c>
+      <c r="C37" t="s">
+        <v>624</v>
+      </c>
+      <c r="D37" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>448</v>
+      </c>
+      <c r="B38" t="s">
+        <v>449</v>
+      </c>
+      <c r="C38" t="s">
+        <v>625</v>
+      </c>
+      <c r="D38" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>450</v>
+      </c>
+      <c r="B39" t="s">
+        <v>451</v>
+      </c>
+      <c r="C39" t="s">
+        <v>618</v>
+      </c>
+      <c r="D39" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>452</v>
+      </c>
+      <c r="B40" t="s">
+        <v>453</v>
+      </c>
+      <c r="C40" t="s">
+        <v>626</v>
+      </c>
+      <c r="D40" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>454</v>
+      </c>
+      <c r="B41" t="s">
+        <v>455</v>
+      </c>
+      <c r="C41" t="s">
+        <v>625</v>
+      </c>
+      <c r="D41" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>456</v>
+      </c>
+      <c r="B42" t="s">
+        <v>457</v>
+      </c>
+      <c r="C42" t="s">
+        <v>621</v>
+      </c>
+      <c r="D42" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>458</v>
+      </c>
+      <c r="B43" t="s">
+        <v>459</v>
+      </c>
+      <c r="C43" t="s">
+        <v>630</v>
+      </c>
+      <c r="D43" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>460</v>
+      </c>
+      <c r="B44" t="s">
+        <v>461</v>
+      </c>
+      <c r="C44" t="s">
+        <v>621</v>
+      </c>
+      <c r="D44" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>462</v>
+      </c>
+      <c r="B45" t="s">
+        <v>463</v>
+      </c>
+      <c r="C45" t="s">
+        <v>628</v>
+      </c>
+      <c r="D45" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>464</v>
+      </c>
+      <c r="B46" t="s">
+        <v>465</v>
+      </c>
+      <c r="C46" t="s">
+        <v>620</v>
+      </c>
+      <c r="D46" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>466</v>
+      </c>
+      <c r="B47" t="s">
+        <v>467</v>
+      </c>
+      <c r="C47" t="s">
+        <v>624</v>
+      </c>
+      <c r="D47" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>468</v>
+      </c>
+      <c r="B48" t="s">
+        <v>469</v>
+      </c>
+      <c r="C48" t="s">
+        <v>624</v>
+      </c>
+      <c r="D48" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>470</v>
+      </c>
+      <c r="B49" t="s">
+        <v>471</v>
+      </c>
+      <c r="C49" t="s">
+        <v>628</v>
+      </c>
+      <c r="D49" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>472</v>
+      </c>
+      <c r="B50" t="s">
+        <v>473</v>
+      </c>
+      <c r="C50" t="s">
+        <v>620</v>
+      </c>
+      <c r="D50" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>474</v>
+      </c>
+      <c r="B51" t="s">
+        <v>475</v>
+      </c>
+      <c r="C51" t="s">
+        <v>627</v>
+      </c>
+      <c r="D51" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>476</v>
+      </c>
+      <c r="B52" t="s">
+        <v>477</v>
+      </c>
+      <c r="C52" t="s">
+        <v>628</v>
+      </c>
+      <c r="D52" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>478</v>
+      </c>
+      <c r="B53" t="s">
+        <v>479</v>
+      </c>
+      <c r="C53" t="s">
+        <v>624</v>
+      </c>
+      <c r="D53" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>480</v>
+      </c>
+      <c r="B54" t="s">
+        <v>481</v>
+      </c>
+      <c r="C54" t="s">
+        <v>626</v>
+      </c>
+      <c r="D54" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>482</v>
+      </c>
+      <c r="B55" t="s">
+        <v>483</v>
+      </c>
+      <c r="C55" t="s">
+        <v>626</v>
+      </c>
+      <c r="D55" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>484</v>
+      </c>
+      <c r="B56" t="s">
+        <v>485</v>
+      </c>
+      <c r="C56" t="s">
+        <v>628</v>
+      </c>
+      <c r="D56" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>486</v>
+      </c>
+      <c r="B57" t="s">
+        <v>487</v>
+      </c>
+      <c r="C57" t="s">
+        <v>618</v>
+      </c>
+      <c r="D57" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>488</v>
+      </c>
+      <c r="B58" t="s">
+        <v>489</v>
+      </c>
+      <c r="C58" t="s">
+        <v>618</v>
+      </c>
+      <c r="D58" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>490</v>
+      </c>
+      <c r="B59" t="s">
+        <v>491</v>
+      </c>
+      <c r="C59" t="s">
+        <v>630</v>
+      </c>
+      <c r="D59" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>492</v>
+      </c>
+      <c r="B60" t="s">
+        <v>493</v>
+      </c>
+      <c r="C60" t="s">
+        <v>623</v>
+      </c>
+      <c r="D60" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>494</v>
+      </c>
+      <c r="B61" t="s">
+        <v>495</v>
+      </c>
+      <c r="C61" t="s">
+        <v>620</v>
+      </c>
+      <c r="D61" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>496</v>
+      </c>
+      <c r="B62" t="s">
+        <v>497</v>
+      </c>
+      <c r="C62" t="s">
+        <v>620</v>
+      </c>
+      <c r="D62" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>498</v>
+      </c>
+      <c r="B63" t="s">
+        <v>499</v>
+      </c>
+      <c r="C63" t="s">
+        <v>621</v>
+      </c>
+      <c r="D63" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>500</v>
+      </c>
+      <c r="B64" t="s">
+        <v>501</v>
+      </c>
+      <c r="C64" t="s">
+        <v>630</v>
+      </c>
+      <c r="D64" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>502</v>
+      </c>
+      <c r="B65" t="s">
+        <v>503</v>
+      </c>
+      <c r="C65" t="s">
+        <v>624</v>
+      </c>
+      <c r="D65" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>504</v>
+      </c>
+      <c r="B66" t="s">
+        <v>505</v>
+      </c>
+      <c r="C66" t="s">
+        <v>630</v>
+      </c>
+      <c r="D66" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>506</v>
+      </c>
+      <c r="B67" t="s">
+        <v>507</v>
+      </c>
+      <c r="C67" t="s">
+        <v>630</v>
+      </c>
+      <c r="D67" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>508</v>
+      </c>
+      <c r="B68" t="s">
+        <v>509</v>
+      </c>
+      <c r="C68" t="s">
+        <v>618</v>
+      </c>
+      <c r="D68" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>510</v>
+      </c>
+      <c r="B69" t="s">
+        <v>511</v>
+      </c>
+      <c r="C69" t="s">
+        <v>620</v>
+      </c>
+      <c r="D69" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>512</v>
+      </c>
+      <c r="B70" t="s">
+        <v>513</v>
+      </c>
+      <c r="C70" t="s">
+        <v>626</v>
+      </c>
+      <c r="D70" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>514</v>
+      </c>
+      <c r="B71" t="s">
+        <v>515</v>
+      </c>
+      <c r="C71" t="s">
+        <v>630</v>
+      </c>
+      <c r="D71" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>516</v>
+      </c>
+      <c r="B72" t="s">
+        <v>517</v>
+      </c>
+      <c r="C72" t="s">
+        <v>624</v>
+      </c>
+      <c r="D72" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>518</v>
+      </c>
+      <c r="B73" t="s">
+        <v>519</v>
+      </c>
+      <c r="C73" t="s">
+        <v>620</v>
+      </c>
+      <c r="D73" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>520</v>
+      </c>
+      <c r="B74" t="s">
+        <v>521</v>
+      </c>
+      <c r="C74" t="s">
+        <v>629</v>
+      </c>
+      <c r="D74" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>522</v>
+      </c>
+      <c r="B75" t="s">
+        <v>523</v>
+      </c>
+      <c r="C75" t="s">
+        <v>630</v>
+      </c>
+      <c r="D75" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>524</v>
+      </c>
+      <c r="B76" t="s">
+        <v>525</v>
+      </c>
+      <c r="C76" t="s">
+        <v>630</v>
+      </c>
+      <c r="D76" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>526</v>
+      </c>
+      <c r="B77" t="s">
+        <v>527</v>
+      </c>
+      <c r="C77" t="s">
+        <v>628</v>
+      </c>
+      <c r="D77" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>528</v>
+      </c>
+      <c r="B78" t="s">
+        <v>529</v>
+      </c>
+      <c r="C78" t="s">
+        <v>621</v>
+      </c>
+      <c r="D78" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>530</v>
+      </c>
+      <c r="B79" t="s">
+        <v>531</v>
+      </c>
+      <c r="C79" t="s">
+        <v>630</v>
+      </c>
+      <c r="D79" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>532</v>
+      </c>
+      <c r="B80" t="s">
+        <v>533</v>
+      </c>
+      <c r="C80" t="s">
+        <v>620</v>
+      </c>
+      <c r="D80" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>534</v>
+      </c>
+      <c r="B81" t="s">
+        <v>535</v>
+      </c>
+      <c r="C81" t="s">
+        <v>624</v>
+      </c>
+      <c r="D81" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>536</v>
+      </c>
+      <c r="B82" t="s">
+        <v>537</v>
+      </c>
+      <c r="C82" t="s">
+        <v>626</v>
+      </c>
+      <c r="D82" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>538</v>
+      </c>
+      <c r="B83" t="s">
+        <v>539</v>
+      </c>
+      <c r="C83" t="s">
+        <v>621</v>
+      </c>
+      <c r="D83" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>540</v>
+      </c>
+      <c r="B84" t="s">
+        <v>541</v>
+      </c>
+      <c r="C84" t="s">
+        <v>621</v>
+      </c>
+      <c r="D84" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>542</v>
+      </c>
+      <c r="B85" t="s">
+        <v>543</v>
+      </c>
+      <c r="C85" t="s">
+        <v>623</v>
+      </c>
+      <c r="D85" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>544</v>
+      </c>
+      <c r="B86" t="s">
+        <v>545</v>
+      </c>
+      <c r="C86" t="s">
+        <v>624</v>
+      </c>
+      <c r="D86" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>546</v>
+      </c>
+      <c r="B87" t="s">
+        <v>547</v>
+      </c>
+      <c r="C87" t="s">
+        <v>618</v>
+      </c>
+      <c r="D87" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>548</v>
+      </c>
+      <c r="B88" t="s">
+        <v>549</v>
+      </c>
+      <c r="C88" t="s">
+        <v>620</v>
+      </c>
+      <c r="D88" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>550</v>
+      </c>
+      <c r="B89" t="s">
+        <v>551</v>
+      </c>
+      <c r="C89" t="s">
+        <v>627</v>
+      </c>
+      <c r="D89" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>552</v>
+      </c>
+      <c r="B90" t="s">
+        <v>553</v>
+      </c>
+      <c r="C90" t="s">
+        <v>624</v>
+      </c>
+      <c r="D90" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>554</v>
+      </c>
+      <c r="B91" t="s">
+        <v>555</v>
+      </c>
+      <c r="C91" t="s">
+        <v>626</v>
+      </c>
+      <c r="D91" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>556</v>
+      </c>
+      <c r="B92" t="s">
+        <v>557</v>
+      </c>
+      <c r="C92" t="s">
+        <v>618</v>
+      </c>
+      <c r="D92" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>558</v>
+      </c>
+      <c r="B93" t="s">
+        <v>559</v>
+      </c>
+      <c r="C93" t="s">
+        <v>620</v>
+      </c>
+      <c r="D93" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>560</v>
+      </c>
+      <c r="B94" t="s">
+        <v>561</v>
+      </c>
+      <c r="C94" t="s">
+        <v>618</v>
+      </c>
+      <c r="D94" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>562</v>
+      </c>
+      <c r="B95" t="s">
+        <v>563</v>
+      </c>
+      <c r="C95" t="s">
+        <v>620</v>
+      </c>
+      <c r="D95" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>564</v>
+      </c>
+      <c r="B96" t="s">
+        <v>565</v>
+      </c>
+      <c r="C96" t="s">
+        <v>618</v>
+      </c>
+      <c r="D96" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>566</v>
+      </c>
+      <c r="B97" t="s">
+        <v>567</v>
+      </c>
+      <c r="C97" t="s">
+        <v>618</v>
+      </c>
+      <c r="D97" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>568</v>
+      </c>
+      <c r="B98" t="s">
+        <v>569</v>
+      </c>
+      <c r="C98" t="s">
+        <v>618</v>
+      </c>
+      <c r="D98" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>570</v>
+      </c>
+      <c r="B99" t="s">
+        <v>571</v>
+      </c>
+      <c r="C99" t="s">
+        <v>618</v>
+      </c>
+      <c r="D99" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>572</v>
+      </c>
+      <c r="B100" t="s">
+        <v>573</v>
+      </c>
+      <c r="C100" t="s">
+        <v>630</v>
+      </c>
+      <c r="D100" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>574</v>
+      </c>
+      <c r="B101" t="s">
+        <v>575</v>
+      </c>
+      <c r="C101" t="s">
+        <v>618</v>
+      </c>
+      <c r="D101" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>576</v>
+      </c>
+      <c r="B102" t="s">
+        <v>577</v>
+      </c>
+      <c r="C102" t="s">
+        <v>626</v>
+      </c>
+      <c r="D102" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>578</v>
+      </c>
+      <c r="B103" t="s">
+        <v>579</v>
+      </c>
+      <c r="C103" t="s">
+        <v>621</v>
+      </c>
+      <c r="D103" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>580</v>
+      </c>
+      <c r="B104" t="s">
+        <v>581</v>
+      </c>
+      <c r="C104" t="s">
+        <v>630</v>
+      </c>
+      <c r="D104" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>582</v>
+      </c>
+      <c r="B105" t="s">
+        <v>583</v>
+      </c>
+      <c r="C105" t="s">
+        <v>630</v>
+      </c>
+      <c r="D105" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>584</v>
+      </c>
+      <c r="B106" t="s">
+        <v>585</v>
+      </c>
+      <c r="C106" t="s">
+        <v>618</v>
+      </c>
+      <c r="D106" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>586</v>
+      </c>
+      <c r="B107" t="s">
+        <v>587</v>
+      </c>
+      <c r="C107" t="s">
+        <v>627</v>
+      </c>
+      <c r="D107" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>588</v>
+      </c>
+      <c r="B108" t="s">
+        <v>589</v>
+      </c>
+      <c r="C108" t="s">
+        <v>628</v>
+      </c>
+      <c r="D108" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>590</v>
+      </c>
+      <c r="B109" t="s">
+        <v>591</v>
+      </c>
+      <c r="C109" t="s">
+        <v>621</v>
+      </c>
+      <c r="D109" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>592</v>
+      </c>
+      <c r="B110" t="s">
+        <v>593</v>
+      </c>
+      <c r="C110" t="s">
+        <v>620</v>
+      </c>
+      <c r="D110" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>594</v>
+      </c>
+      <c r="B111" t="s">
+        <v>595</v>
+      </c>
+      <c r="C111" t="s">
+        <v>621</v>
+      </c>
+      <c r="D111" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>596</v>
+      </c>
+      <c r="B112" t="s">
+        <v>597</v>
+      </c>
+      <c r="C112" t="s">
+        <v>618</v>
+      </c>
+      <c r="D112" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>598</v>
+      </c>
+      <c r="B113" t="s">
+        <v>599</v>
+      </c>
+      <c r="C113" t="s">
+        <v>627</v>
+      </c>
+      <c r="D113" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>600</v>
+      </c>
+      <c r="B114" t="s">
+        <v>601</v>
+      </c>
+      <c r="C114" t="s">
+        <v>629</v>
+      </c>
+      <c r="D114" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>602</v>
+      </c>
+      <c r="B115" t="s">
+        <v>603</v>
+      </c>
+      <c r="C115" t="s">
+        <v>626</v>
+      </c>
+      <c r="D115" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>604</v>
+      </c>
+      <c r="B116" t="s">
+        <v>605</v>
+      </c>
+      <c r="C116" t="s">
+        <v>623</v>
+      </c>
+      <c r="D116" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>606</v>
+      </c>
+      <c r="B117" t="s">
+        <v>607</v>
+      </c>
+      <c r="C117" t="s">
+        <v>627</v>
+      </c>
+      <c r="D117" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>608</v>
+      </c>
+      <c r="B118" t="s">
+        <v>609</v>
+      </c>
+      <c r="C118" t="s">
+        <v>630</v>
+      </c>
+      <c r="D118" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>610</v>
+      </c>
+      <c r="B119" t="s">
+        <v>611</v>
+      </c>
+      <c r="C119" t="s">
+        <v>630</v>
+      </c>
+      <c r="D119" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>612</v>
+      </c>
+      <c r="B120" t="s">
+        <v>613</v>
+      </c>
+      <c r="C120" t="s">
+        <v>621</v>
+      </c>
+      <c r="D120" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>614</v>
+      </c>
+      <c r="B121" t="s">
+        <v>615</v>
+      </c>
+      <c r="C121" t="s">
+        <v>630</v>
+      </c>
+      <c r="D121" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>616</v>
+      </c>
+      <c r="B122" t="s">
+        <v>617</v>
+      </c>
+      <c r="C122" t="s">
+        <v>618</v>
+      </c>
+      <c r="D122" s="3">
+        <v>45622</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A123" s="7" t="s">
+        <v>695</v>
+      </c>
+      <c r="B123" s="8" t="s">
+        <v>696</v>
+      </c>
+      <c r="C123" t="s">
+        <v>618</v>
+      </c>
+      <c r="D123" s="3">
+        <v>45666</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A124" s="7" t="s">
+        <v>697</v>
+      </c>
+      <c r="B124" s="8" t="s">
+        <v>698</v>
+      </c>
+      <c r="C124" t="s">
+        <v>630</v>
+      </c>
+      <c r="D124" s="3">
+        <v>45666</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A125" s="7" t="s">
+        <v>699</v>
+      </c>
+      <c r="B125" s="8" t="s">
+        <v>700</v>
+      </c>
+      <c r="C125" t="s">
+        <v>618</v>
+      </c>
+      <c r="D125" s="3">
+        <v>45666</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A126" s="7" t="s">
+        <v>701</v>
+      </c>
+      <c r="B126" s="8" t="s">
+        <v>702</v>
+      </c>
+      <c r="C126" s="7" t="s">
+        <v>623</v>
+      </c>
+      <c r="D126" s="3">
+        <v>45666</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A127" s="7" t="s">
+        <v>709</v>
+      </c>
+      <c r="B127" s="8" t="s">
+        <v>710</v>
+      </c>
+      <c r="C127" t="s">
+        <v>630</v>
+      </c>
+      <c r="D127" s="3">
+        <v>45846</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A128" s="7" t="s">
+        <v>711</v>
+      </c>
+      <c r="B128" s="8" t="s">
+        <v>712</v>
+      </c>
+      <c r="C128" t="s">
+        <v>630</v>
+      </c>
+      <c r="D128" s="3">
+        <v>45846</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A129" s="7" t="s">
+        <v>713</v>
+      </c>
+      <c r="B129" s="8" t="s">
+        <v>714</v>
+      </c>
+      <c r="C129" t="s">
+        <v>630</v>
+      </c>
+      <c r="D129" s="3">
+        <v>45846</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A130" s="7" t="s">
+        <v>715</v>
+      </c>
+      <c r="B130" s="8" t="s">
+        <v>716</v>
+      </c>
+      <c r="C130" t="s">
+        <v>630</v>
+      </c>
+      <c r="D130" s="3">
+        <v>45846</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92098685-FF19-46AD-A7A9-F4030AB9C8B1}">
   <dimension ref="A1:J156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+    <sheetView topLeftCell="A133" workbookViewId="0">
       <selection activeCell="C155" sqref="C155"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Minor tweaks to topic mapping
</commit_message>
<xml_diff>
--- a/input/mapping_tabeller.xlsx
+++ b/input/mapping_tabeller.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admkbo\Documents\FTIND\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B80A27E5-486B-4D9C-BC50-D0E16B24A79B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E901FD-203D-4D16-86D1-A7939677BA04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{6B009A8E-40F0-41F8-8A22-826EDE827CF8}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2197" uniqueCount="744">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2215" uniqueCount="763">
   <si>
     <t>Albanien</t>
   </si>
@@ -2275,6 +2275,63 @@
   </si>
   <si>
     <t>Reglerne for opnåelsen af dansk statsborgerskab bør strammes</t>
+  </si>
+  <si>
+    <t>EmneNr</t>
+  </si>
+  <si>
+    <t>Topic 0</t>
+  </si>
+  <si>
+    <t>Topic 1</t>
+  </si>
+  <si>
+    <t>Topic 3</t>
+  </si>
+  <si>
+    <t>Topic 4</t>
+  </si>
+  <si>
+    <t>Topic 5</t>
+  </si>
+  <si>
+    <t>Topic 7</t>
+  </si>
+  <si>
+    <t>Topic 8</t>
+  </si>
+  <si>
+    <t>Topic 9</t>
+  </si>
+  <si>
+    <t>Topic 10</t>
+  </si>
+  <si>
+    <t>Topic 11</t>
+  </si>
+  <si>
+    <t>Topic 12</t>
+  </si>
+  <si>
+    <t>Topic 13</t>
+  </si>
+  <si>
+    <t>Topic 14</t>
+  </si>
+  <si>
+    <t>Topic 15</t>
+  </si>
+  <si>
+    <t>Topic 16</t>
+  </si>
+  <si>
+    <t>Topic 17</t>
+  </si>
+  <si>
+    <t>Topic 18</t>
+  </si>
+  <si>
+    <t>Topic 19</t>
   </si>
 </sst>
 </file>
@@ -2400,12 +2457,6 @@
   </cellStyles>
   <dxfs count="16">
     <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <border outline="0">
         <top style="thin">
           <color auto="1"/>
@@ -2478,6 +2529,12 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
   </dxfs>
@@ -2491,10 +2548,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2546,40 +2599,40 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{2C1F5FC9-D397-455C-AEAF-D1763528A602}" name="Emner" displayName="Emner" ref="A1:D19" totalsRowShown="0" dataDxfId="14">
   <autoFilter ref="A1:D19" xr:uid="{2C1F5FC9-D397-455C-AEAF-D1763528A602}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{6F47ADCF-7B5E-431B-8209-B52E2671F6C3}" name="Id" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{625A89F7-2E0B-4AE9-8481-CBE8317B581F}" name="AutomatiskEmne" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{64403E5D-601B-4B88-B55D-4ECF3EA9DC38}" name="EmneGruppe" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{CF0732A2-488A-4A32-B356-40B8CE60F4B8}" name="SidstOpdatret" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{6F47ADCF-7B5E-431B-8209-B52E2671F6C3}" name="EmneNr" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{625A89F7-2E0B-4AE9-8481-CBE8317B581F}" name="AutomatiskEmne" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{64403E5D-601B-4B88-B55D-4ECF3EA9DC38}" name="EmneGruppe" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{CF0732A2-488A-4A32-B356-40B8CE60F4B8}" name="SidstOpdatret" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{ACEBC73D-D5CB-474D-A08E-341527931D76}" name="Table8" displayName="Table8" ref="A1:A14" totalsRowShown="0" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{ACEBC73D-D5CB-474D-A08E-341527931D76}" name="Table8" displayName="Table8" ref="A1:A14" totalsRowShown="0" dataDxfId="9">
   <autoFilter ref="A1:A14" xr:uid="{ACEBC73D-D5CB-474D-A08E-341527931D76}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{3D760C71-CA3D-4682-AB2E-A98C0BA67482}" name="Topics to choose from" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{3D760C71-CA3D-4682-AB2E-A98C0BA67482}" name="Topics to choose from" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{204A3821-716B-47DA-873B-31C8C0CEF80B}" name="EmnerOLD" displayName="EmnerOLD" ref="A1:D130" totalsRowShown="0" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{204A3821-716B-47DA-873B-31C8C0CEF80B}" name="EmnerOLD" displayName="EmnerOLD" ref="A1:D130" totalsRowShown="0" dataDxfId="7">
   <autoFilter ref="A1:D130" xr:uid="{2C1F5FC9-D397-455C-AEAF-D1763528A602}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{94BA0EB3-0C75-479D-9BD6-7C6FB84F78EE}" name="Id" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{A5450B2C-F4C6-4F5C-9C58-5034F7F7DA04}" name="AutomatiskEmne" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{27DD0F04-ABC0-4A1C-BD5A-95A66D0F1812}" name="EmneGruppe" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{DD14152F-048A-4656-8E38-362FA4F4752D}" name="SidstOpdatret" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{94BA0EB3-0C75-479D-9BD6-7C6FB84F78EE}" name="Id" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{A5450B2C-F4C6-4F5C-9C58-5034F7F7DA04}" name="AutomatiskEmne" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{27DD0F04-ABC0-4A1C-BD5A-95A66D0F1812}" name="EmneGruppe" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{DD14152F-048A-4656-8E38-362FA4F4752D}" name="SidstOpdatret" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{74B9B96F-B2B9-4B1F-B795-88782D08D518}" name="Partihoppere" displayName="Partihoppere" ref="A1:J156" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{74B9B96F-B2B9-4B1F-B795-88782D08D518}" name="Partihoppere" displayName="Partihoppere" ref="A1:J156" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
   <autoFilter ref="A1:J156" xr:uid="{74B9B96F-B2B9-4B1F-B795-88782D08D518}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J156">
     <sortCondition ref="C1:C156"/>
@@ -5723,12 +5776,12 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" customWidth="1"/>
     <col min="2" max="2" width="71.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="53.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.33203125" customWidth="1"/>
@@ -5736,7 +5789,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>373</v>
+        <v>744</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>374</v>
@@ -5749,8 +5802,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="11">
-        <v>0</v>
+      <c r="A2" s="11" t="s">
+        <v>745</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>719</v>
@@ -5758,11 +5811,13 @@
       <c r="C2" s="9" t="s">
         <v>737</v>
       </c>
-      <c r="D2" s="10"/>
+      <c r="D2" s="10">
+        <v>45863</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="11">
-        <v>1</v>
+      <c r="A3" s="11" t="s">
+        <v>746</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>720</v>
@@ -5770,11 +5825,13 @@
       <c r="C3" s="9" t="s">
         <v>738</v>
       </c>
-      <c r="D3" s="10"/>
+      <c r="D3" s="10">
+        <v>45863</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="11">
-        <v>3</v>
+      <c r="A4" s="11" t="s">
+        <v>747</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>721</v>
@@ -5782,11 +5839,13 @@
       <c r="C4" s="9" t="s">
         <v>739</v>
       </c>
-      <c r="D4" s="10"/>
+      <c r="D4" s="10">
+        <v>45863</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="11">
-        <v>4</v>
+      <c r="A5" s="11" t="s">
+        <v>748</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>722</v>
@@ -5794,11 +5853,13 @@
       <c r="C5" s="9" t="s">
         <v>737</v>
       </c>
-      <c r="D5" s="10"/>
+      <c r="D5" s="10">
+        <v>45863</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="11">
-        <v>5</v>
+      <c r="A6" s="11" t="s">
+        <v>749</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>723</v>
@@ -5806,11 +5867,13 @@
       <c r="C6" s="9" t="s">
         <v>740</v>
       </c>
-      <c r="D6" s="10"/>
+      <c r="D6" s="10">
+        <v>45863</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="11">
-        <v>7</v>
+      <c r="A7" s="11" t="s">
+        <v>750</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>724</v>
@@ -5818,11 +5881,13 @@
       <c r="C7" s="9" t="s">
         <v>741</v>
       </c>
-      <c r="D7" s="10"/>
+      <c r="D7" s="10">
+        <v>45863</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="11">
-        <v>8</v>
+      <c r="A8" s="11" t="s">
+        <v>751</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>725</v>
@@ -5830,11 +5895,13 @@
       <c r="C8" s="9" t="s">
         <v>742</v>
       </c>
-      <c r="D8" s="10"/>
+      <c r="D8" s="10">
+        <v>45863</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="11">
-        <v>9</v>
+      <c r="A9" s="11" t="s">
+        <v>752</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>726</v>
@@ -5842,11 +5909,13 @@
       <c r="C9" s="9" t="s">
         <v>740</v>
       </c>
-      <c r="D9" s="10"/>
+      <c r="D9" s="10">
+        <v>45863</v>
+      </c>
     </row>
     <row r="10" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="A10" s="11">
-        <v>10</v>
+      <c r="A10" s="11" t="s">
+        <v>753</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>727</v>
@@ -5854,11 +5923,13 @@
       <c r="C10" s="9" t="s">
         <v>740</v>
       </c>
-      <c r="D10" s="10"/>
+      <c r="D10" s="10">
+        <v>45863</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="11">
-        <v>11</v>
+      <c r="A11" s="11" t="s">
+        <v>754</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>728</v>
@@ -5866,11 +5937,13 @@
       <c r="C11" s="9" t="s">
         <v>740</v>
       </c>
-      <c r="D11" s="10"/>
+      <c r="D11" s="10">
+        <v>45863</v>
+      </c>
     </row>
     <row r="12" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="A12" s="11">
-        <v>12</v>
+      <c r="A12" s="11" t="s">
+        <v>755</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>729</v>
@@ -5878,11 +5951,13 @@
       <c r="C12" s="9" t="s">
         <v>743</v>
       </c>
-      <c r="D12" s="10"/>
+      <c r="D12" s="10">
+        <v>45863</v>
+      </c>
     </row>
     <row r="13" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="11">
-        <v>13</v>
+      <c r="A13" s="11" t="s">
+        <v>756</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>730</v>
@@ -5890,11 +5965,13 @@
       <c r="C13" s="9" t="s">
         <v>742</v>
       </c>
-      <c r="D13" s="10"/>
+      <c r="D13" s="10">
+        <v>45863</v>
+      </c>
     </row>
     <row r="14" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="11">
-        <v>14</v>
+      <c r="A14" s="11" t="s">
+        <v>757</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>731</v>
@@ -5902,11 +5979,13 @@
       <c r="C14" s="9" t="s">
         <v>742</v>
       </c>
-      <c r="D14" s="10"/>
+      <c r="D14" s="10">
+        <v>45863</v>
+      </c>
     </row>
     <row r="15" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="11">
-        <v>15</v>
+      <c r="A15" s="11" t="s">
+        <v>758</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>732</v>
@@ -5914,11 +5993,13 @@
       <c r="C15" s="9" t="s">
         <v>742</v>
       </c>
-      <c r="D15" s="10"/>
+      <c r="D15" s="10">
+        <v>45863</v>
+      </c>
     </row>
     <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="11">
-        <v>16</v>
+      <c r="A16" s="11" t="s">
+        <v>759</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>733</v>
@@ -5926,11 +6007,13 @@
       <c r="C16" s="9" t="s">
         <v>740</v>
       </c>
-      <c r="D16" s="10"/>
+      <c r="D16" s="10">
+        <v>45863</v>
+      </c>
     </row>
     <row r="17" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="11">
-        <v>17</v>
+      <c r="A17" s="11" t="s">
+        <v>760</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>734</v>
@@ -5938,11 +6021,13 @@
       <c r="C17" s="9" t="s">
         <v>742</v>
       </c>
-      <c r="D17" s="9"/>
+      <c r="D17" s="10">
+        <v>45863</v>
+      </c>
     </row>
     <row r="18" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="11">
-        <v>18</v>
+      <c r="A18" s="11" t="s">
+        <v>761</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>735</v>
@@ -5950,11 +6035,13 @@
       <c r="C18" s="9" t="s">
         <v>743</v>
       </c>
-      <c r="D18" s="9"/>
+      <c r="D18" s="10">
+        <v>45863</v>
+      </c>
     </row>
     <row r="19" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="A19" s="11">
-        <v>19</v>
+      <c r="A19" s="11" t="s">
+        <v>762</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>736</v>
@@ -5962,7 +6049,9 @@
       <c r="C19" s="9" t="s">
         <v>740</v>
       </c>
-      <c r="D19" s="9"/>
+      <c r="D19" s="10">
+        <v>45863</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>